<commit_message>
car details in progress
</commit_message>
<xml_diff>
--- a/Samochody.xlsx
+++ b/Samochody.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NASA\PracaInz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC53D55-A478-4D05-8C3F-6E0CCF266685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7973468-50E2-4F24-81E2-93EC8589CCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,9 +192,6 @@
     <t>Pagani Huayra</t>
   </si>
   <si>
-    <t>Subaru Impreza WRX STI</t>
-  </si>
-  <si>
     <t>Ferrari F40</t>
   </si>
   <si>
@@ -784,6 +781,9 @@
   </si>
   <si>
     <t>Bentley Continental Supersport Convertible</t>
+  </si>
+  <si>
+    <t>Subaru Impreza WRX</t>
   </si>
 </sst>
 </file>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,13 +1143,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F1" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -1158,37 +1158,37 @@
         <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L1" t="s">
+        <v>224</v>
+      </c>
+      <c r="M1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N1" t="s">
+        <v>228</v>
+      </c>
+      <c r="O1" t="s">
+        <v>250</v>
+      </c>
+      <c r="P1" t="s">
         <v>225</v>
       </c>
-      <c r="M1" t="s">
-        <v>231</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
+        <v>226</v>
+      </c>
+      <c r="R1" t="s">
+        <v>227</v>
+      </c>
+      <c r="S1" t="s">
         <v>229</v>
       </c>
-      <c r="O1" t="s">
-        <v>251</v>
-      </c>
-      <c r="P1" t="s">
-        <v>226</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>227</v>
-      </c>
-      <c r="R1" t="s">
-        <v>228</v>
-      </c>
-      <c r="S1" t="s">
-        <v>230</v>
-      </c>
       <c r="T1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1202,7 +1202,7 @@
         <v>2016</v>
       </c>
       <c r="D2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E2">
         <v>5.7</v>
@@ -1265,7 +1265,7 @@
         <v>2011</v>
       </c>
       <c r="D3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E3">
         <v>6.2</v>
@@ -1328,7 +1328,7 @@
         <v>2019</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E4">
         <v>3.3</v>
@@ -1391,7 +1391,7 @@
         <v>2011</v>
       </c>
       <c r="D5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E5">
         <v>4.8</v>
@@ -1454,7 +1454,7 @@
         <v>1967</v>
       </c>
       <c r="D6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E6">
         <v>4.9000000000000004</v>
@@ -1517,7 +1517,7 @@
         <v>2013</v>
       </c>
       <c r="D7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E7">
         <v>4.3</v>
@@ -1580,7 +1580,7 @@
         <v>1970</v>
       </c>
       <c r="D8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E8">
         <v>4.9000000000000004</v>
@@ -1643,7 +1643,7 @@
         <v>1966</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -1706,7 +1706,7 @@
         <v>1984</v>
       </c>
       <c r="D10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E10">
         <v>2.1</v>
@@ -1769,7 +1769,7 @@
         <v>1967</v>
       </c>
       <c r="D11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E11">
         <v>7</v>
@@ -1832,7 +1832,7 @@
         <v>2019</v>
       </c>
       <c r="D12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1889,13 +1889,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C13">
         <v>2007</v>
       </c>
       <c r="D13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E13">
         <v>3.8</v>
@@ -1958,7 +1958,7 @@
         <v>1986</v>
       </c>
       <c r="D14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E14">
         <v>2.9</v>
@@ -2021,7 +2021,7 @@
         <v>2016</v>
       </c>
       <c r="D15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E15">
         <v>3.8</v>
@@ -2084,7 +2084,7 @@
         <v>1997</v>
       </c>
       <c r="D16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E16">
         <v>3.6</v>
@@ -2147,7 +2147,7 @@
         <v>2006</v>
       </c>
       <c r="D17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E17">
         <v>5.4</v>
@@ -2210,7 +2210,7 @@
         <v>2004</v>
       </c>
       <c r="D18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E18">
         <v>4.3</v>
@@ -2273,7 +2273,7 @@
         <v>2020</v>
       </c>
       <c r="D19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -2336,7 +2336,7 @@
         <v>1998</v>
       </c>
       <c r="D20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E20">
         <v>2.8</v>
@@ -2399,7 +2399,7 @@
         <v>2010</v>
       </c>
       <c r="D21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E21">
         <v>1.4</v>
@@ -2462,7 +2462,7 @@
         <v>2017</v>
       </c>
       <c r="D22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -2519,13 +2519,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C23">
         <v>2010</v>
       </c>
       <c r="D23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E23">
         <v>6</v>
@@ -2588,7 +2588,7 @@
         <v>2010</v>
       </c>
       <c r="D24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E24">
         <v>4.7</v>
@@ -2651,7 +2651,7 @@
         <v>2004</v>
       </c>
       <c r="D25" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -2714,7 +2714,7 @@
         <v>2015</v>
       </c>
       <c r="D26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E26">
         <v>4.4000000000000004</v>
@@ -2777,7 +2777,7 @@
         <v>2010</v>
       </c>
       <c r="D27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E27">
         <v>4.2</v>
@@ -2840,7 +2840,7 @@
         <v>1965</v>
       </c>
       <c r="D28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E28">
         <v>6.4</v>
@@ -2903,7 +2903,7 @@
         <v>2008</v>
       </c>
       <c r="D29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E29">
         <v>3.2</v>
@@ -2966,7 +2966,55 @@
         <v>1980</v>
       </c>
       <c r="D30" t="s">
-        <v>242</v>
+        <v>241</v>
+      </c>
+      <c r="E30">
+        <v>3.5</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>277</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>5.6</v>
+      </c>
+      <c r="K30">
+        <v>262</v>
+      </c>
+      <c r="L30">
+        <v>330</v>
+      </c>
+      <c r="M30">
+        <v>1300</v>
+      </c>
+      <c r="N30">
+        <v>153</v>
+      </c>
+      <c r="O30">
+        <v>116</v>
+      </c>
+      <c r="P30">
+        <v>436</v>
+      </c>
+      <c r="Q30">
+        <v>182</v>
+      </c>
+      <c r="R30">
+        <v>114</v>
+      </c>
+      <c r="S30">
+        <v>256</v>
+      </c>
+      <c r="T30">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -2981,7 +3029,55 @@
         <v>1999</v>
       </c>
       <c r="D31" t="s">
-        <v>246</v>
+        <v>245</v>
+      </c>
+      <c r="E31">
+        <v>2.8</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>193</v>
+      </c>
+      <c r="H31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <v>240</v>
+      </c>
+      <c r="L31">
+        <v>280</v>
+      </c>
+      <c r="M31">
+        <v>1395</v>
+      </c>
+      <c r="N31">
+        <v>440</v>
+      </c>
+      <c r="O31">
+        <v>63</v>
+      </c>
+      <c r="P31">
+        <v>447</v>
+      </c>
+      <c r="Q31">
+        <v>174</v>
+      </c>
+      <c r="R31">
+        <v>142</v>
+      </c>
+      <c r="S31">
+        <v>273</v>
+      </c>
+      <c r="T31">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -2990,16 +3086,64 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C32">
         <v>2010</v>
       </c>
       <c r="D32" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="E32">
+        <v>3.6</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>304</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>6</v>
+      </c>
+      <c r="K32">
+        <v>235</v>
+      </c>
+      <c r="L32">
+        <v>371</v>
+      </c>
+      <c r="M32">
+        <v>1695</v>
+      </c>
+      <c r="N32">
+        <v>320</v>
+      </c>
+      <c r="O32">
+        <v>72</v>
+      </c>
+      <c r="P32">
+        <v>484</v>
+      </c>
+      <c r="Q32">
+        <v>192</v>
+      </c>
+      <c r="R32">
+        <v>138</v>
+      </c>
+      <c r="S32">
+        <v>285</v>
+      </c>
+      <c r="T32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3011,10 +3155,58 @@
         <v>2002</v>
       </c>
       <c r="D33" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>226</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>6.4</v>
+      </c>
+      <c r="K33">
+        <v>235</v>
+      </c>
+      <c r="L33">
+        <v>300</v>
+      </c>
+      <c r="M33">
+        <v>1335</v>
+      </c>
+      <c r="N33">
+        <v>65</v>
+      </c>
+      <c r="O33">
+        <v>61</v>
+      </c>
+      <c r="P33">
+        <v>380</v>
+      </c>
+      <c r="Q33">
+        <v>181</v>
+      </c>
+      <c r="R33">
+        <v>136</v>
+      </c>
+      <c r="S33">
+        <v>251</v>
+      </c>
+      <c r="T33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3026,10 +3218,58 @@
         <v>2001</v>
       </c>
       <c r="D34" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="E34">
+        <v>5.7</v>
+      </c>
+      <c r="F34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>329</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34">
+        <v>6</v>
+      </c>
+      <c r="K34">
+        <v>250</v>
+      </c>
+      <c r="L34">
+        <v>475</v>
+      </c>
+      <c r="M34">
+        <v>1635</v>
+      </c>
+      <c r="N34">
+        <v>215</v>
+      </c>
+      <c r="O34">
+        <v>63</v>
+      </c>
+      <c r="P34">
+        <v>492</v>
+      </c>
+      <c r="Q34">
+        <v>189</v>
+      </c>
+      <c r="R34">
+        <v>133</v>
+      </c>
+      <c r="S34">
+        <v>257</v>
+      </c>
+      <c r="T34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3041,10 +3281,58 @@
         <v>2002</v>
       </c>
       <c r="D35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>218</v>
+      </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <v>7.6</v>
+      </c>
+      <c r="K35">
+        <v>232</v>
+      </c>
+      <c r="L35">
+        <v>295</v>
+      </c>
+      <c r="M35">
+        <v>1565</v>
+      </c>
+      <c r="N35">
+        <v>283</v>
+      </c>
+      <c r="O35">
+        <v>70</v>
+      </c>
+      <c r="P35">
+        <v>449</v>
+      </c>
+      <c r="Q35">
+        <v>172</v>
+      </c>
+      <c r="R35">
+        <v>141</v>
+      </c>
+      <c r="S35">
+        <v>167</v>
+      </c>
+      <c r="T35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3056,10 +3344,58 @@
         <v>1955</v>
       </c>
       <c r="D36" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+      <c r="G36">
+        <v>215</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>2</v>
+      </c>
+      <c r="J36">
+        <v>10</v>
+      </c>
+      <c r="K36">
+        <v>260</v>
+      </c>
+      <c r="L36">
+        <v>275</v>
+      </c>
+      <c r="M36">
+        <v>1295</v>
+      </c>
+      <c r="N36">
+        <v>237</v>
+      </c>
+      <c r="O36">
+        <v>100</v>
+      </c>
+      <c r="P36">
+        <v>452</v>
+      </c>
+      <c r="Q36">
+        <v>179</v>
+      </c>
+      <c r="R36">
+        <v>130</v>
+      </c>
+      <c r="S36">
+        <v>240</v>
+      </c>
+      <c r="T36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3071,10 +3407,58 @@
         <v>1982</v>
       </c>
       <c r="D37" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E37">
+        <v>5.7</v>
+      </c>
+      <c r="F37">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <v>230</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>6.7</v>
+      </c>
+      <c r="K37">
+        <v>204</v>
+      </c>
+      <c r="L37">
+        <v>373</v>
+      </c>
+      <c r="M37">
+        <v>1596</v>
+      </c>
+      <c r="N37">
+        <v>286</v>
+      </c>
+      <c r="O37">
+        <v>90</v>
+      </c>
+      <c r="P37">
+        <v>470</v>
+      </c>
+      <c r="Q37">
+        <v>175</v>
+      </c>
+      <c r="R37">
+        <v>122</v>
+      </c>
+      <c r="S37">
+        <v>249</v>
+      </c>
+      <c r="T37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3086,10 +3470,58 @@
         <v>2008</v>
       </c>
       <c r="D38" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <v>359</v>
+      </c>
+      <c r="H38">
+        <v>5</v>
+      </c>
+      <c r="I38">
+        <v>4</v>
+      </c>
+      <c r="J38">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K38">
+        <v>250</v>
+      </c>
+      <c r="L38">
+        <v>363</v>
+      </c>
+      <c r="M38">
+        <v>1560</v>
+      </c>
+      <c r="N38">
+        <v>390</v>
+      </c>
+      <c r="O38">
+        <v>55</v>
+      </c>
+      <c r="P38">
+        <v>451</v>
+      </c>
+      <c r="Q38">
+        <v>181</v>
+      </c>
+      <c r="R38">
+        <v>148</v>
+      </c>
+      <c r="S38">
+        <v>265</v>
+      </c>
+      <c r="T38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -3101,10 +3533,58 @@
         <v>1976</v>
       </c>
       <c r="D39" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>260</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>2</v>
+      </c>
+      <c r="J39">
+        <v>5.5</v>
+      </c>
+      <c r="K39">
+        <v>250</v>
+      </c>
+      <c r="L39">
+        <v>343</v>
+      </c>
+      <c r="M39">
+        <v>1140</v>
+      </c>
+      <c r="N39">
+        <v>184</v>
+      </c>
+      <c r="O39">
+        <v>80</v>
+      </c>
+      <c r="P39">
+        <v>429</v>
+      </c>
+      <c r="Q39">
+        <v>178</v>
+      </c>
+      <c r="R39">
+        <v>130</v>
+      </c>
+      <c r="S39">
+        <v>227</v>
+      </c>
+      <c r="T39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -3116,10 +3596,58 @@
         <v>2014</v>
       </c>
       <c r="D40" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E40">
+        <v>4.7</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <v>435</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K40">
+        <v>250</v>
+      </c>
+      <c r="L40">
+        <v>700</v>
+      </c>
+      <c r="M40">
+        <v>1785</v>
+      </c>
+      <c r="N40">
+        <v>241</v>
+      </c>
+      <c r="O40">
+        <v>65</v>
+      </c>
+      <c r="P40">
+        <v>461</v>
+      </c>
+      <c r="Q40">
+        <v>188</v>
+      </c>
+      <c r="R40">
+        <v>131</v>
+      </c>
+      <c r="S40">
+        <v>259</v>
+      </c>
+      <c r="T40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -3131,10 +3659,58 @@
         <v>1970</v>
       </c>
       <c r="D41" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="E41">
+        <v>5.6</v>
+      </c>
+      <c r="F41">
+        <v>8</v>
+      </c>
+      <c r="G41">
+        <v>275</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <v>6.5</v>
+      </c>
+      <c r="K41">
+        <v>201</v>
+      </c>
+      <c r="L41">
+        <v>468</v>
+      </c>
+      <c r="M41">
+        <v>1454</v>
+      </c>
+      <c r="N41">
+        <v>234</v>
+      </c>
+      <c r="O41">
+        <v>54</v>
+      </c>
+      <c r="P41">
+        <v>486</v>
+      </c>
+      <c r="Q41">
+        <v>193</v>
+      </c>
+      <c r="R41">
+        <v>129</v>
+      </c>
+      <c r="S41">
+        <v>279</v>
+      </c>
+      <c r="T41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -3146,10 +3722,58 @@
         <v>2007</v>
       </c>
       <c r="D42" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="E42">
+        <v>3.8</v>
+      </c>
+      <c r="F42">
+        <v>6</v>
+      </c>
+      <c r="G42">
+        <v>265</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42">
+        <v>7.1</v>
+      </c>
+      <c r="K42">
+        <v>240</v>
+      </c>
+      <c r="L42">
+        <v>329</v>
+      </c>
+      <c r="M42">
+        <v>1665</v>
+      </c>
+      <c r="N42">
+        <v>263</v>
+      </c>
+      <c r="O42">
+        <v>67</v>
+      </c>
+      <c r="P42">
+        <v>457</v>
+      </c>
+      <c r="Q42">
+        <v>183</v>
+      </c>
+      <c r="R42">
+        <v>138</v>
+      </c>
+      <c r="S42">
+        <v>258</v>
+      </c>
+      <c r="T42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -3158,13 +3782,61 @@
         <v>46</v>
       </c>
       <c r="C43">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D43" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E43">
+        <v>6.2</v>
+      </c>
+      <c r="F43">
+        <v>8</v>
+      </c>
+      <c r="G43">
+        <v>571</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>3.8</v>
+      </c>
+      <c r="K43">
+        <v>317</v>
+      </c>
+      <c r="L43">
+        <v>650</v>
+      </c>
+      <c r="M43">
+        <v>1620</v>
+      </c>
+      <c r="N43">
+        <v>176</v>
+      </c>
+      <c r="O43">
+        <v>85</v>
+      </c>
+      <c r="P43">
+        <v>463</v>
+      </c>
+      <c r="Q43">
+        <v>193</v>
+      </c>
+      <c r="R43">
+        <v>207</v>
+      </c>
+      <c r="S43">
+        <v>268</v>
+      </c>
+      <c r="T43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3176,10 +3848,58 @@
         <v>2014</v>
       </c>
       <c r="D44" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E44">
+        <v>3.8</v>
+      </c>
+      <c r="F44">
+        <v>6</v>
+      </c>
+      <c r="G44">
+        <v>400</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <v>4.5</v>
+      </c>
+      <c r="K44">
+        <v>304</v>
+      </c>
+      <c r="L44">
+        <v>440</v>
+      </c>
+      <c r="M44">
+        <v>1415</v>
+      </c>
+      <c r="N44">
+        <v>340</v>
+      </c>
+      <c r="O44">
+        <v>64</v>
+      </c>
+      <c r="P44">
+        <v>449</v>
+      </c>
+      <c r="Q44">
+        <v>181</v>
+      </c>
+      <c r="R44">
+        <v>130</v>
+      </c>
+      <c r="S44">
+        <v>245</v>
+      </c>
+      <c r="T44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -3191,10 +3911,58 @@
         <v>2006</v>
       </c>
       <c r="D45" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>200</v>
+      </c>
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>7.2</v>
+      </c>
+      <c r="K45">
+        <v>243</v>
+      </c>
+      <c r="L45">
+        <v>280</v>
+      </c>
+      <c r="M45">
+        <v>1336</v>
+      </c>
+      <c r="N45">
+        <v>350</v>
+      </c>
+      <c r="O45">
+        <v>55</v>
+      </c>
+      <c r="P45">
+        <v>422</v>
+      </c>
+      <c r="Q45">
+        <v>176</v>
+      </c>
+      <c r="R45">
+        <v>147</v>
+      </c>
+      <c r="S45">
+        <v>258</v>
+      </c>
+      <c r="T45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3206,10 +3974,58 @@
         <v>2009</v>
       </c>
       <c r="D46" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="E46">
+        <v>3.7</v>
+      </c>
+      <c r="F46">
+        <v>6</v>
+      </c>
+      <c r="G46">
+        <v>328</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="J46">
+        <v>5.3</v>
+      </c>
+      <c r="K46">
+        <v>275</v>
+      </c>
+      <c r="L46">
+        <v>363</v>
+      </c>
+      <c r="M46">
+        <v>1496</v>
+      </c>
+      <c r="N46">
+        <v>235</v>
+      </c>
+      <c r="O46">
+        <v>72</v>
+      </c>
+      <c r="P46">
+        <v>425</v>
+      </c>
+      <c r="Q46">
+        <v>185</v>
+      </c>
+      <c r="R46">
+        <v>131</v>
+      </c>
+      <c r="S46">
+        <v>255</v>
+      </c>
+      <c r="T46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3221,10 +4037,58 @@
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="E47">
+        <v>1.4</v>
+      </c>
+      <c r="F47">
+        <v>4</v>
+      </c>
+      <c r="G47">
+        <v>180</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <v>6.9</v>
+      </c>
+      <c r="K47">
+        <v>229</v>
+      </c>
+      <c r="L47">
+        <v>250</v>
+      </c>
+      <c r="M47">
+        <v>1194</v>
+      </c>
+      <c r="N47">
+        <v>204</v>
+      </c>
+      <c r="O47">
+        <v>45</v>
+      </c>
+      <c r="P47">
+        <v>398</v>
+      </c>
+      <c r="Q47">
+        <v>168</v>
+      </c>
+      <c r="R47">
+        <v>190</v>
+      </c>
+      <c r="S47">
+        <v>247</v>
+      </c>
+      <c r="T47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3236,10 +4100,58 @@
         <v>2003</v>
       </c>
       <c r="D48" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48">
+        <v>220</v>
+      </c>
+      <c r="H48">
+        <v>4</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>6.3</v>
+      </c>
+      <c r="K48">
+        <v>214</v>
+      </c>
+      <c r="L48">
+        <v>206</v>
+      </c>
+      <c r="M48">
+        <v>1170</v>
+      </c>
+      <c r="N48">
+        <v>504</v>
+      </c>
+      <c r="O48">
+        <v>50</v>
+      </c>
+      <c r="P48">
+        <v>439</v>
+      </c>
+      <c r="Q48">
+        <v>170</v>
+      </c>
+      <c r="R48">
+        <v>138</v>
+      </c>
+      <c r="S48">
+        <v>257</v>
+      </c>
+      <c r="T48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3251,10 +4163,58 @@
         <v>2006</v>
       </c>
       <c r="D49" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="E49">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F49">
+        <v>8</v>
+      </c>
+      <c r="G49">
+        <v>304</v>
+      </c>
+      <c r="H49">
+        <v>4</v>
+      </c>
+      <c r="I49">
+        <v>2</v>
+      </c>
+      <c r="J49">
+        <v>5.5</v>
+      </c>
+      <c r="K49">
+        <v>230</v>
+      </c>
+      <c r="L49">
+        <v>427</v>
+      </c>
+      <c r="M49">
+        <v>1565</v>
+      </c>
+      <c r="N49">
+        <v>350</v>
+      </c>
+      <c r="O49">
+        <v>61</v>
+      </c>
+      <c r="P49">
+        <v>477</v>
+      </c>
+      <c r="Q49">
+        <v>188</v>
+      </c>
+      <c r="R49">
+        <v>139</v>
+      </c>
+      <c r="S49">
+        <v>272</v>
+      </c>
+      <c r="T49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3266,10 +4226,58 @@
         <v>2010</v>
       </c>
       <c r="D50" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E50">
+        <v>7</v>
+      </c>
+      <c r="F50">
+        <v>8</v>
+      </c>
+      <c r="G50">
+        <v>590</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
+        <v>2</v>
+      </c>
+      <c r="J50">
+        <v>3.2</v>
+      </c>
+      <c r="K50">
+        <v>310</v>
+      </c>
+      <c r="L50">
+        <v>640</v>
+      </c>
+      <c r="M50">
+        <v>1245</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>110</v>
+      </c>
+      <c r="P50">
+        <v>448</v>
+      </c>
+      <c r="Q50">
+        <v>200</v>
+      </c>
+      <c r="R50">
+        <v>117</v>
+      </c>
+      <c r="S50">
+        <v>289</v>
+      </c>
+      <c r="T50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3281,202 +4289,394 @@
         <v>2017</v>
       </c>
       <c r="D51" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E51">
+        <v>6</v>
+      </c>
+      <c r="F51">
+        <v>12</v>
+      </c>
+      <c r="G51">
+        <v>730</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <v>3.3</v>
+      </c>
+      <c r="K51">
+        <v>360</v>
+      </c>
+      <c r="L51">
+        <v>1000</v>
+      </c>
+      <c r="M51">
+        <v>1350</v>
+      </c>
+      <c r="N51">
+        <v>156</v>
+      </c>
+      <c r="O51">
+        <v>100</v>
+      </c>
+      <c r="P51">
+        <v>460</v>
+      </c>
+      <c r="Q51">
+        <v>204</v>
+      </c>
+      <c r="R51">
+        <v>117</v>
+      </c>
+      <c r="S51">
+        <v>280</v>
+      </c>
+      <c r="T51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>252</v>
       </c>
       <c r="C52">
         <v>2002</v>
       </c>
       <c r="D52" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <v>218</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="I52">
+        <v>4</v>
+      </c>
+      <c r="J52">
+        <v>6.2</v>
+      </c>
+      <c r="K52">
+        <v>230</v>
+      </c>
+      <c r="L52">
+        <v>292</v>
+      </c>
+      <c r="M52">
+        <v>1470</v>
+      </c>
+      <c r="N52">
+        <v>401</v>
+      </c>
+      <c r="O52">
+        <v>60</v>
+      </c>
+      <c r="P52">
+        <v>441</v>
+      </c>
+      <c r="Q52">
+        <v>173</v>
+      </c>
+      <c r="R52">
+        <v>144</v>
+      </c>
+      <c r="S52">
+        <v>253</v>
+      </c>
+      <c r="T52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C53">
         <v>1991</v>
       </c>
       <c r="D53" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E53">
+        <v>2.9</v>
+      </c>
+      <c r="F53">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>478</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K53">
+        <v>324</v>
+      </c>
+      <c r="L53">
+        <v>577</v>
+      </c>
+      <c r="M53">
+        <v>1235</v>
+      </c>
+      <c r="N53">
+        <v>123</v>
+      </c>
+      <c r="O53">
+        <v>120</v>
+      </c>
+      <c r="P53">
+        <v>436</v>
+      </c>
+      <c r="Q53">
+        <v>197</v>
+      </c>
+      <c r="R53">
+        <v>113</v>
+      </c>
+      <c r="S53">
+        <v>245</v>
+      </c>
+      <c r="T53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C54">
         <v>2016</v>
       </c>
       <c r="D54" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="E54">
+        <v>3.8</v>
+      </c>
+      <c r="F54">
+        <v>8</v>
+      </c>
+      <c r="G54">
+        <v>675</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="J54">
+        <v>2.9</v>
+      </c>
+      <c r="K54">
+        <v>330</v>
+      </c>
+      <c r="L54">
+        <v>700</v>
+      </c>
+      <c r="M54">
+        <v>1328</v>
+      </c>
+      <c r="N54">
+        <v>145</v>
+      </c>
+      <c r="O54">
+        <v>72</v>
+      </c>
+      <c r="P54">
+        <v>451</v>
+      </c>
+      <c r="Q54">
+        <v>191</v>
+      </c>
+      <c r="R54">
+        <v>120</v>
+      </c>
+      <c r="S54">
+        <v>267</v>
+      </c>
+      <c r="T54">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C55">
         <v>2003</v>
       </c>
       <c r="D55" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C56">
         <v>2002</v>
       </c>
       <c r="D56" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C57">
         <v>2008</v>
       </c>
       <c r="D57" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58">
         <v>2023</v>
       </c>
       <c r="D58" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59">
         <v>2012</v>
       </c>
       <c r="D59" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C60">
         <v>2019</v>
       </c>
       <c r="D60" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C61">
         <v>2008</v>
       </c>
       <c r="D61" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C62">
         <v>2003</v>
       </c>
       <c r="D62" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63">
         <v>2002</v>
       </c>
       <c r="D63" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64">
         <v>2004</v>
       </c>
       <c r="D64" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3491,7 +4691,7 @@
         <v>1969</v>
       </c>
       <c r="D65" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3506,7 +4706,7 @@
         <v>1999</v>
       </c>
       <c r="D66" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3515,13 +4715,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C67">
         <v>1982</v>
       </c>
       <c r="D67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3530,13 +4730,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C68">
         <v>2006</v>
       </c>
       <c r="D68" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3545,13 +4745,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C69">
         <v>2007</v>
       </c>
       <c r="D69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3560,13 +4760,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C70">
         <v>1999</v>
       </c>
       <c r="D70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3581,7 +4781,7 @@
         <v>1999</v>
       </c>
       <c r="D71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3590,13 +4790,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C72">
         <v>1965</v>
       </c>
       <c r="D72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3605,13 +4805,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C73">
         <v>2005</v>
       </c>
       <c r="D73" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3626,7 +4826,7 @@
         <v>2018</v>
       </c>
       <c r="D74" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3635,13 +4835,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C75">
         <v>2008</v>
       </c>
       <c r="D75" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3650,13 +4850,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C76">
         <v>2017</v>
       </c>
       <c r="D76" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3665,13 +4865,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C77">
         <v>2018</v>
       </c>
       <c r="D77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3680,13 +4880,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C78">
         <v>2011</v>
       </c>
       <c r="D78" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3701,7 +4901,7 @@
         <v>2015</v>
       </c>
       <c r="D79" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3710,13 +4910,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C80">
         <v>2012</v>
       </c>
       <c r="D80" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3725,13 +4925,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C81">
         <v>2017</v>
       </c>
       <c r="D81" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3740,13 +4940,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C82">
         <v>2005</v>
       </c>
       <c r="D82" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3755,13 +4955,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C83">
         <v>2014</v>
       </c>
       <c r="D83" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3770,13 +4970,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C84">
         <v>2020</v>
       </c>
       <c r="D84" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -3785,13 +4985,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C85">
         <v>2014</v>
       </c>
       <c r="D85" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3800,13 +5000,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C86">
         <v>2008</v>
       </c>
       <c r="D86" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3815,13 +5015,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C87">
         <v>2017</v>
       </c>
       <c r="D87" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3830,13 +5030,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C88">
         <v>2014</v>
       </c>
       <c r="D88" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3845,13 +5045,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C89">
         <v>2003</v>
       </c>
       <c r="D89" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3860,13 +5060,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C90">
         <v>2023</v>
       </c>
       <c r="D90" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3875,13 +5075,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C91">
         <v>2017</v>
       </c>
       <c r="D91" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -3890,13 +5090,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C92">
         <v>2012</v>
       </c>
       <c r="D92" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3905,13 +5105,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C93">
         <v>2015</v>
       </c>
       <c r="D93" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3920,13 +5120,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C94">
         <v>2005</v>
       </c>
       <c r="D94" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3941,7 +5141,7 @@
         <v>1964</v>
       </c>
       <c r="D95" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3950,13 +5150,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C96">
         <v>2009</v>
       </c>
       <c r="D96" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3965,13 +5165,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C97">
         <v>2018</v>
       </c>
       <c r="D97" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3980,13 +5180,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C98">
         <v>2007</v>
       </c>
       <c r="D98" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3995,13 +5195,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C99">
         <v>2009</v>
       </c>
       <c r="D99" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4010,13 +5210,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C100">
         <v>1989</v>
       </c>
       <c r="D100" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4031,7 +5231,7 @@
         <v>1967</v>
       </c>
       <c r="D101" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4046,7 +5246,7 @@
         <v>1957</v>
       </c>
       <c r="D102" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4055,13 +5255,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C103">
         <v>1963</v>
       </c>
       <c r="D103" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4070,13 +5270,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C104">
         <v>1991</v>
       </c>
       <c r="D104" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -4085,13 +5285,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C105">
         <v>2019</v>
       </c>
       <c r="D105" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -4100,13 +5300,13 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C106">
         <v>2007</v>
       </c>
       <c r="D106" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -4115,13 +5315,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C107">
         <v>1969</v>
       </c>
       <c r="D107" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -4130,13 +5330,13 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C108">
         <v>1993</v>
       </c>
       <c r="D108" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -4145,13 +5345,13 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C109">
         <v>1963</v>
       </c>
       <c r="D109" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -4160,13 +5360,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C110">
         <v>1994</v>
       </c>
       <c r="D110" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -4175,13 +5375,13 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C111">
         <v>1983</v>
       </c>
       <c r="D111" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -4190,13 +5390,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C112">
         <v>2017</v>
       </c>
       <c r="D112" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -4205,13 +5405,13 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C113">
         <v>1996</v>
       </c>
       <c r="D113" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -4220,13 +5420,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C114">
         <v>2013</v>
       </c>
       <c r="D114" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -4235,13 +5435,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C115">
         <v>2012</v>
       </c>
       <c r="D115" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -4250,13 +5450,13 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C116">
         <v>2003</v>
       </c>
       <c r="D116" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -4265,13 +5465,13 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C117">
         <v>2023</v>
       </c>
       <c r="D117" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -4280,13 +5480,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C118">
         <v>2019</v>
       </c>
       <c r="D118" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -4295,13 +5495,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C119">
         <v>2018</v>
       </c>
       <c r="D119" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -4310,13 +5510,13 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C120">
         <v>2017</v>
       </c>
       <c r="D120" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4325,13 +5525,13 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C121">
         <v>2023</v>
       </c>
       <c r="D121" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4340,13 +5540,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C122">
         <v>2013</v>
       </c>
       <c r="D122" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4355,13 +5555,13 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C123">
         <v>2002</v>
       </c>
       <c r="D123" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4370,13 +5570,13 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C124">
         <v>2013</v>
       </c>
       <c r="D124" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -4385,13 +5585,13 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C125">
         <v>2019</v>
       </c>
       <c r="D125" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4400,13 +5600,13 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C126">
         <v>1993</v>
       </c>
       <c r="D126" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -4415,13 +5615,13 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C127">
         <v>2012</v>
       </c>
       <c r="D127" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -4430,13 +5630,13 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C128">
         <v>2018</v>
       </c>
       <c r="D128" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -4445,13 +5645,13 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C129">
         <v>2010</v>
       </c>
       <c r="D129" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4460,13 +5660,13 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C130">
         <v>2004</v>
       </c>
       <c r="D130" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -4475,13 +5675,13 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C131">
         <v>2022</v>
       </c>
       <c r="D131" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -4490,13 +5690,13 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C132">
         <v>2010</v>
       </c>
       <c r="D132" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -4511,7 +5711,7 @@
         <v>2010</v>
       </c>
       <c r="D133" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -4520,13 +5720,13 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C134">
         <v>2010</v>
       </c>
       <c r="D134" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -4535,13 +5735,13 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C135">
         <v>1996</v>
       </c>
       <c r="D135" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -4550,13 +5750,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C136">
         <v>2016</v>
       </c>
       <c r="D136" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -4565,13 +5765,13 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C137">
         <v>2016</v>
       </c>
       <c r="D137" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4580,13 +5780,13 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C138">
         <v>2004</v>
       </c>
       <c r="D138" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -4595,13 +5795,13 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C139">
         <v>2006</v>
       </c>
       <c r="D139" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -4610,13 +5810,13 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C140">
         <v>2005</v>
       </c>
       <c r="D140" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -4625,13 +5825,13 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C141">
         <v>2004</v>
       </c>
       <c r="D141" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4640,13 +5840,13 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C142">
         <v>2004</v>
       </c>
       <c r="D142" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4655,13 +5855,13 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C143">
         <v>1967</v>
       </c>
       <c r="D143" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -4670,13 +5870,13 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C144">
         <v>1965</v>
       </c>
       <c r="D144" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -4685,13 +5885,13 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C145">
         <v>1992</v>
       </c>
       <c r="D145" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -4700,13 +5900,13 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C146">
         <v>2021</v>
       </c>
       <c r="D146" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -4715,13 +5915,13 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C147">
         <v>2005</v>
       </c>
       <c r="D147" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4730,13 +5930,13 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C148">
         <v>2022</v>
       </c>
       <c r="D148" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4745,13 +5945,13 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C149">
         <v>2017</v>
       </c>
       <c r="D149" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4760,13 +5960,13 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C150">
         <v>2021</v>
       </c>
       <c r="D150" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -4775,13 +5975,13 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C151">
         <v>2010</v>
       </c>
       <c r="D151" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -4790,13 +5990,13 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C152">
         <v>2014</v>
       </c>
       <c r="D152" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4805,13 +6005,13 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C153">
         <v>2020</v>
       </c>
       <c r="D153" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4820,13 +6020,13 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C154">
         <v>2006</v>
       </c>
       <c r="D154" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4835,13 +6035,13 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C155">
         <v>1998</v>
       </c>
       <c r="D155" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -4850,13 +6050,13 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C156">
         <v>2009</v>
       </c>
       <c r="D156" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4865,13 +6065,13 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C157">
         <v>2007</v>
       </c>
       <c r="D157" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -4880,13 +6080,13 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C158">
         <v>2020</v>
       </c>
       <c r="D158" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4895,13 +6095,13 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C159">
         <v>2023</v>
       </c>
       <c r="D159" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4910,13 +6110,13 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C160">
         <v>2016</v>
       </c>
       <c r="D160" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4925,13 +6125,13 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C161">
         <v>1966</v>
       </c>
       <c r="D161" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4940,13 +6140,13 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C162">
         <v>2000</v>
       </c>
       <c r="D162" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4955,13 +6155,13 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C163">
         <v>1969</v>
       </c>
       <c r="D163" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4970,13 +6170,13 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C164">
         <v>2018</v>
       </c>
       <c r="D164" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4985,13 +6185,13 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C165">
         <v>1963</v>
       </c>
       <c r="D165" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -5000,13 +6200,13 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C166">
         <v>1971</v>
       </c>
       <c r="D166" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -5015,13 +6215,13 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C167">
         <v>2015</v>
       </c>
       <c r="D167" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -5030,13 +6230,13 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C168">
         <v>2017</v>
       </c>
       <c r="D168" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -5045,13 +6245,13 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C169">
         <v>2012</v>
       </c>
       <c r="D169" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -5060,13 +6260,13 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C170">
         <v>1963</v>
       </c>
       <c r="D170" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -5075,13 +6275,13 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C171">
         <v>2010</v>
       </c>
       <c r="D171" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -5090,13 +6290,13 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C172">
         <v>2007</v>
       </c>
       <c r="D172" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -5105,13 +6305,13 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C173">
         <v>2023</v>
       </c>
       <c r="D173" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -5120,13 +6320,13 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C174">
         <v>2018</v>
       </c>
       <c r="D174" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -5135,13 +6335,13 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C175">
         <v>1997</v>
       </c>
       <c r="D175" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -5150,13 +6350,13 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C176">
         <v>2007</v>
       </c>
       <c r="D176" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -5165,13 +6365,13 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C177">
         <v>1972</v>
       </c>
       <c r="D177" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -5180,13 +6380,13 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C178">
         <v>2014</v>
       </c>
       <c r="D178" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -5195,13 +6395,13 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C179">
         <v>2022</v>
       </c>
       <c r="D179" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -5210,13 +6410,13 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C180">
         <v>2018</v>
       </c>
       <c r="D180" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -5225,13 +6425,13 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C181">
         <v>1973</v>
       </c>
       <c r="D181" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -5240,13 +6440,13 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C182">
         <v>2001</v>
       </c>
       <c r="D182" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -5255,13 +6455,13 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C183">
         <v>1977</v>
       </c>
       <c r="D183" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -5270,13 +6470,13 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C184">
         <v>2005</v>
       </c>
       <c r="D184" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -5285,13 +6485,13 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C185">
         <v>2018</v>
       </c>
       <c r="D185" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -5300,13 +6500,13 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C186">
         <v>2013</v>
       </c>
       <c r="D186" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -5315,13 +6515,13 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C187">
         <v>1967</v>
       </c>
       <c r="D187" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -5330,13 +6530,13 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C188">
         <v>2022</v>
       </c>
       <c r="D188" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -5345,13 +6545,13 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C189">
         <v>2009</v>
       </c>
       <c r="D189" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -5360,13 +6560,13 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C190">
         <v>2019</v>
       </c>
       <c r="D190" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -5375,13 +6575,13 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C191">
         <v>2021</v>
       </c>
       <c r="D191" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5396,7 +6596,7 @@
         <v>2017</v>
       </c>
       <c r="D192" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -5405,13 +6605,13 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C193">
         <v>2022</v>
       </c>
       <c r="D193" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -5420,13 +6620,13 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C194">
         <v>1995</v>
       </c>
       <c r="D194" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -5435,13 +6635,13 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C195">
         <v>2016</v>
       </c>
       <c r="D195" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -5450,13 +6650,13 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C196">
         <v>2020</v>
       </c>
       <c r="D196" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5471,7 +6671,7 @@
         <v>1978</v>
       </c>
       <c r="D197" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -5480,13 +6680,13 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C198">
         <v>2020</v>
       </c>
       <c r="D198" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -5495,13 +6695,13 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C199">
         <v>2014</v>
       </c>
       <c r="D199" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -5510,13 +6710,13 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C200">
         <v>2012</v>
       </c>
       <c r="D200" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -5525,13 +6725,13 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C201">
         <v>2021</v>
       </c>
       <c r="D201" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -5540,13 +6740,13 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C202">
         <v>2019</v>
       </c>
       <c r="D202" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5555,13 +6755,13 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C203">
         <v>2000</v>
       </c>
       <c r="D203" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -5570,13 +6770,13 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C204">
         <v>2013</v>
       </c>
       <c r="D204" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -5585,13 +6785,13 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C205">
         <v>2018</v>
       </c>
       <c r="D205" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5600,13 +6800,13 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C206">
         <v>2017</v>
       </c>
       <c r="D206" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -5615,13 +6815,13 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C207">
         <v>2009</v>
       </c>
       <c r="D207" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5630,13 +6830,13 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C208">
         <v>2020</v>
       </c>
       <c r="D208" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -5645,13 +6845,13 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C209">
         <v>2009</v>
       </c>
       <c r="D209" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -5660,13 +6860,13 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C210">
         <v>2020</v>
       </c>
       <c r="D210" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5675,13 +6875,13 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C211">
         <v>2007</v>
       </c>
       <c r="D211" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5690,13 +6890,13 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C212">
         <v>2001</v>
       </c>
       <c r="D212" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5705,13 +6905,13 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C213">
         <v>2020</v>
       </c>
       <c r="D213" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5720,13 +6920,13 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C214">
         <v>2016</v>
       </c>
       <c r="D214" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5735,13 +6935,13 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C215">
         <v>2007</v>
       </c>
       <c r="D215" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5750,13 +6950,13 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C216">
         <v>2010</v>
       </c>
       <c r="D216" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5765,13 +6965,13 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C217">
         <v>2013</v>
       </c>
       <c r="D217" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5780,13 +6980,13 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C218">
         <v>2015</v>
       </c>
       <c r="D218" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5795,13 +6995,13 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C219">
         <v>2003</v>
       </c>
       <c r="D219" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5810,13 +7010,13 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C220">
         <v>2017</v>
       </c>
       <c r="D220" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5825,13 +7025,13 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C221">
         <v>2011</v>
       </c>
       <c r="D221" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5840,13 +7040,13 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C222">
         <v>2018</v>
       </c>
       <c r="D222" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
@@ -5855,13 +7055,13 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C223">
         <v>2014</v>
       </c>
       <c r="D223" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5870,13 +7070,13 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C224">
         <v>2007</v>
       </c>
       <c r="D224" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5885,13 +7085,13 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C225">
         <v>2005</v>
       </c>
       <c r="D225" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -5900,13 +7100,13 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C226">
         <v>2016</v>
       </c>
       <c r="D226" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -5915,13 +7115,13 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C227">
         <v>2014</v>
       </c>
       <c r="D227" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5930,13 +7130,13 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C228">
         <v>2021</v>
       </c>
       <c r="D228" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -5945,13 +7145,13 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C229">
         <v>2023</v>
       </c>
       <c r="D229" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -5960,13 +7160,13 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C230">
         <v>1971</v>
       </c>
       <c r="D230" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5975,13 +7175,13 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C231">
         <v>2015</v>
       </c>
       <c r="D231" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -5990,13 +7190,13 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C232">
         <v>2012</v>
       </c>
       <c r="D232" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -6005,13 +7205,13 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C233">
         <v>2012</v>
       </c>
       <c r="D233" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -6020,13 +7220,13 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C234">
         <v>2016</v>
       </c>
       <c r="D234" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -6035,13 +7235,13 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C235">
         <v>2015</v>
       </c>
       <c r="D235" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -6050,13 +7250,13 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C236">
         <v>2022</v>
       </c>
       <c r="D236" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -6065,13 +7265,13 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C237">
         <v>2018</v>
       </c>
       <c r="D237" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -6080,13 +7280,13 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C238">
         <v>2020</v>
       </c>
       <c r="D238" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
@@ -6095,13 +7295,13 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C239">
         <v>2023</v>
       </c>
       <c r="D239" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -6110,13 +7310,13 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C240">
         <v>2020</v>
       </c>
       <c r="D240" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -6125,13 +7325,13 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C241">
         <v>2008</v>
       </c>
       <c r="D241" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -6140,13 +7340,13 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C242">
         <v>2006</v>
       </c>
       <c r="D242" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New records in data
</commit_message>
<xml_diff>
--- a/Samochody.xlsx
+++ b/Samochody.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NASA\PracaInz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1849FFEC-8075-4991-A3A2-057122BEFD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D17AD44-9F6C-4471-A7BC-577F26BDA31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="257">
   <si>
     <t>Nazwa</t>
   </si>
@@ -789,6 +789,18 @@
   <si>
     <t>Subaru Impreza WRX</t>
   </si>
+  <si>
+    <t>DMC DeLorean</t>
+  </si>
+  <si>
+    <t>Plymouth GTX</t>
+  </si>
+  <si>
+    <t>Mitsubishi Eclipse</t>
+  </si>
+  <si>
+    <t>Chevrolet Camaro</t>
+  </si>
 </sst>
 </file>
 
@@ -1105,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T242"/>
+  <dimension ref="A1:T246"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="D247" sqref="D247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16190,7 +16202,7 @@
     </row>
     <row r="240" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A240">
-        <f t="shared" ref="A240:A242" si="4">A239+1</f>
+        <f t="shared" ref="A240:A246" si="4">A239+1</f>
         <v>239</v>
       </c>
       <c r="B240" t="s">
@@ -16253,17 +16265,16 @@
     </row>
     <row r="241" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A241">
-        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
       <c r="C241">
-        <v>2008</v>
+        <v>1995</v>
       </c>
       <c r="D241" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E241">
         <v>2</v>
@@ -16272,108 +16283,356 @@
         <v>4</v>
       </c>
       <c r="G241">
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="H241">
+        <v>4</v>
+      </c>
+      <c r="I241">
+        <v>2</v>
+      </c>
+      <c r="J241">
+        <v>7</v>
+      </c>
+      <c r="K241">
+        <v>226</v>
+      </c>
+      <c r="L241">
+        <v>290</v>
+      </c>
+      <c r="M241">
+        <v>1305</v>
+      </c>
+      <c r="N241">
+        <v>241</v>
+      </c>
+      <c r="O241">
+        <v>64</v>
+      </c>
+      <c r="P241">
+        <v>438</v>
+      </c>
+      <c r="Q241">
+        <v>175</v>
+      </c>
+      <c r="R241">
+        <v>130</v>
+      </c>
+      <c r="S241">
+        <v>251</v>
+      </c>
+      <c r="T241">
         <v>5</v>
-      </c>
-      <c r="I241">
-        <v>5</v>
-      </c>
-      <c r="J241">
-        <v>6.4</v>
-      </c>
-      <c r="K241">
-        <v>247</v>
-      </c>
-      <c r="L241">
-        <v>300</v>
-      </c>
-      <c r="M241">
-        <v>1375</v>
-      </c>
-      <c r="N241">
-        <v>341</v>
-      </c>
-      <c r="O241">
-        <v>55</v>
-      </c>
-      <c r="P241">
-        <v>432</v>
-      </c>
-      <c r="Q241">
-        <v>177</v>
-      </c>
-      <c r="R241">
-        <v>146</v>
-      </c>
-      <c r="S241">
-        <v>258</v>
-      </c>
-      <c r="T241">
-        <v>6</v>
       </c>
     </row>
     <row r="242" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" t="s">
+        <v>253</v>
+      </c>
+      <c r="C242">
+        <v>1982</v>
+      </c>
+      <c r="D242" t="s">
+        <v>241</v>
+      </c>
+      <c r="E242">
+        <v>2.9</v>
+      </c>
+      <c r="F242">
+        <v>6</v>
+      </c>
+      <c r="G242">
+        <v>145</v>
+      </c>
+      <c r="H242">
+        <v>2</v>
+      </c>
+      <c r="I242">
+        <v>2</v>
+      </c>
+      <c r="J242">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K242">
+        <v>209</v>
+      </c>
+      <c r="L242">
+        <v>225</v>
+      </c>
+      <c r="M242">
+        <v>1233</v>
+      </c>
+      <c r="N242">
+        <v>396</v>
+      </c>
+      <c r="O242">
+        <v>52</v>
+      </c>
+      <c r="P242">
+        <v>427</v>
+      </c>
+      <c r="Q242">
+        <v>199</v>
+      </c>
+      <c r="R242">
+        <v>114</v>
+      </c>
+      <c r="S242">
+        <v>241</v>
+      </c>
+      <c r="T242">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" t="s">
+        <v>254</v>
+      </c>
+      <c r="C243">
+        <v>1971</v>
+      </c>
+      <c r="D243" t="s">
+        <v>240</v>
+      </c>
+      <c r="E243">
+        <v>7.2</v>
+      </c>
+      <c r="F243">
+        <v>8</v>
+      </c>
+      <c r="G243">
+        <v>375</v>
+      </c>
+      <c r="H243">
+        <v>2</v>
+      </c>
+      <c r="I243">
+        <v>4</v>
+      </c>
+      <c r="J243">
+        <v>6</v>
+      </c>
+      <c r="K243">
+        <v>216</v>
+      </c>
+      <c r="L243">
+        <v>529</v>
+      </c>
+      <c r="M243">
+        <v>1840</v>
+      </c>
+      <c r="N243">
+        <v>438</v>
+      </c>
+      <c r="O243">
+        <v>72</v>
+      </c>
+      <c r="P243">
+        <v>516</v>
+      </c>
+      <c r="Q243">
+        <v>201</v>
+      </c>
+      <c r="R243">
+        <v>134</v>
+      </c>
+      <c r="S243">
+        <v>292</v>
+      </c>
+      <c r="T243">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>256</v>
+      </c>
+      <c r="C244">
+        <v>1972</v>
+      </c>
+      <c r="D244" t="s">
+        <v>245</v>
+      </c>
+      <c r="E244">
+        <v>5</v>
+      </c>
+      <c r="F244">
+        <v>8</v>
+      </c>
+      <c r="G244">
+        <v>203</v>
+      </c>
+      <c r="H244">
+        <v>4</v>
+      </c>
+      <c r="I244">
+        <v>2</v>
+      </c>
+      <c r="J244">
+        <v>7.8</v>
+      </c>
+      <c r="K244">
+        <v>201</v>
+      </c>
+      <c r="L244">
+        <v>407</v>
+      </c>
+      <c r="M244">
+        <v>1560</v>
+      </c>
+      <c r="N244">
+        <v>178</v>
+      </c>
+      <c r="O244">
+        <v>79</v>
+      </c>
+      <c r="P244">
+        <v>478</v>
+      </c>
+      <c r="Q244">
+        <v>189</v>
+      </c>
+      <c r="R244">
+        <v>130</v>
+      </c>
+      <c r="S244">
+        <v>274</v>
+      </c>
+      <c r="T244">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245" t="s">
+        <v>220</v>
+      </c>
+      <c r="C245">
+        <v>2008</v>
+      </c>
+      <c r="D245" t="s">
+        <v>244</v>
+      </c>
+      <c r="E245">
+        <v>2</v>
+      </c>
+      <c r="F245">
+        <v>4</v>
+      </c>
+      <c r="G245">
+        <v>240</v>
+      </c>
+      <c r="H245">
+        <v>5</v>
+      </c>
+      <c r="I245">
+        <v>5</v>
+      </c>
+      <c r="J245">
+        <v>6.4</v>
+      </c>
+      <c r="K245">
+        <v>247</v>
+      </c>
+      <c r="L245">
+        <v>300</v>
+      </c>
+      <c r="M245">
+        <v>1375</v>
+      </c>
+      <c r="N245">
+        <v>341</v>
+      </c>
+      <c r="O245">
+        <v>55</v>
+      </c>
+      <c r="P245">
+        <v>432</v>
+      </c>
+      <c r="Q245">
+        <v>177</v>
+      </c>
+      <c r="R245">
+        <v>146</v>
+      </c>
+      <c r="S245">
+        <v>258</v>
+      </c>
+      <c r="T245">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="246" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A246">
         <f t="shared" si="4"/>
-        <v>241</v>
-      </c>
-      <c r="B242" t="s">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
         <v>221</v>
       </c>
-      <c r="C242">
+      <c r="C246">
         <v>2006</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D246" t="s">
         <v>244</v>
       </c>
-      <c r="E242">
+      <c r="E246">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F242">
+      <c r="F246">
         <v>4</v>
       </c>
-      <c r="G242">
+      <c r="G246">
         <v>260</v>
       </c>
-      <c r="H242">
+      <c r="H246">
         <v>5</v>
       </c>
-      <c r="I242">
+      <c r="I246">
         <v>5</v>
       </c>
-      <c r="J242">
+      <c r="J246">
         <v>6.1</v>
       </c>
-      <c r="K242">
+      <c r="K246">
         <v>250</v>
       </c>
-      <c r="L242">
+      <c r="L246">
         <v>380</v>
       </c>
-      <c r="M242">
+      <c r="M246">
         <v>1410</v>
       </c>
-      <c r="N242">
+      <c r="N246">
         <v>290</v>
       </c>
-      <c r="O242">
+      <c r="O246">
         <v>55</v>
       </c>
-      <c r="P242">
+      <c r="P246">
         <v>444</v>
       </c>
-      <c r="Q242">
+      <c r="Q246">
         <v>177</v>
       </c>
-      <c r="R242">
+      <c r="R246">
         <v>147</v>
       </c>
-      <c r="S242">
+      <c r="S246">
         <v>264</v>
       </c>
-      <c r="T242">
+      <c r="T246">
         <v>6</v>
       </c>
     </row>
@@ -16384,10 +16643,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D8D5CA-9744-4893-9B14-DF471DE70DC3}">
-  <dimension ref="A1:A241"/>
+  <dimension ref="A1:A245"/>
   <sheetViews>
-    <sheetView topLeftCell="A155" workbookViewId="0">
-      <selection activeCell="A169" sqref="A169"/>
+    <sheetView topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="D236" sqref="D236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17832,12 +18091,36 @@
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" t="str">
         <f>'Kompletne dane'!B241</f>
-        <v>Seat Leon Cupra</v>
+        <v>Mitsubishi Eclipse</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241" t="str">
         <f>'Kompletne dane'!B242</f>
+        <v>DMC DeLorean</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="str">
+        <f>'Kompletne dane'!B243</f>
+        <v>Plymouth GTX</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="str">
+        <f>'Kompletne dane'!B244</f>
+        <v>Chevrolet Camaro</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="str">
+        <f>'Kompletne dane'!B245</f>
+        <v>Seat Leon Cupra</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="str">
+        <f>'Kompletne dane'!B246</f>
         <v>Mazda 3 MPS</v>
       </c>
     </row>
@@ -17848,10 +18131,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD037B1-ACD9-48BE-8904-7C9CBB062CA9}">
-  <dimension ref="A1:R241"/>
+  <dimension ref="A1:R245"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="K125" sqref="K125"/>
+    <sheetView topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="A234" sqref="A234:R245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35542,11 +35825,11 @@
     <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240">
         <f>'Kompletne dane'!C241</f>
-        <v>2008</v>
+        <v>1995</v>
       </c>
       <c r="B240" t="str">
         <f>'Kompletne dane'!D241</f>
-        <v>C</v>
+        <v>S</v>
       </c>
       <c r="C240">
         <f>'Kompletne dane'!E241</f>
@@ -35558,132 +35841,428 @@
       </c>
       <c r="E240">
         <f>'Kompletne dane'!G241</f>
-        <v>240</v>
+        <v>213</v>
       </c>
       <c r="F240">
         <f>'Kompletne dane'!H241</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G240">
         <f>'Kompletne dane'!I241</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H240">
         <f>'Kompletne dane'!J241</f>
-        <v>6.4</v>
+        <v>7</v>
       </c>
       <c r="I240">
         <f>'Kompletne dane'!K241</f>
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="J240">
         <f>'Kompletne dane'!L241</f>
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="K240">
         <f>'Kompletne dane'!M241</f>
-        <v>1375</v>
+        <v>1305</v>
       </c>
       <c r="L240">
         <f>'Kompletne dane'!N241</f>
-        <v>341</v>
+        <v>241</v>
       </c>
       <c r="M240">
         <f>'Kompletne dane'!O241</f>
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="N240">
         <f>'Kompletne dane'!P241</f>
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="O240">
         <f>'Kompletne dane'!Q241</f>
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="P240">
         <f>'Kompletne dane'!R241</f>
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="Q240">
         <f>'Kompletne dane'!S241</f>
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="R240">
         <f>'Kompletne dane'!T241</f>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="241" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A241">
         <f>'Kompletne dane'!C242</f>
-        <v>2006</v>
+        <v>1982</v>
       </c>
       <c r="B241" t="str">
         <f>'Kompletne dane'!D242</f>
-        <v>C</v>
+        <v>S</v>
       </c>
       <c r="C241">
         <f>'Kompletne dane'!E242</f>
-        <v>2.2999999999999998</v>
+        <v>2.9</v>
       </c>
       <c r="D241">
         <f>'Kompletne dane'!F242</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E241">
         <f>'Kompletne dane'!G242</f>
-        <v>260</v>
+        <v>145</v>
       </c>
       <c r="F241">
         <f>'Kompletne dane'!H242</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G241">
         <f>'Kompletne dane'!I242</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H241">
         <f>'Kompletne dane'!J242</f>
-        <v>6.1</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I241">
         <f>'Kompletne dane'!K242</f>
-        <v>250</v>
+        <v>209</v>
       </c>
       <c r="J241">
         <f>'Kompletne dane'!L242</f>
-        <v>380</v>
+        <v>225</v>
       </c>
       <c r="K241">
         <f>'Kompletne dane'!M242</f>
-        <v>1410</v>
+        <v>1233</v>
       </c>
       <c r="L241">
         <f>'Kompletne dane'!N242</f>
-        <v>290</v>
+        <v>396</v>
       </c>
       <c r="M241">
         <f>'Kompletne dane'!O242</f>
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N241">
         <f>'Kompletne dane'!P242</f>
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="O241">
         <f>'Kompletne dane'!Q242</f>
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="P241">
         <f>'Kompletne dane'!R242</f>
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="Q241">
         <f>'Kompletne dane'!S242</f>
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="R241">
         <f>'Kompletne dane'!T242</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <f>'Kompletne dane'!C243</f>
+        <v>1971</v>
+      </c>
+      <c r="B242" t="str">
+        <f>'Kompletne dane'!D243</f>
+        <v>E</v>
+      </c>
+      <c r="C242">
+        <f>'Kompletne dane'!E243</f>
+        <v>7.2</v>
+      </c>
+      <c r="D242">
+        <f>'Kompletne dane'!F243</f>
+        <v>8</v>
+      </c>
+      <c r="E242">
+        <f>'Kompletne dane'!G243</f>
+        <v>375</v>
+      </c>
+      <c r="F242">
+        <f>'Kompletne dane'!H243</f>
+        <v>2</v>
+      </c>
+      <c r="G242">
+        <f>'Kompletne dane'!I243</f>
+        <v>4</v>
+      </c>
+      <c r="H242">
+        <f>'Kompletne dane'!J243</f>
+        <v>6</v>
+      </c>
+      <c r="I242">
+        <f>'Kompletne dane'!K243</f>
+        <v>216</v>
+      </c>
+      <c r="J242">
+        <f>'Kompletne dane'!L243</f>
+        <v>529</v>
+      </c>
+      <c r="K242">
+        <f>'Kompletne dane'!M243</f>
+        <v>1840</v>
+      </c>
+      <c r="L242">
+        <f>'Kompletne dane'!N243</f>
+        <v>438</v>
+      </c>
+      <c r="M242">
+        <f>'Kompletne dane'!O243</f>
+        <v>72</v>
+      </c>
+      <c r="N242">
+        <f>'Kompletne dane'!P243</f>
+        <v>516</v>
+      </c>
+      <c r="O242">
+        <f>'Kompletne dane'!Q243</f>
+        <v>201</v>
+      </c>
+      <c r="P242">
+        <f>'Kompletne dane'!R243</f>
+        <v>134</v>
+      </c>
+      <c r="Q242">
+        <f>'Kompletne dane'!S243</f>
+        <v>292</v>
+      </c>
+      <c r="R242">
+        <f>'Kompletne dane'!T243</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <f>'Kompletne dane'!C244</f>
+        <v>1972</v>
+      </c>
+      <c r="B243" t="str">
+        <f>'Kompletne dane'!D244</f>
+        <v>D</v>
+      </c>
+      <c r="C243">
+        <f>'Kompletne dane'!E244</f>
+        <v>5</v>
+      </c>
+      <c r="D243">
+        <f>'Kompletne dane'!F244</f>
+        <v>8</v>
+      </c>
+      <c r="E243">
+        <f>'Kompletne dane'!G244</f>
+        <v>203</v>
+      </c>
+      <c r="F243">
+        <f>'Kompletne dane'!H244</f>
+        <v>4</v>
+      </c>
+      <c r="G243">
+        <f>'Kompletne dane'!I244</f>
+        <v>2</v>
+      </c>
+      <c r="H243">
+        <f>'Kompletne dane'!J244</f>
+        <v>7.8</v>
+      </c>
+      <c r="I243">
+        <f>'Kompletne dane'!K244</f>
+        <v>201</v>
+      </c>
+      <c r="J243">
+        <f>'Kompletne dane'!L244</f>
+        <v>407</v>
+      </c>
+      <c r="K243">
+        <f>'Kompletne dane'!M244</f>
+        <v>1560</v>
+      </c>
+      <c r="L243">
+        <f>'Kompletne dane'!N244</f>
+        <v>178</v>
+      </c>
+      <c r="M243">
+        <f>'Kompletne dane'!O244</f>
+        <v>79</v>
+      </c>
+      <c r="N243">
+        <f>'Kompletne dane'!P244</f>
+        <v>478</v>
+      </c>
+      <c r="O243">
+        <f>'Kompletne dane'!Q244</f>
+        <v>189</v>
+      </c>
+      <c r="P243">
+        <f>'Kompletne dane'!R244</f>
+        <v>130</v>
+      </c>
+      <c r="Q243">
+        <f>'Kompletne dane'!S244</f>
+        <v>274</v>
+      </c>
+      <c r="R243">
+        <f>'Kompletne dane'!T244</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <f>'Kompletne dane'!C245</f>
+        <v>2008</v>
+      </c>
+      <c r="B244" t="str">
+        <f>'Kompletne dane'!D245</f>
+        <v>C</v>
+      </c>
+      <c r="C244">
+        <f>'Kompletne dane'!E245</f>
+        <v>2</v>
+      </c>
+      <c r="D244">
+        <f>'Kompletne dane'!F245</f>
+        <v>4</v>
+      </c>
+      <c r="E244">
+        <f>'Kompletne dane'!G245</f>
+        <v>240</v>
+      </c>
+      <c r="F244">
+        <f>'Kompletne dane'!H245</f>
+        <v>5</v>
+      </c>
+      <c r="G244">
+        <f>'Kompletne dane'!I245</f>
+        <v>5</v>
+      </c>
+      <c r="H244">
+        <f>'Kompletne dane'!J245</f>
+        <v>6.4</v>
+      </c>
+      <c r="I244">
+        <f>'Kompletne dane'!K245</f>
+        <v>247</v>
+      </c>
+      <c r="J244">
+        <f>'Kompletne dane'!L245</f>
+        <v>300</v>
+      </c>
+      <c r="K244">
+        <f>'Kompletne dane'!M245</f>
+        <v>1375</v>
+      </c>
+      <c r="L244">
+        <f>'Kompletne dane'!N245</f>
+        <v>341</v>
+      </c>
+      <c r="M244">
+        <f>'Kompletne dane'!O245</f>
+        <v>55</v>
+      </c>
+      <c r="N244">
+        <f>'Kompletne dane'!P245</f>
+        <v>432</v>
+      </c>
+      <c r="O244">
+        <f>'Kompletne dane'!Q245</f>
+        <v>177</v>
+      </c>
+      <c r="P244">
+        <f>'Kompletne dane'!R245</f>
+        <v>146</v>
+      </c>
+      <c r="Q244">
+        <f>'Kompletne dane'!S245</f>
+        <v>258</v>
+      </c>
+      <c r="R244">
+        <f>'Kompletne dane'!T245</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <f>'Kompletne dane'!C246</f>
+        <v>2006</v>
+      </c>
+      <c r="B245" t="str">
+        <f>'Kompletne dane'!D246</f>
+        <v>C</v>
+      </c>
+      <c r="C245">
+        <f>'Kompletne dane'!E246</f>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D245">
+        <f>'Kompletne dane'!F246</f>
+        <v>4</v>
+      </c>
+      <c r="E245">
+        <f>'Kompletne dane'!G246</f>
+        <v>260</v>
+      </c>
+      <c r="F245">
+        <f>'Kompletne dane'!H246</f>
+        <v>5</v>
+      </c>
+      <c r="G245">
+        <f>'Kompletne dane'!I246</f>
+        <v>5</v>
+      </c>
+      <c r="H245">
+        <f>'Kompletne dane'!J246</f>
+        <v>6.1</v>
+      </c>
+      <c r="I245">
+        <f>'Kompletne dane'!K246</f>
+        <v>250</v>
+      </c>
+      <c r="J245">
+        <f>'Kompletne dane'!L246</f>
+        <v>380</v>
+      </c>
+      <c r="K245">
+        <f>'Kompletne dane'!M246</f>
+        <v>1410</v>
+      </c>
+      <c r="L245">
+        <f>'Kompletne dane'!N246</f>
+        <v>290</v>
+      </c>
+      <c r="M245">
+        <f>'Kompletne dane'!O246</f>
+        <v>55</v>
+      </c>
+      <c r="N245">
+        <f>'Kompletne dane'!P246</f>
+        <v>444</v>
+      </c>
+      <c r="O245">
+        <f>'Kompletne dane'!Q246</f>
+        <v>177</v>
+      </c>
+      <c r="P245">
+        <f>'Kompletne dane'!R246</f>
+        <v>147</v>
+      </c>
+      <c r="Q245">
+        <f>'Kompletne dane'!S246</f>
+        <v>264</v>
+      </c>
+      <c r="R245">
+        <f>'Kompletne dane'!T246</f>
         <v>6</v>
       </c>
     </row>
@@ -35694,10 +36273,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91F0DD7-08C7-45FC-9056-C10D607016CE}">
-  <dimension ref="A1:A241"/>
+  <dimension ref="A1:A245"/>
   <sheetViews>
-    <sheetView topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="A229" sqref="A229:A245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37139,12 +37718,36 @@
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240">
         <f>IF('Cechy aut'!B240="A",1,IF('Cechy aut'!B240="B",2,IF('Cechy aut'!B240="C",3,IF('Cechy aut'!B240="D",4,IF('Cechy aut'!B240="E",5,IF('Cechy aut'!B240="F",6,IF('Cechy aut'!B240="S",7)))))))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A241">
         <f>IF('Cechy aut'!B241="A",1,IF('Cechy aut'!B241="B",2,IF('Cechy aut'!B241="C",3,IF('Cechy aut'!B241="D",4,IF('Cechy aut'!B241="E",5,IF('Cechy aut'!B241="F",6,IF('Cechy aut'!B241="S",7)))))))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <f>IF('Cechy aut'!B242="A",1,IF('Cechy aut'!B242="B",2,IF('Cechy aut'!B242="C",3,IF('Cechy aut'!B242="D",4,IF('Cechy aut'!B242="E",5,IF('Cechy aut'!B242="F",6,IF('Cechy aut'!B242="S",7)))))))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <f>IF('Cechy aut'!B243="A",1,IF('Cechy aut'!B243="B",2,IF('Cechy aut'!B243="C",3,IF('Cechy aut'!B243="D",4,IF('Cechy aut'!B243="E",5,IF('Cechy aut'!B243="F",6,IF('Cechy aut'!B243="S",7)))))))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <f>IF('Cechy aut'!B244="A",1,IF('Cechy aut'!B244="B",2,IF('Cechy aut'!B244="C",3,IF('Cechy aut'!B244="D",4,IF('Cechy aut'!B244="E",5,IF('Cechy aut'!B244="F",6,IF('Cechy aut'!B244="S",7)))))))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <f>IF('Cechy aut'!B245="A",1,IF('Cechy aut'!B245="B",2,IF('Cechy aut'!B245="C",3,IF('Cechy aut'!B245="D",4,IF('Cechy aut'!B245="E",5,IF('Cechy aut'!B245="F",6,IF('Cechy aut'!B245="S",7)))))))</f>
         <v>3</v>
       </c>
     </row>
@@ -37155,10 +37758,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CF09BC-BA71-498C-BCF7-A747FC04EA4C}">
-  <dimension ref="A1:R241"/>
+  <dimension ref="A1:R245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V25" sqref="V25"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54855,11 +55458,11 @@
     <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240">
         <f>('Cechy aut'!A240-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))/(MAX('Cechy aut'!A$1:'Cechy aut'!A$241)-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))</f>
-        <v>0.77941176470588236</v>
+        <v>0.58823529411764708</v>
       </c>
       <c r="B240">
         <f>(Segmenty!A240-MIN(Segmenty!A$1:'Segmenty'!A$241))/(MAX(Segmenty!A$1:'Segmenty'!A$241)-MIN(Segmenty!A$1:'Segmenty'!A$241))</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="C240">
         <f>('Cechy aut'!C240-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))/(MAX('Cechy aut'!C$1:'Cechy aut'!C$241)-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))</f>
@@ -54871,132 +55474,428 @@
       </c>
       <c r="E240">
         <f>('Cechy aut'!E240-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))/(MAX('Cechy aut'!E$1:'Cechy aut'!E$241)-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))</f>
-        <v>0.10761154855643044</v>
+        <v>8.9895013123359582E-2</v>
       </c>
       <c r="F240">
         <f>('Cechy aut'!F240-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))/(MAX('Cechy aut'!F$1:'Cechy aut'!F$241)-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="G240">
         <f>('Cechy aut'!G240-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))/(MAX('Cechy aut'!G$1:'Cechy aut'!G$241)-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H240">
         <f>('Cechy aut'!H240-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))/(MAX('Cechy aut'!H$1:'Cechy aut'!H$241)-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))</f>
-        <v>0.31746031746031744</v>
+        <v>0.36507936507936506</v>
       </c>
       <c r="I240">
         <f>('Cechy aut'!I240-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))/(MAX('Cechy aut'!I$1:'Cechy aut'!I$241)-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))</f>
-        <v>0.27514792899408286</v>
+        <v>0.21301775147928995</v>
       </c>
       <c r="J240">
         <f>('Cechy aut'!J240-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))/(MAX('Cechy aut'!J$1:'Cechy aut'!J$241)-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))</f>
-        <v>0.12926992632283993</v>
+        <v>0.12257200267916946</v>
       </c>
       <c r="K240">
         <f>('Cechy aut'!K240-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))/(MAX('Cechy aut'!K$1:'Cechy aut'!K$241)-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))</f>
-        <v>0.35294117647058826</v>
+        <v>0.31862745098039214</v>
       </c>
       <c r="L240">
         <f>('Cechy aut'!L240-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))/(MAX('Cechy aut'!L$1:'Cechy aut'!L$241)-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))</f>
-        <v>0.4194341943419434</v>
+        <v>0.29643296432964328</v>
       </c>
       <c r="M240">
         <f>('Cechy aut'!M240-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))/(MAX('Cechy aut'!M$1:'Cechy aut'!M$241)-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))</f>
-        <v>0.34591194968553457</v>
+        <v>0.40251572327044027</v>
       </c>
       <c r="N240">
         <f>('Cechy aut'!N240-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))/(MAX('Cechy aut'!N$1:'Cechy aut'!N$241)-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))</f>
-        <v>0.53586497890295359</v>
+        <v>0.56118143459915615</v>
       </c>
       <c r="O240">
         <f>('Cechy aut'!O240-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))/(MAX('Cechy aut'!O$1:'Cechy aut'!O$241)-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))</f>
-        <v>0.44578313253012047</v>
+        <v>0.42168674698795183</v>
       </c>
       <c r="P240">
         <f>('Cechy aut'!P240-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))/(MAX('Cechy aut'!P$1:'Cechy aut'!P$241)-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))</f>
-        <v>0.8571428571428571</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="Q240">
         <f>('Cechy aut'!Q240-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))/(MAX('Cechy aut'!Q$1:'Cechy aut'!Q$241)-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))</f>
-        <v>0.53465346534653468</v>
+        <v>0.46534653465346537</v>
       </c>
       <c r="R240">
         <f>('Cechy aut'!R240-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))/(MAX('Cechy aut'!R$1:'Cechy aut'!R$241)-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))</f>
-        <v>0.5714285714285714</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="241" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A241">
         <f>('Cechy aut'!A241-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))/(MAX('Cechy aut'!A$1:'Cechy aut'!A$241)-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))</f>
-        <v>0.75</v>
+        <v>0.39705882352941174</v>
       </c>
       <c r="B241">
         <f>(Segmenty!A241-MIN(Segmenty!A$1:'Segmenty'!A$241))/(MAX(Segmenty!A$1:'Segmenty'!A$241)-MIN(Segmenty!A$1:'Segmenty'!A$241))</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="C241">
         <f>('Cechy aut'!C241-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))/(MAX('Cechy aut'!C$1:'Cechy aut'!C$241)-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))</f>
-        <v>0.27380952380952378</v>
+        <v>0.34523809523809523</v>
       </c>
       <c r="D241">
         <f>('Cechy aut'!D241-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))/(MAX('Cechy aut'!D$1:'Cechy aut'!D$241)-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))</f>
-        <v>0.14285714285714285</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="E241">
         <f>('Cechy aut'!E241-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))/(MAX('Cechy aut'!E$1:'Cechy aut'!E$241)-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))</f>
-        <v>0.12073490813648294</v>
+        <v>4.5275590551181105E-2</v>
       </c>
       <c r="F241">
         <f>('Cechy aut'!F241-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))/(MAX('Cechy aut'!F$1:'Cechy aut'!F$241)-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))</f>
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="G241">
         <f>('Cechy aut'!G241-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))/(MAX('Cechy aut'!G$1:'Cechy aut'!G$241)-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H241">
         <f>('Cechy aut'!H241-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))/(MAX('Cechy aut'!H$1:'Cechy aut'!H$241)-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))</f>
-        <v>0.29365079365079366</v>
+        <v>0.58730158730158732</v>
       </c>
       <c r="I241">
         <f>('Cechy aut'!I241-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))/(MAX('Cechy aut'!I$1:'Cechy aut'!I$241)-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))</f>
-        <v>0.28402366863905326</v>
+        <v>0.16272189349112426</v>
       </c>
       <c r="J241">
         <f>('Cechy aut'!J241-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))/(MAX('Cechy aut'!J$1:'Cechy aut'!J$241)-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))</f>
-        <v>0.18285331547220363</v>
+        <v>7.9035498995311454E-2</v>
       </c>
       <c r="K241">
         <f>('Cechy aut'!K241-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))/(MAX('Cechy aut'!K$1:'Cechy aut'!K$241)-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))</f>
-        <v>0.37009803921568629</v>
+        <v>0.28333333333333333</v>
       </c>
       <c r="L241">
         <f>('Cechy aut'!L241-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))/(MAX('Cechy aut'!L$1:'Cechy aut'!L$241)-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))</f>
-        <v>0.35670356703567035</v>
+        <v>0.4870848708487085</v>
       </c>
       <c r="M241">
         <f>('Cechy aut'!M241-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))/(MAX('Cechy aut'!M$1:'Cechy aut'!M$241)-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))</f>
-        <v>0.34591194968553457</v>
+        <v>0.32704402515723269</v>
       </c>
       <c r="N241">
         <f>('Cechy aut'!N241-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))/(MAX('Cechy aut'!N$1:'Cechy aut'!N$241)-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))</f>
-        <v>0.5864978902953587</v>
+        <v>0.51476793248945152</v>
       </c>
       <c r="O241">
         <f>('Cechy aut'!O241-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))/(MAX('Cechy aut'!O$1:'Cechy aut'!O$241)-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))</f>
-        <v>0.44578313253012047</v>
+        <v>0.71084337349397586</v>
       </c>
       <c r="P241">
         <f>('Cechy aut'!P241-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))/(MAX('Cechy aut'!P$1:'Cechy aut'!P$241)-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))</f>
-        <v>0.875</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="Q241">
         <f>('Cechy aut'!Q241-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))/(MAX('Cechy aut'!Q$1:'Cechy aut'!Q$241)-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))</f>
-        <v>0.59405940594059403</v>
+        <v>0.36633663366336633</v>
       </c>
       <c r="R241">
         <f>('Cechy aut'!R241-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))/(MAX('Cechy aut'!R$1:'Cechy aut'!R$241)-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))</f>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="242" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <f>('Cechy aut'!A242-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))/(MAX('Cechy aut'!A$1:'Cechy aut'!A$241)-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))</f>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="B242">
+        <f>(Segmenty!A242-MIN(Segmenty!A$1:'Segmenty'!A$241))/(MAX(Segmenty!A$1:'Segmenty'!A$241)-MIN(Segmenty!A$1:'Segmenty'!A$241))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C242">
+        <f>('Cechy aut'!C242-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))/(MAX('Cechy aut'!C$1:'Cechy aut'!C$241)-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="D242">
+        <f>('Cechy aut'!D242-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))/(MAX('Cechy aut'!D$1:'Cechy aut'!D$241)-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="E242">
+        <f>('Cechy aut'!E242-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))/(MAX('Cechy aut'!E$1:'Cechy aut'!E$241)-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))</f>
+        <v>0.19619422572178477</v>
+      </c>
+      <c r="F242">
+        <f>('Cechy aut'!F242-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))/(MAX('Cechy aut'!F$1:'Cechy aut'!F$241)-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))</f>
+        <v>0</v>
+      </c>
+      <c r="G242">
+        <f>('Cechy aut'!G242-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))/(MAX('Cechy aut'!G$1:'Cechy aut'!G$241)-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H242">
+        <f>('Cechy aut'!H242-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))/(MAX('Cechy aut'!H$1:'Cechy aut'!H$241)-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))</f>
+        <v>0.28571428571428575</v>
+      </c>
+      <c r="I242">
+        <f>('Cechy aut'!I242-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))/(MAX('Cechy aut'!I$1:'Cechy aut'!I$241)-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))</f>
+        <v>0.18343195266272189</v>
+      </c>
+      <c r="J242">
+        <f>('Cechy aut'!J242-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))/(MAX('Cechy aut'!J$1:'Cechy aut'!J$241)-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))</f>
+        <v>0.28265237776289348</v>
+      </c>
+      <c r="K242">
+        <f>('Cechy aut'!K242-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))/(MAX('Cechy aut'!K$1:'Cechy aut'!K$241)-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))</f>
+        <v>0.58088235294117652</v>
+      </c>
+      <c r="L242">
+        <f>('Cechy aut'!L242-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))/(MAX('Cechy aut'!L$1:'Cechy aut'!L$241)-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))</f>
+        <v>0.53874538745387457</v>
+      </c>
+      <c r="M242">
+        <f>('Cechy aut'!M242-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))/(MAX('Cechy aut'!M$1:'Cechy aut'!M$241)-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))</f>
+        <v>0.45283018867924529</v>
+      </c>
+      <c r="N242">
+        <f>('Cechy aut'!N242-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))/(MAX('Cechy aut'!N$1:'Cechy aut'!N$241)-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))</f>
+        <v>0.89029535864978904</v>
+      </c>
+      <c r="O242">
+        <f>('Cechy aut'!O242-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))/(MAX('Cechy aut'!O$1:'Cechy aut'!O$241)-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))</f>
+        <v>0.73493975903614461</v>
+      </c>
+      <c r="P242">
+        <f>('Cechy aut'!P242-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))/(MAX('Cechy aut'!P$1:'Cechy aut'!P$241)-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))</f>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="Q242">
+        <f>('Cechy aut'!Q242-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))/(MAX('Cechy aut'!Q$1:'Cechy aut'!Q$241)-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))</f>
+        <v>0.87128712871287128</v>
+      </c>
+      <c r="R242">
+        <f>('Cechy aut'!R242-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))/(MAX('Cechy aut'!R$1:'Cechy aut'!R$241)-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))</f>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <f>('Cechy aut'!A243-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))/(MAX('Cechy aut'!A$1:'Cechy aut'!A$241)-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))</f>
+        <v>0.25</v>
+      </c>
+      <c r="B243">
+        <f>(Segmenty!A243-MIN(Segmenty!A$1:'Segmenty'!A$241))/(MAX(Segmenty!A$1:'Segmenty'!A$241)-MIN(Segmenty!A$1:'Segmenty'!A$241))</f>
+        <v>0.5</v>
+      </c>
+      <c r="C243">
+        <f>('Cechy aut'!C243-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))/(MAX('Cechy aut'!C$1:'Cechy aut'!C$241)-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))</f>
+        <v>0.59523809523809523</v>
+      </c>
+      <c r="D243">
+        <f>('Cechy aut'!D243-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))/(MAX('Cechy aut'!D$1:'Cechy aut'!D$241)-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))</f>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="E243">
+        <f>('Cechy aut'!E243-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))/(MAX('Cechy aut'!E$1:'Cechy aut'!E$241)-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F243">
+        <f>('Cechy aut'!F243-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))/(MAX('Cechy aut'!F$1:'Cechy aut'!F$241)-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))</f>
+        <v>0.5</v>
+      </c>
+      <c r="G243">
+        <f>('Cechy aut'!G243-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))/(MAX('Cechy aut'!G$1:'Cechy aut'!G$241)-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))</f>
+        <v>0</v>
+      </c>
+      <c r="H243">
+        <f>('Cechy aut'!H243-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))/(MAX('Cechy aut'!H$1:'Cechy aut'!H$241)-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))</f>
+        <v>0.4285714285714286</v>
+      </c>
+      <c r="I243">
+        <f>('Cechy aut'!I243-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))/(MAX('Cechy aut'!I$1:'Cechy aut'!I$241)-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))</f>
+        <v>0.13905325443786981</v>
+      </c>
+      <c r="J243">
+        <f>('Cechy aut'!J243-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))/(MAX('Cechy aut'!J$1:'Cechy aut'!J$241)-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))</f>
+        <v>0.20093770931011387</v>
+      </c>
+      <c r="K243">
+        <f>('Cechy aut'!K243-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))/(MAX('Cechy aut'!K$1:'Cechy aut'!K$241)-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))</f>
+        <v>0.44362745098039214</v>
+      </c>
+      <c r="L243">
+        <f>('Cechy aut'!L243-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))/(MAX('Cechy aut'!L$1:'Cechy aut'!L$241)-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))</f>
+        <v>0.21894218942189422</v>
+      </c>
+      <c r="M243">
+        <f>('Cechy aut'!M243-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))/(MAX('Cechy aut'!M$1:'Cechy aut'!M$241)-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))</f>
+        <v>0.49685534591194969</v>
+      </c>
+      <c r="N243">
+        <f>('Cechy aut'!N243-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))/(MAX('Cechy aut'!N$1:'Cechy aut'!N$241)-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))</f>
+        <v>0.72995780590717296</v>
+      </c>
+      <c r="O243">
+        <f>('Cechy aut'!O243-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))/(MAX('Cechy aut'!O$1:'Cechy aut'!O$241)-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))</f>
+        <v>0.59036144578313254</v>
+      </c>
+      <c r="P243">
+        <f>('Cechy aut'!P243-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))/(MAX('Cechy aut'!P$1:'Cechy aut'!P$241)-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="Q243">
+        <f>('Cechy aut'!Q243-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))/(MAX('Cechy aut'!Q$1:'Cechy aut'!Q$241)-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))</f>
+        <v>0.69306930693069302</v>
+      </c>
+      <c r="R243">
+        <f>('Cechy aut'!R243-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))/(MAX('Cechy aut'!R$1:'Cechy aut'!R$241)-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))</f>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <f>('Cechy aut'!A244-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))/(MAX('Cechy aut'!A$1:'Cechy aut'!A$241)-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))</f>
+        <v>0.77941176470588236</v>
+      </c>
+      <c r="B244">
+        <f>(Segmenty!A244-MIN(Segmenty!A$1:'Segmenty'!A$241))/(MAX(Segmenty!A$1:'Segmenty'!A$241)-MIN(Segmenty!A$1:'Segmenty'!A$241))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C244">
+        <f>('Cechy aut'!C244-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))/(MAX('Cechy aut'!C$1:'Cechy aut'!C$241)-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))</f>
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="D244">
+        <f>('Cechy aut'!D244-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))/(MAX('Cechy aut'!D$1:'Cechy aut'!D$241)-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="E244">
+        <f>('Cechy aut'!E244-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))/(MAX('Cechy aut'!E$1:'Cechy aut'!E$241)-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))</f>
+        <v>0.10761154855643044</v>
+      </c>
+      <c r="F244">
+        <f>('Cechy aut'!F244-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))/(MAX('Cechy aut'!F$1:'Cechy aut'!F$241)-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))</f>
+        <v>0.75</v>
+      </c>
+      <c r="G244">
+        <f>('Cechy aut'!G244-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))/(MAX('Cechy aut'!G$1:'Cechy aut'!G$241)-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))</f>
+        <v>1</v>
+      </c>
+      <c r="H244">
+        <f>('Cechy aut'!H244-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))/(MAX('Cechy aut'!H$1:'Cechy aut'!H$241)-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))</f>
+        <v>0.31746031746031744</v>
+      </c>
+      <c r="I244">
+        <f>('Cechy aut'!I244-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))/(MAX('Cechy aut'!I$1:'Cechy aut'!I$241)-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))</f>
+        <v>0.27514792899408286</v>
+      </c>
+      <c r="J244">
+        <f>('Cechy aut'!J244-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))/(MAX('Cechy aut'!J$1:'Cechy aut'!J$241)-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))</f>
+        <v>0.12926992632283993</v>
+      </c>
+      <c r="K244">
+        <f>('Cechy aut'!K244-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))/(MAX('Cechy aut'!K$1:'Cechy aut'!K$241)-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))</f>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="L244">
+        <f>('Cechy aut'!L244-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))/(MAX('Cechy aut'!L$1:'Cechy aut'!L$241)-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))</f>
+        <v>0.4194341943419434</v>
+      </c>
+      <c r="M244">
+        <f>('Cechy aut'!M244-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))/(MAX('Cechy aut'!M$1:'Cechy aut'!M$241)-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))</f>
+        <v>0.34591194968553457</v>
+      </c>
+      <c r="N244">
+        <f>('Cechy aut'!N244-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))/(MAX('Cechy aut'!N$1:'Cechy aut'!N$241)-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))</f>
+        <v>0.53586497890295359</v>
+      </c>
+      <c r="O244">
+        <f>('Cechy aut'!O244-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))/(MAX('Cechy aut'!O$1:'Cechy aut'!O$241)-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))</f>
+        <v>0.44578313253012047</v>
+      </c>
+      <c r="P244">
+        <f>('Cechy aut'!P244-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))/(MAX('Cechy aut'!P$1:'Cechy aut'!P$241)-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Q244">
+        <f>('Cechy aut'!Q244-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))/(MAX('Cechy aut'!Q$1:'Cechy aut'!Q$241)-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))</f>
+        <v>0.53465346534653468</v>
+      </c>
+      <c r="R244">
+        <f>('Cechy aut'!R244-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))/(MAX('Cechy aut'!R$1:'Cechy aut'!R$241)-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))</f>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <f>('Cechy aut'!A245-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))/(MAX('Cechy aut'!A$1:'Cechy aut'!A$241)-MIN('Cechy aut'!A$1:'Cechy aut'!A$241))</f>
+        <v>0.75</v>
+      </c>
+      <c r="B245">
+        <f>(Segmenty!A245-MIN(Segmenty!A$1:'Segmenty'!A$241))/(MAX(Segmenty!A$1:'Segmenty'!A$241)-MIN(Segmenty!A$1:'Segmenty'!A$241))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C245">
+        <f>('Cechy aut'!C245-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))/(MAX('Cechy aut'!C$1:'Cechy aut'!C$241)-MIN('Cechy aut'!C$1:'Cechy aut'!C$241))</f>
+        <v>0.27380952380952378</v>
+      </c>
+      <c r="D245">
+        <f>('Cechy aut'!D245-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))/(MAX('Cechy aut'!D$1:'Cechy aut'!D$241)-MIN('Cechy aut'!D$1:'Cechy aut'!D$241))</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="E245">
+        <f>('Cechy aut'!E245-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))/(MAX('Cechy aut'!E$1:'Cechy aut'!E$241)-MIN('Cechy aut'!E$1:'Cechy aut'!E$241))</f>
+        <v>0.12073490813648294</v>
+      </c>
+      <c r="F245">
+        <f>('Cechy aut'!F245-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))/(MAX('Cechy aut'!F$1:'Cechy aut'!F$241)-MIN('Cechy aut'!F$1:'Cechy aut'!F$241))</f>
+        <v>0.75</v>
+      </c>
+      <c r="G245">
+        <f>('Cechy aut'!G245-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))/(MAX('Cechy aut'!G$1:'Cechy aut'!G$241)-MIN('Cechy aut'!G$1:'Cechy aut'!G$241))</f>
+        <v>1</v>
+      </c>
+      <c r="H245">
+        <f>('Cechy aut'!H245-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))/(MAX('Cechy aut'!H$1:'Cechy aut'!H$241)-MIN('Cechy aut'!H$1:'Cechy aut'!H$241))</f>
+        <v>0.29365079365079366</v>
+      </c>
+      <c r="I245">
+        <f>('Cechy aut'!I245-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))/(MAX('Cechy aut'!I$1:'Cechy aut'!I$241)-MIN('Cechy aut'!I$1:'Cechy aut'!I$241))</f>
+        <v>0.28402366863905326</v>
+      </c>
+      <c r="J245">
+        <f>('Cechy aut'!J245-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))/(MAX('Cechy aut'!J$1:'Cechy aut'!J$241)-MIN('Cechy aut'!J$1:'Cechy aut'!J$241))</f>
+        <v>0.18285331547220363</v>
+      </c>
+      <c r="K245">
+        <f>('Cechy aut'!K245-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))/(MAX('Cechy aut'!K$1:'Cechy aut'!K$241)-MIN('Cechy aut'!K$1:'Cechy aut'!K$241))</f>
+        <v>0.37009803921568629</v>
+      </c>
+      <c r="L245">
+        <f>('Cechy aut'!L245-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))/(MAX('Cechy aut'!L$1:'Cechy aut'!L$241)-MIN('Cechy aut'!L$1:'Cechy aut'!L$241))</f>
+        <v>0.35670356703567035</v>
+      </c>
+      <c r="M245">
+        <f>('Cechy aut'!M245-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))/(MAX('Cechy aut'!M$1:'Cechy aut'!M$241)-MIN('Cechy aut'!M$1:'Cechy aut'!M$241))</f>
+        <v>0.34591194968553457</v>
+      </c>
+      <c r="N245">
+        <f>('Cechy aut'!N245-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))/(MAX('Cechy aut'!N$1:'Cechy aut'!N$241)-MIN('Cechy aut'!N$1:'Cechy aut'!N$241))</f>
+        <v>0.5864978902953587</v>
+      </c>
+      <c r="O245">
+        <f>('Cechy aut'!O245-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))/(MAX('Cechy aut'!O$1:'Cechy aut'!O$241)-MIN('Cechy aut'!O$1:'Cechy aut'!O$241))</f>
+        <v>0.44578313253012047</v>
+      </c>
+      <c r="P245">
+        <f>('Cechy aut'!P245-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))/(MAX('Cechy aut'!P$1:'Cechy aut'!P$241)-MIN('Cechy aut'!P$1:'Cechy aut'!P$241))</f>
+        <v>0.875</v>
+      </c>
+      <c r="Q245">
+        <f>('Cechy aut'!Q245-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))/(MAX('Cechy aut'!Q$1:'Cechy aut'!Q$241)-MIN('Cechy aut'!Q$1:'Cechy aut'!Q$241))</f>
+        <v>0.59405940594059403</v>
+      </c>
+      <c r="R245">
+        <f>('Cechy aut'!R245-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))/(MAX('Cechy aut'!R$1:'Cechy aut'!R$241)-MIN('Cechy aut'!R$1:'Cechy aut'!R$241))</f>
         <v>0.5714285714285714</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CSV files and reading them
</commit_message>
<xml_diff>
--- a/Samochody.xlsx
+++ b/Samochody.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NASA\PracaInz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D17AD44-9F6C-4471-A7BC-577F26BDA31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426DB9AF-19BE-45FD-9144-16C499D68F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37760,8 +37760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8CF09BC-BA71-498C-BCF7-A747FC04EA4C}">
   <dimension ref="A1:R245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="Z217" sqref="Z217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed merging and names of features in excel
</commit_message>
<xml_diff>
--- a/Samochody.xlsx
+++ b/Samochody.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NASA\PracaInz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4578542D-221A-46AE-BAD7-00D673AA6437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3B66DD-12DF-449F-A2D8-1786F25E79AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28170" yWindow="1260" windowWidth="27900" windowHeight="12285" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,22 +705,7 @@
     <t>Moment obrotowy [Nm]</t>
   </si>
   <si>
-    <t>długość [cm]</t>
-  </si>
-  <si>
-    <t>szerokość [cm]</t>
-  </si>
-  <si>
-    <t>wysokość [cm]</t>
-  </si>
-  <si>
-    <t>pojemność bagażnika [l]</t>
-  </si>
-  <si>
     <t>Rozstaw osi [cm]</t>
-  </si>
-  <si>
-    <t>masa [kg]</t>
   </si>
   <si>
     <t>Porsche 911 (997) Carrera S</t>
@@ -742,12 +727,6 @@
   </si>
   <si>
     <t>Nissan Skyline GTR R34 V-Spec</t>
-  </si>
-  <si>
-    <t>prędkość maksymalna [km/h]</t>
-  </si>
-  <si>
-    <t>przyspieszenie 0-100 km/h [s]</t>
   </si>
   <si>
     <t>E</t>
@@ -780,9 +759,6 @@
     <t>Liczba biegów</t>
   </si>
   <si>
-    <t>Pojemnośc baku</t>
-  </si>
-  <si>
     <t>Bentley Continental Supersport Convertible</t>
   </si>
   <si>
@@ -799,6 +775,30 @@
   </si>
   <si>
     <t>Chevrolet Camaro</t>
+  </si>
+  <si>
+    <t>Pojemnośc baku [l]</t>
+  </si>
+  <si>
+    <t>Przyspieszenie 0-100 km/h [s]</t>
+  </si>
+  <si>
+    <t>Prędkość maksymalna [km/h]</t>
+  </si>
+  <si>
+    <t>Masa [kg]</t>
+  </si>
+  <si>
+    <t>Pojemność bagażnika [l]</t>
+  </si>
+  <si>
+    <t>Długość [cm]</t>
+  </si>
+  <si>
+    <t>Szerokość [cm]</t>
+  </si>
+  <si>
+    <t>Wysokość [cm]</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T246"/>
   <sheetViews>
-    <sheetView topLeftCell="A211" workbookViewId="0">
-      <selection activeCell="D247" sqref="D247"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1136,7 +1136,7 @@
     <col min="11" max="11" width="26.5703125" customWidth="1"/>
     <col min="12" max="12" width="22.5703125" customWidth="1"/>
     <col min="14" max="14" width="21.7109375" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
     <col min="16" max="16" width="11.85546875" customWidth="1"/>
     <col min="17" max="17" width="13.5703125" customWidth="1"/>
     <col min="18" max="18" width="13.28515625" customWidth="1"/>
@@ -1173,37 +1173,37 @@
         <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="K1" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="L1" t="s">
         <v>224</v>
       </c>
       <c r="M1" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="N1" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="O1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P1" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>255</v>
+      </c>
+      <c r="R1" t="s">
+        <v>256</v>
+      </c>
+      <c r="S1" t="s">
         <v>225</v>
       </c>
-      <c r="Q1" t="s">
-        <v>226</v>
-      </c>
-      <c r="R1" t="s">
-        <v>227</v>
-      </c>
-      <c r="S1" t="s">
-        <v>229</v>
-      </c>
       <c r="T1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
         <v>2016</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E2">
         <v>5.7</v>
@@ -1280,7 +1280,7 @@
         <v>2011</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E3">
         <v>6.2</v>
@@ -1343,7 +1343,7 @@
         <v>2019</v>
       </c>
       <c r="D4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E4">
         <v>3.3</v>
@@ -1406,7 +1406,7 @@
         <v>2011</v>
       </c>
       <c r="D5" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E5">
         <v>4.8</v>
@@ -1469,7 +1469,7 @@
         <v>1967</v>
       </c>
       <c r="D6" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E6">
         <v>4.9000000000000004</v>
@@ -1532,7 +1532,7 @@
         <v>2013</v>
       </c>
       <c r="D7" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E7">
         <v>4.3</v>
@@ -1595,7 +1595,7 @@
         <v>1970</v>
       </c>
       <c r="D8" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E8">
         <v>4.9000000000000004</v>
@@ -1658,7 +1658,7 @@
         <v>1966</v>
       </c>
       <c r="D9" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -1721,7 +1721,7 @@
         <v>1984</v>
       </c>
       <c r="D10" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E10">
         <v>2.1</v>
@@ -1784,7 +1784,7 @@
         <v>1967</v>
       </c>
       <c r="D11" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E11">
         <v>7</v>
@@ -1847,7 +1847,7 @@
         <v>2019</v>
       </c>
       <c r="D12" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1904,13 +1904,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C13">
         <v>2007</v>
       </c>
       <c r="D13" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E13">
         <v>3.8</v>
@@ -1973,7 +1973,7 @@
         <v>1986</v>
       </c>
       <c r="D14" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E14">
         <v>2.9</v>
@@ -2036,7 +2036,7 @@
         <v>2016</v>
       </c>
       <c r="D15" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E15">
         <v>3.8</v>
@@ -2099,7 +2099,7 @@
         <v>1997</v>
       </c>
       <c r="D16" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E16">
         <v>3.6</v>
@@ -2162,7 +2162,7 @@
         <v>2006</v>
       </c>
       <c r="D17" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E17">
         <v>5.4</v>
@@ -2225,7 +2225,7 @@
         <v>2004</v>
       </c>
       <c r="D18" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E18">
         <v>4.3</v>
@@ -2288,7 +2288,7 @@
         <v>2020</v>
       </c>
       <c r="D19" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -2351,7 +2351,7 @@
         <v>1998</v>
       </c>
       <c r="D20" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E20">
         <v>2.8</v>
@@ -2414,7 +2414,7 @@
         <v>2010</v>
       </c>
       <c r="D21" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E21">
         <v>1.4</v>
@@ -2477,7 +2477,7 @@
         <v>2017</v>
       </c>
       <c r="D22" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -2534,13 +2534,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C23">
         <v>2010</v>
       </c>
       <c r="D23" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E23">
         <v>6</v>
@@ -2603,7 +2603,7 @@
         <v>2010</v>
       </c>
       <c r="D24" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E24">
         <v>4.7</v>
@@ -2666,7 +2666,7 @@
         <v>2004</v>
       </c>
       <c r="D25" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -2729,7 +2729,7 @@
         <v>2015</v>
       </c>
       <c r="D26" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E26">
         <v>4.4000000000000004</v>
@@ -2792,7 +2792,7 @@
         <v>2010</v>
       </c>
       <c r="D27" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E27">
         <v>4.2</v>
@@ -2855,7 +2855,7 @@
         <v>1965</v>
       </c>
       <c r="D28" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E28">
         <v>6.4</v>
@@ -2918,7 +2918,7 @@
         <v>2008</v>
       </c>
       <c r="D29" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E29">
         <v>3.2</v>
@@ -2981,7 +2981,7 @@
         <v>1980</v>
       </c>
       <c r="D30" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E30">
         <v>3.5</v>
@@ -3044,7 +3044,7 @@
         <v>1999</v>
       </c>
       <c r="D31" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E31">
         <v>2.8</v>
@@ -3107,7 +3107,7 @@
         <v>2010</v>
       </c>
       <c r="D32" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E32">
         <v>3.6</v>
@@ -3170,7 +3170,7 @@
         <v>2002</v>
       </c>
       <c r="D33" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -3233,7 +3233,7 @@
         <v>2001</v>
       </c>
       <c r="D34" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E34">
         <v>5.7</v>
@@ -3296,7 +3296,7 @@
         <v>2002</v>
       </c>
       <c r="D35" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -3359,7 +3359,7 @@
         <v>1955</v>
       </c>
       <c r="D36" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -3422,7 +3422,7 @@
         <v>1982</v>
       </c>
       <c r="D37" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E37">
         <v>5.7</v>
@@ -3485,7 +3485,7 @@
         <v>2008</v>
       </c>
       <c r="D38" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -3548,7 +3548,7 @@
         <v>1976</v>
       </c>
       <c r="D39" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -3611,7 +3611,7 @@
         <v>2014</v>
       </c>
       <c r="D40" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E40">
         <v>4.7</v>
@@ -3674,7 +3674,7 @@
         <v>1970</v>
       </c>
       <c r="D41" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E41">
         <v>5.6</v>
@@ -3737,7 +3737,7 @@
         <v>2007</v>
       </c>
       <c r="D42" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E42">
         <v>3.8</v>
@@ -3800,7 +3800,7 @@
         <v>2013</v>
       </c>
       <c r="D43" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E43">
         <v>6.2</v>
@@ -3863,7 +3863,7 @@
         <v>2014</v>
       </c>
       <c r="D44" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E44">
         <v>3.8</v>
@@ -3926,7 +3926,7 @@
         <v>2006</v>
       </c>
       <c r="D45" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -3989,7 +3989,7 @@
         <v>2009</v>
       </c>
       <c r="D46" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E46">
         <v>3.7</v>
@@ -4052,7 +4052,7 @@
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E47">
         <v>1.4</v>
@@ -4115,7 +4115,7 @@
         <v>2003</v>
       </c>
       <c r="D48" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E48">
         <v>2</v>
@@ -4178,7 +4178,7 @@
         <v>2006</v>
       </c>
       <c r="D49" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E49">
         <v>4.5999999999999996</v>
@@ -4241,7 +4241,7 @@
         <v>2010</v>
       </c>
       <c r="D50" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -4304,7 +4304,7 @@
         <v>2017</v>
       </c>
       <c r="D51" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E51">
         <v>6</v>
@@ -4361,13 +4361,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C52">
         <v>2002</v>
       </c>
       <c r="D52" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -4430,7 +4430,7 @@
         <v>1991</v>
       </c>
       <c r="D53" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E53">
         <v>2.9</v>
@@ -4493,7 +4493,7 @@
         <v>2016</v>
       </c>
       <c r="D54" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E54">
         <v>3.8</v>
@@ -4556,7 +4556,7 @@
         <v>2003</v>
       </c>
       <c r="D55" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E55">
         <v>3.6</v>
@@ -4619,7 +4619,7 @@
         <v>2002</v>
       </c>
       <c r="D56" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E56">
         <v>2</v>
@@ -4682,7 +4682,7 @@
         <v>2008</v>
       </c>
       <c r="D57" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E57">
         <v>3.2</v>
@@ -4745,7 +4745,7 @@
         <v>2023</v>
       </c>
       <c r="D58" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E58">
         <v>4</v>
@@ -4808,7 +4808,7 @@
         <v>2012</v>
       </c>
       <c r="D59" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E59">
         <v>5.2</v>
@@ -4871,7 +4871,7 @@
         <v>2018</v>
       </c>
       <c r="D60" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="E60">
         <v>1.6</v>
@@ -4934,7 +4934,7 @@
         <v>2008</v>
       </c>
       <c r="D61" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E61">
         <v>2.5</v>
@@ -4997,7 +4997,7 @@
         <v>2003</v>
       </c>
       <c r="D62" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -5060,7 +5060,7 @@
         <v>2002</v>
       </c>
       <c r="D63" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E63">
         <v>2.2999999999999998</v>
@@ -5123,7 +5123,7 @@
         <v>2004</v>
       </c>
       <c r="D64" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E64">
         <v>1.8</v>
@@ -5186,7 +5186,7 @@
         <v>1969</v>
       </c>
       <c r="D65" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E65">
         <v>6.6</v>
@@ -5249,7 +5249,7 @@
         <v>1999</v>
       </c>
       <c r="D66" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E66">
         <v>4.5999999999999996</v>
@@ -5312,7 +5312,7 @@
         <v>1982</v>
       </c>
       <c r="D67" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E67">
         <v>1.6</v>
@@ -5375,7 +5375,7 @@
         <v>2006</v>
       </c>
       <c r="D68" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E68">
         <v>1.8</v>
@@ -5438,7 +5438,7 @@
         <v>2007</v>
       </c>
       <c r="D69" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E69">
         <v>3.5</v>
@@ -5501,7 +5501,7 @@
         <v>1999</v>
       </c>
       <c r="D70" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E70">
         <v>4.2</v>
@@ -5564,7 +5564,7 @@
         <v>1999</v>
       </c>
       <c r="D71" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E71">
         <v>5.7</v>
@@ -5627,7 +5627,7 @@
         <v>1965</v>
       </c>
       <c r="D72" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E72">
         <v>7</v>
@@ -5690,7 +5690,7 @@
         <v>2005</v>
       </c>
       <c r="D73" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E73">
         <v>4.4000000000000004</v>
@@ -5753,7 +5753,7 @@
         <v>2018</v>
       </c>
       <c r="D74" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -5816,7 +5816,7 @@
         <v>2008</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E75">
         <v>4.7</v>
@@ -5879,7 +5879,7 @@
         <v>2017</v>
       </c>
       <c r="D76" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E76">
         <v>6.2</v>
@@ -5942,7 +5942,7 @@
         <v>2018</v>
       </c>
       <c r="D77" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E77">
         <v>1.5</v>
@@ -6005,7 +6005,7 @@
         <v>2011</v>
       </c>
       <c r="D78" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E78">
         <v>3.2</v>
@@ -6068,7 +6068,7 @@
         <v>2015</v>
       </c>
       <c r="D79" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E79">
         <v>5</v>
@@ -6131,7 +6131,7 @@
         <v>2011</v>
       </c>
       <c r="D80" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E80">
         <v>2.5</v>
@@ -6194,7 +6194,7 @@
         <v>2017</v>
       </c>
       <c r="D81" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E81">
         <v>5</v>
@@ -6257,7 +6257,7 @@
         <v>2005</v>
       </c>
       <c r="D82" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E82">
         <v>6.2</v>
@@ -6320,7 +6320,7 @@
         <v>2014</v>
       </c>
       <c r="D83" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E83">
         <v>4.4000000000000004</v>
@@ -6383,7 +6383,7 @@
         <v>2020</v>
       </c>
       <c r="D84" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E84">
         <v>4</v>
@@ -6446,7 +6446,7 @@
         <v>2014</v>
       </c>
       <c r="D85" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E85">
         <v>6.5</v>
@@ -6509,7 +6509,7 @@
         <v>2008</v>
       </c>
       <c r="D86" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E86">
         <v>3.4</v>
@@ -6572,7 +6572,7 @@
         <v>2017</v>
       </c>
       <c r="D87" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E87">
         <v>8</v>
@@ -6635,7 +6635,7 @@
         <v>2014</v>
       </c>
       <c r="D88" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E88">
         <v>4.7</v>
@@ -6698,7 +6698,7 @@
         <v>2003</v>
       </c>
       <c r="D89" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E89">
         <v>1.8</v>
@@ -6761,7 +6761,7 @@
         <v>2023</v>
       </c>
       <c r="D90" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E90">
         <v>4</v>
@@ -6824,7 +6824,7 @@
         <v>2017</v>
       </c>
       <c r="D91" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E91">
         <v>4.4000000000000004</v>
@@ -6887,7 +6887,7 @@
         <v>2012</v>
       </c>
       <c r="D92" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E92">
         <v>6</v>
@@ -6950,7 +6950,7 @@
         <v>2015</v>
       </c>
       <c r="D93" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E93">
         <v>1.8</v>
@@ -7013,7 +7013,7 @@
         <v>2005</v>
       </c>
       <c r="D94" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E94">
         <v>3</v>
@@ -7076,7 +7076,7 @@
         <v>1964</v>
       </c>
       <c r="D95" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E95">
         <v>4.7</v>
@@ -7139,7 +7139,7 @@
         <v>2009</v>
       </c>
       <c r="D96" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E96">
         <v>8.4</v>
@@ -7202,7 +7202,7 @@
         <v>2018</v>
       </c>
       <c r="D97" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E97">
         <v>4.4000000000000004</v>
@@ -7265,7 +7265,7 @@
         <v>2007</v>
       </c>
       <c r="D98" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E98">
         <v>3.4</v>
@@ -7328,7 +7328,7 @@
         <v>2009</v>
       </c>
       <c r="D99" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E99">
         <v>2</v>
@@ -7391,7 +7391,7 @@
         <v>1988</v>
       </c>
       <c r="D100" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E100">
         <v>2.8</v>
@@ -7454,7 +7454,7 @@
         <v>1967</v>
       </c>
       <c r="D101" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E101">
         <v>5.3</v>
@@ -7517,7 +7517,7 @@
         <v>1957</v>
       </c>
       <c r="D102" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E102">
         <v>4.5999999999999996</v>
@@ -7580,7 +7580,7 @@
         <v>1963</v>
       </c>
       <c r="D103" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E103">
         <v>3</v>
@@ -7643,7 +7643,7 @@
         <v>1991</v>
       </c>
       <c r="D104" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E104">
         <v>3.4</v>
@@ -7706,7 +7706,7 @@
         <v>2019</v>
       </c>
       <c r="D105" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E105">
         <v>4</v>
@@ -7769,7 +7769,7 @@
         <v>2007</v>
       </c>
       <c r="D106" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E106">
         <v>2.5</v>
@@ -7826,13 +7826,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C107">
         <v>1969</v>
       </c>
       <c r="D107" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E107">
         <v>2.2999999999999998</v>
@@ -7895,7 +7895,7 @@
         <v>1993</v>
       </c>
       <c r="D108" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E108">
         <v>3.5</v>
@@ -7958,7 +7958,7 @@
         <v>1963</v>
       </c>
       <c r="D109" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E109">
         <v>2.2999999999999998</v>
@@ -8021,7 +8021,7 @@
         <v>1994</v>
       </c>
       <c r="D110" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E110">
         <v>1.6</v>
@@ -8084,7 +8084,7 @@
         <v>1983</v>
       </c>
       <c r="D111" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E111">
         <v>4.8</v>
@@ -8147,7 +8147,7 @@
         <v>2017</v>
       </c>
       <c r="D112" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E112">
         <v>4</v>
@@ -8210,7 +8210,7 @@
         <v>1996</v>
       </c>
       <c r="D113" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E113">
         <v>4.7</v>
@@ -8273,7 +8273,7 @@
         <v>2013</v>
       </c>
       <c r="D114" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E114">
         <v>3.4</v>
@@ -8336,7 +8336,7 @@
         <v>2012</v>
       </c>
       <c r="D115" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E115">
         <v>5.2</v>
@@ -8399,7 +8399,7 @@
         <v>2003</v>
       </c>
       <c r="D116" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E116">
         <v>2</v>
@@ -8462,7 +8462,7 @@
         <v>2023</v>
       </c>
       <c r="D117" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E117">
         <v>4</v>
@@ -8525,7 +8525,7 @@
         <v>2019</v>
       </c>
       <c r="D118" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E118">
         <v>4</v>
@@ -8588,7 +8588,7 @@
         <v>2018</v>
       </c>
       <c r="D119" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E119">
         <v>3.9</v>
@@ -8651,7 +8651,7 @@
         <v>2017</v>
       </c>
       <c r="D120" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E120">
         <v>3.8</v>
@@ -8714,7 +8714,7 @@
         <v>2023</v>
       </c>
       <c r="D121" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E121">
         <v>5.2</v>
@@ -8777,7 +8777,7 @@
         <v>2013</v>
       </c>
       <c r="D122" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E122">
         <v>3</v>
@@ -8840,7 +8840,7 @@
         <v>2002</v>
       </c>
       <c r="D123" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E123">
         <v>1.8</v>
@@ -8903,7 +8903,7 @@
         <v>2013</v>
       </c>
       <c r="D124" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E124">
         <v>2</v>
@@ -8966,7 +8966,7 @@
         <v>2019</v>
       </c>
       <c r="D125" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E125">
         <v>3</v>
@@ -9029,7 +9029,7 @@
         <v>1993</v>
       </c>
       <c r="D126" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E126">
         <v>4.9000000000000004</v>
@@ -9092,7 +9092,7 @@
         <v>2012</v>
       </c>
       <c r="D127" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E127">
         <v>4</v>
@@ -9155,7 +9155,7 @@
         <v>2018</v>
       </c>
       <c r="D128" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E128">
         <v>1.7</v>
@@ -9212,13 +9212,13 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C129">
         <v>2010</v>
       </c>
       <c r="D129" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E129">
         <v>5.2</v>
@@ -9275,13 +9275,13 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C130">
         <v>2004</v>
       </c>
       <c r="D130" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E130">
         <v>2</v>
@@ -9344,7 +9344,7 @@
         <v>2022</v>
       </c>
       <c r="D131" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E131">
         <v>4</v>
@@ -9407,7 +9407,7 @@
         <v>2010</v>
       </c>
       <c r="D132" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E132">
         <v>4.2</v>
@@ -9470,7 +9470,7 @@
         <v>2010</v>
       </c>
       <c r="D133" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E133">
         <v>5</v>
@@ -9533,7 +9533,7 @@
         <v>2010</v>
       </c>
       <c r="D134" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E134">
         <v>4.2</v>
@@ -9596,7 +9596,7 @@
         <v>1996</v>
       </c>
       <c r="D135" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E135">
         <v>5.5</v>
@@ -9659,7 +9659,7 @@
         <v>2016</v>
       </c>
       <c r="D136" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E136">
         <v>2</v>
@@ -9722,7 +9722,7 @@
         <v>2016</v>
       </c>
       <c r="D137" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E137">
         <v>5.5</v>
@@ -9779,13 +9779,13 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C138">
         <v>2004</v>
       </c>
       <c r="D138" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E138">
         <v>4.5999999999999996</v>
@@ -9848,7 +9848,7 @@
         <v>2006</v>
       </c>
       <c r="D139" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E139">
         <v>2</v>
@@ -9911,7 +9911,7 @@
         <v>2005</v>
       </c>
       <c r="D140" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E140">
         <v>4.9000000000000004</v>
@@ -9974,7 +9974,7 @@
         <v>2004</v>
       </c>
       <c r="D141" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E141">
         <v>4.2</v>
@@ -10037,7 +10037,7 @@
         <v>2004</v>
       </c>
       <c r="D142" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E142">
         <v>3</v>
@@ -10100,7 +10100,7 @@
         <v>1967</v>
       </c>
       <c r="D143" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="E143">
         <v>1.3</v>
@@ -10163,7 +10163,7 @@
         <v>1965</v>
       </c>
       <c r="D144" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E144">
         <v>1.6</v>
@@ -10226,7 +10226,7 @@
         <v>1982</v>
       </c>
       <c r="D145" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E145">
         <v>2</v>
@@ -10289,7 +10289,7 @@
         <v>2020</v>
       </c>
       <c r="D146" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E146">
         <v>2</v>
@@ -10352,7 +10352,7 @@
         <v>2005</v>
       </c>
       <c r="D147" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E147">
         <v>5</v>
@@ -10415,7 +10415,7 @@
         <v>2022</v>
       </c>
       <c r="D148" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E148">
         <v>3</v>
@@ -10478,7 +10478,7 @@
         <v>2017</v>
       </c>
       <c r="D149" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E149">
         <v>4.4000000000000004</v>
@@ -10541,7 +10541,7 @@
         <v>2021</v>
       </c>
       <c r="D150" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E150">
         <v>6.5</v>
@@ -10604,7 +10604,7 @@
         <v>2010</v>
       </c>
       <c r="D151" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E151">
         <v>6.5</v>
@@ -10667,7 +10667,7 @@
         <v>2014</v>
       </c>
       <c r="D152" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E152">
         <v>6.2</v>
@@ -10730,7 +10730,7 @@
         <v>2020</v>
       </c>
       <c r="D153" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E153">
         <v>4</v>
@@ -10793,7 +10793,7 @@
         <v>2008</v>
       </c>
       <c r="D154" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E154">
         <v>5.4</v>
@@ -10856,7 +10856,7 @@
         <v>1999</v>
       </c>
       <c r="D155" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E155">
         <v>6</v>
@@ -10919,7 +10919,7 @@
         <v>2009</v>
       </c>
       <c r="D156" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E156">
         <v>6.5</v>
@@ -10982,7 +10982,7 @@
         <v>2007</v>
       </c>
       <c r="D157" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E157">
         <v>1.3</v>
@@ -11045,7 +11045,7 @@
         <v>2020</v>
       </c>
       <c r="D158" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E158">
         <v>2</v>
@@ -11108,7 +11108,7 @@
         <v>2023</v>
       </c>
       <c r="D159" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E159">
         <v>3</v>
@@ -11171,7 +11171,7 @@
         <v>2016</v>
       </c>
       <c r="D160" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E160">
         <v>4</v>
@@ -11234,7 +11234,7 @@
         <v>1966</v>
       </c>
       <c r="D161" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E161">
         <v>7</v>
@@ -11297,7 +11297,7 @@
         <v>2000</v>
       </c>
       <c r="D162" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E162">
         <v>8</v>
@@ -11360,7 +11360,7 @@
         <v>1969</v>
       </c>
       <c r="D163" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E163">
         <v>7</v>
@@ -11423,7 +11423,7 @@
         <v>2018</v>
       </c>
       <c r="D164" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E164">
         <v>5.2</v>
@@ -11486,7 +11486,7 @@
         <v>1963</v>
       </c>
       <c r="D165" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E165">
         <v>4</v>
@@ -11549,7 +11549,7 @@
         <v>1970</v>
       </c>
       <c r="D166" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E166">
         <v>7.4</v>
@@ -11612,7 +11612,7 @@
         <v>2015</v>
       </c>
       <c r="D167" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E167">
         <v>2.5</v>
@@ -11675,7 +11675,7 @@
         <v>2017</v>
       </c>
       <c r="D168" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E168">
         <v>4</v>
@@ -11738,7 +11738,7 @@
         <v>2012</v>
       </c>
       <c r="D169" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E169">
         <v>3.5</v>
@@ -11801,7 +11801,7 @@
         <v>1963</v>
       </c>
       <c r="D170" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E170">
         <v>5.4</v>
@@ -11864,7 +11864,7 @@
         <v>2010</v>
       </c>
       <c r="D171" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E171">
         <v>3.8</v>
@@ -11927,7 +11927,7 @@
         <v>2007</v>
       </c>
       <c r="D172" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E172">
         <v>4.2</v>
@@ -11990,7 +11990,7 @@
         <v>2023</v>
       </c>
       <c r="D173" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E173">
         <v>0</v>
@@ -12053,7 +12053,7 @@
         <v>2018</v>
       </c>
       <c r="D174" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E174">
         <v>4</v>
@@ -12116,7 +12116,7 @@
         <v>1997</v>
       </c>
       <c r="D175" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E175">
         <v>6</v>
@@ -12179,7 +12179,7 @@
         <v>2007</v>
       </c>
       <c r="D176" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E176">
         <v>3</v>
@@ -12242,7 +12242,7 @@
         <v>1972</v>
       </c>
       <c r="D177" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E177">
         <v>7.5</v>
@@ -12305,7 +12305,7 @@
         <v>2014</v>
       </c>
       <c r="D178" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E178">
         <v>3.7</v>
@@ -12368,7 +12368,7 @@
         <v>2022</v>
       </c>
       <c r="D179" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E179">
         <v>0</v>
@@ -12431,7 +12431,7 @@
         <v>2018</v>
       </c>
       <c r="D180" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E180">
         <v>3</v>
@@ -12494,7 +12494,7 @@
         <v>1973</v>
       </c>
       <c r="D181" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E181">
         <v>2.4</v>
@@ -12557,7 +12557,7 @@
         <v>2001</v>
       </c>
       <c r="D182" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E182">
         <v>2.7</v>
@@ -12620,7 +12620,7 @@
         <v>1977</v>
       </c>
       <c r="D183" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E183">
         <v>2</v>
@@ -12683,7 +12683,7 @@
         <v>2005</v>
       </c>
       <c r="D184" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E184">
         <v>5</v>
@@ -12746,7 +12746,7 @@
         <v>2018</v>
       </c>
       <c r="D185" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E185">
         <v>2</v>
@@ -12809,7 +12809,7 @@
         <v>2013</v>
       </c>
       <c r="D186" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E186">
         <v>2</v>
@@ -12872,7 +12872,7 @@
         <v>1967</v>
       </c>
       <c r="D187" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="E187">
         <v>7</v>
@@ -12935,7 +12935,7 @@
         <v>2022</v>
       </c>
       <c r="D188" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E188">
         <v>6.5</v>
@@ -12992,13 +12992,13 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C189">
         <v>2009</v>
       </c>
       <c r="D189" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E189">
         <v>6.5</v>
@@ -13061,7 +13061,7 @@
         <v>2019</v>
       </c>
       <c r="D190" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E190">
         <v>5</v>
@@ -13124,7 +13124,7 @@
         <v>2021</v>
       </c>
       <c r="D191" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E191">
         <v>6.2</v>
@@ -13187,7 +13187,7 @@
         <v>2017</v>
       </c>
       <c r="D192" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E192">
         <v>3.5</v>
@@ -13250,7 +13250,7 @@
         <v>2022</v>
       </c>
       <c r="D193" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E193">
         <v>4.4000000000000004</v>
@@ -13313,7 +13313,7 @@
         <v>1995</v>
       </c>
       <c r="D194" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E194">
         <v>6</v>
@@ -13376,7 +13376,7 @@
         <v>2016</v>
       </c>
       <c r="D195" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E195">
         <v>7</v>
@@ -13439,7 +13439,7 @@
         <v>2020</v>
       </c>
       <c r="D196" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E196">
         <v>3.5</v>
@@ -13502,7 +13502,7 @@
         <v>1978</v>
       </c>
       <c r="D197" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E197">
         <v>5.7</v>
@@ -13565,7 +13565,7 @@
         <v>2019</v>
       </c>
       <c r="D198" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E198">
         <v>3.8</v>
@@ -13628,7 +13628,7 @@
         <v>2014</v>
       </c>
       <c r="D199" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E199">
         <v>4.5</v>
@@ -13691,7 +13691,7 @@
         <v>2012</v>
       </c>
       <c r="D200" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E200">
         <v>5.2</v>
@@ -13754,7 +13754,7 @@
         <v>2021</v>
       </c>
       <c r="D201" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E201">
         <v>6.5</v>
@@ -13817,7 +13817,7 @@
         <v>2019</v>
       </c>
       <c r="D202" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E202">
         <v>8</v>
@@ -13874,13 +13874,13 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C203">
         <v>2000</v>
       </c>
       <c r="D203" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E203">
         <v>2.6</v>
@@ -13943,7 +13943,7 @@
         <v>2013</v>
       </c>
       <c r="D204" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E204">
         <v>4.5999999999999996</v>
@@ -14006,7 +14006,7 @@
         <v>2018</v>
       </c>
       <c r="D205" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E205">
         <v>3.8</v>
@@ -14069,7 +14069,7 @@
         <v>2017</v>
       </c>
       <c r="D206" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E206">
         <v>6.2</v>
@@ -14132,7 +14132,7 @@
         <v>2009</v>
       </c>
       <c r="D207" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E207">
         <v>3.8</v>
@@ -14195,7 +14195,7 @@
         <v>2020</v>
       </c>
       <c r="D208" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E208">
         <v>3</v>
@@ -14258,7 +14258,7 @@
         <v>2009</v>
       </c>
       <c r="D209" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E209">
         <v>4</v>
@@ -14321,7 +14321,7 @@
         <v>2020</v>
       </c>
       <c r="D210" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E210">
         <v>5.2</v>
@@ -14384,7 +14384,7 @@
         <v>2007</v>
       </c>
       <c r="D211" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E211">
         <v>7</v>
@@ -14447,7 +14447,7 @@
         <v>2001</v>
       </c>
       <c r="D212" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E212">
         <v>1.3</v>
@@ -14510,7 +14510,7 @@
         <v>2020</v>
       </c>
       <c r="D213" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E213">
         <v>5.2</v>
@@ -14573,7 +14573,7 @@
         <v>2016</v>
       </c>
       <c r="D214" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E214">
         <v>4</v>
@@ -14636,7 +14636,7 @@
         <v>2007</v>
       </c>
       <c r="D215" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E215">
         <v>5.4</v>
@@ -14699,7 +14699,7 @@
         <v>2010</v>
       </c>
       <c r="D216" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E216">
         <v>3.8</v>
@@ -14762,7 +14762,7 @@
         <v>2013</v>
       </c>
       <c r="D217" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E217">
         <v>8.4</v>
@@ -14825,7 +14825,7 @@
         <v>2015</v>
       </c>
       <c r="D218" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E218">
         <v>6.5</v>
@@ -14888,7 +14888,7 @@
         <v>2003</v>
       </c>
       <c r="D219" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E219">
         <v>3.5</v>
@@ -14951,7 +14951,7 @@
         <v>2017</v>
       </c>
       <c r="D220" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E220">
         <v>5.2</v>
@@ -15014,7 +15014,7 @@
         <v>2011</v>
       </c>
       <c r="D221" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E221">
         <v>3.6</v>
@@ -15077,7 +15077,7 @@
         <v>2018</v>
       </c>
       <c r="D222" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E222">
         <v>6.2</v>
@@ -15140,7 +15140,7 @@
         <v>2014</v>
       </c>
       <c r="D223" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E223">
         <v>3.8</v>
@@ -15203,7 +15203,7 @@
         <v>2007</v>
       </c>
       <c r="D224" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E224">
         <v>2.5</v>
@@ -15266,7 +15266,7 @@
         <v>2005</v>
       </c>
       <c r="D225" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E225">
         <v>5.7</v>
@@ -15329,7 +15329,7 @@
         <v>2016</v>
       </c>
       <c r="D226" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E226">
         <v>3</v>
@@ -15392,7 +15392,7 @@
         <v>2014</v>
       </c>
       <c r="D227" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E227">
         <v>3.8</v>
@@ -15455,7 +15455,7 @@
         <v>2021</v>
       </c>
       <c r="D228" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E228">
         <v>3</v>
@@ -15518,7 +15518,7 @@
         <v>2023</v>
       </c>
       <c r="D229" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E229">
         <v>2.4</v>
@@ -15581,7 +15581,7 @@
         <v>1971</v>
       </c>
       <c r="D230" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E230">
         <v>3.9</v>
@@ -15644,7 +15644,7 @@
         <v>2015</v>
       </c>
       <c r="D231" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E231">
         <v>6.2</v>
@@ -15707,7 +15707,7 @@
         <v>2012</v>
       </c>
       <c r="D232" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E232">
         <v>5.2</v>
@@ -15770,7 +15770,7 @@
         <v>2012</v>
       </c>
       <c r="D233" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E233">
         <v>6</v>
@@ -15833,7 +15833,7 @@
         <v>2016</v>
       </c>
       <c r="D234" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E234">
         <v>6</v>
@@ -15896,7 +15896,7 @@
         <v>2015</v>
       </c>
       <c r="D235" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E235">
         <v>6.5</v>
@@ -15959,7 +15959,7 @@
         <v>2022</v>
       </c>
       <c r="D236" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E236">
         <v>3</v>
@@ -16022,7 +16022,7 @@
         <v>2018</v>
       </c>
       <c r="D237" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E237">
         <v>3</v>
@@ -16085,7 +16085,7 @@
         <v>2020</v>
       </c>
       <c r="D238" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E238">
         <v>8</v>
@@ -16148,7 +16148,7 @@
         <v>2023</v>
       </c>
       <c r="D239" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E239">
         <v>3.5</v>
@@ -16205,13 +16205,13 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="C240">
         <v>2020</v>
       </c>
       <c r="D240" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E240">
         <v>3.5</v>
@@ -16267,13 +16267,13 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C241">
         <v>1995</v>
       </c>
       <c r="D241" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E241">
         <v>2</v>
@@ -16329,13 +16329,13 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C242">
         <v>1982</v>
       </c>
       <c r="D242" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="E242">
         <v>2.9</v>
@@ -16391,13 +16391,13 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C243">
         <v>1971</v>
       </c>
       <c r="D243" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E243">
         <v>7.2</v>
@@ -16453,13 +16453,13 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C244">
         <v>1972</v>
       </c>
       <c r="D244" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E244">
         <v>5</v>
@@ -16521,7 +16521,7 @@
         <v>2008</v>
       </c>
       <c r="D245" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E245">
         <v>2</v>
@@ -16584,7 +16584,7 @@
         <v>2006</v>
       </c>
       <c r="D246" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E246">
         <v>2.2999999999999998</v>
@@ -16644,7 +16644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D8D5CA-9744-4893-9B14-DF471DE70DC3}">
   <dimension ref="A1:A245"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" workbookViewId="0">
+    <sheetView topLeftCell="A215" workbookViewId="0">
       <selection activeCell="D236" sqref="D236"/>
     </sheetView>
   </sheetViews>
@@ -36278,7 +36278,7 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36331,12 +36331,12 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <v>przyspieszenie 0-100 km/h [s]</v>
+        <v>Przyspieszenie 0-100 km/h [s]</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <v>prędkość maksymalna [km/h]</v>
+        <v>Prędkość maksymalna [km/h]</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -36346,32 +36346,32 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <v>masa [kg]</v>
+        <v>Masa [kg]</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <v>pojemność bagażnika [l]</v>
+        <v>Pojemność bagażnika [l]</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <v>Pojemnośc baku</v>
+        <v>Pojemnośc baku [l]</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <v>długość [cm]</v>
+        <v>Długość [cm]</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <v>szerokość [cm]</v>
+        <v>Szerokość [cm]</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <v>wysokość [cm]</v>
+        <v>Wysokość [cm]</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
writing results to xlsx added position column added
</commit_message>
<xml_diff>
--- a/Samochody.xlsx
+++ b/Samochody.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NASA\PracaInz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E013A5A-E53C-4B4D-A3F7-85936691D345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2516A500-B807-42AB-9659-A33509D9F192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="525" yWindow="1305" windowWidth="27900" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kompletne dane" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Rok produkcji</t>
-  </si>
-  <si>
-    <t>Numer</t>
   </si>
   <si>
     <t>Liczba cylindrów</t>
@@ -777,9 +774,6 @@
     <t>Chevrolet Camaro</t>
   </si>
   <si>
-    <t>Pojemnośc baku [l]</t>
-  </si>
-  <si>
     <t>Przyspieszenie 0-100 km/h [s]</t>
   </si>
   <si>
@@ -811,6 +805,12 @@
   </si>
   <si>
     <t>Buick Regal Grand National</t>
+  </si>
+  <si>
+    <t>Pojemność baku [l]</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -1130,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="D251" sqref="D251"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,7 +1158,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1170,13 +1170,13 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>222</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>223</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -1185,37 +1185,37 @@
         <v>2</v>
       </c>
       <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" t="s">
+        <v>223</v>
+      </c>
+      <c r="M1" t="s">
         <v>250</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>251</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>259</v>
+      </c>
+      <c r="P1" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>253</v>
+      </c>
+      <c r="R1" t="s">
+        <v>254</v>
+      </c>
+      <c r="S1" t="s">
         <v>224</v>
       </c>
-      <c r="M1" t="s">
-        <v>252</v>
-      </c>
-      <c r="N1" t="s">
-        <v>253</v>
-      </c>
-      <c r="O1" t="s">
-        <v>249</v>
-      </c>
-      <c r="P1" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>255</v>
-      </c>
-      <c r="R1" t="s">
-        <v>256</v>
-      </c>
-      <c r="S1" t="s">
-        <v>225</v>
-      </c>
       <c r="T1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -1223,13 +1223,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>2016</v>
       </c>
       <c r="D2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E2">
         <v>5.7</v>
@@ -1286,13 +1286,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>2011</v>
       </c>
       <c r="D3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E3">
         <v>6.2</v>
@@ -1349,13 +1349,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>2019</v>
       </c>
       <c r="D4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E4">
         <v>3.3</v>
@@ -1412,13 +1412,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>2011</v>
       </c>
       <c r="D5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E5">
         <v>4.8</v>
@@ -1475,13 +1475,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>1967</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E6">
         <v>4.9000000000000004</v>
@@ -1538,13 +1538,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>2013</v>
       </c>
       <c r="D7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E7">
         <v>4.3</v>
@@ -1601,13 +1601,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>1970</v>
       </c>
       <c r="D8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E8">
         <v>4.9000000000000004</v>
@@ -1664,13 +1664,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>1966</v>
       </c>
       <c r="D9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -1727,13 +1727,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>1984</v>
       </c>
       <c r="D10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E10">
         <v>2.1</v>
@@ -1790,13 +1790,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>1967</v>
       </c>
       <c r="D11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E11">
         <v>7</v>
@@ -1853,13 +1853,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12">
         <v>2019</v>
       </c>
       <c r="D12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1916,13 +1916,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C13">
         <v>2007</v>
       </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E13">
         <v>3.8</v>
@@ -1979,13 +1979,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>1986</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E14">
         <v>2.9</v>
@@ -2042,13 +2042,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>2016</v>
       </c>
       <c r="D15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E15">
         <v>3.8</v>
@@ -2105,13 +2105,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>1997</v>
       </c>
       <c r="D16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E16">
         <v>3.6</v>
@@ -2168,13 +2168,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>2006</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E17">
         <v>5.4</v>
@@ -2231,13 +2231,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>2004</v>
       </c>
       <c r="D18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E18">
         <v>4.3</v>
@@ -2294,13 +2294,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19">
         <v>2020</v>
       </c>
       <c r="D19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -2357,13 +2357,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20">
         <v>1998</v>
       </c>
       <c r="D20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E20">
         <v>2.8</v>
@@ -2420,13 +2420,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21">
         <v>2010</v>
       </c>
       <c r="D21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E21">
         <v>1.4</v>
@@ -2483,13 +2483,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>2017</v>
       </c>
       <c r="D22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -2546,13 +2546,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C23">
         <v>2010</v>
       </c>
       <c r="D23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E23">
         <v>6</v>
@@ -2609,13 +2609,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>2010</v>
       </c>
       <c r="D24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E24">
         <v>4.7</v>
@@ -2672,13 +2672,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>2004</v>
       </c>
       <c r="D25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -2735,13 +2735,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>2015</v>
       </c>
       <c r="D26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E26">
         <v>4.4000000000000004</v>
@@ -2798,13 +2798,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>2010</v>
       </c>
       <c r="D27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E27">
         <v>4.2</v>
@@ -2861,13 +2861,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>1965</v>
       </c>
       <c r="D28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E28">
         <v>6.4</v>
@@ -2924,13 +2924,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>2008</v>
       </c>
       <c r="D29" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E29">
         <v>3.2</v>
@@ -2987,13 +2987,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>1980</v>
       </c>
       <c r="D30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E30">
         <v>3.5</v>
@@ -3050,13 +3050,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31">
         <v>1999</v>
       </c>
       <c r="D31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E31">
         <v>2.8</v>
@@ -3113,13 +3113,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C32">
         <v>2010</v>
       </c>
       <c r="D32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E32">
         <v>3.6</v>
@@ -3176,13 +3176,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <v>2002</v>
       </c>
       <c r="D33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -3239,13 +3239,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34">
         <v>2001</v>
       </c>
       <c r="D34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E34">
         <v>5.7</v>
@@ -3302,13 +3302,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35">
         <v>2002</v>
       </c>
       <c r="D35" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -3365,13 +3365,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>1955</v>
       </c>
       <c r="D36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E36">
         <v>3</v>
@@ -3428,13 +3428,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37">
         <v>1982</v>
       </c>
       <c r="D37" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E37">
         <v>5.7</v>
@@ -3491,13 +3491,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>2008</v>
       </c>
       <c r="D38" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -3554,13 +3554,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39">
         <v>1976</v>
       </c>
       <c r="D39" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -3617,13 +3617,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40">
         <v>2014</v>
       </c>
       <c r="D40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E40">
         <v>4.7</v>
@@ -3680,13 +3680,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41">
         <v>1970</v>
       </c>
       <c r="D41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E41">
         <v>5.6</v>
@@ -3743,13 +3743,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42">
         <v>2007</v>
       </c>
       <c r="D42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E42">
         <v>3.8</v>
@@ -3806,13 +3806,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43">
         <v>2013</v>
       </c>
       <c r="D43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E43">
         <v>6.2</v>
@@ -3869,13 +3869,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C44">
         <v>2014</v>
       </c>
       <c r="D44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E44">
         <v>3.8</v>
@@ -3932,13 +3932,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45">
         <v>2006</v>
       </c>
       <c r="D45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -3995,13 +3995,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46">
         <v>2009</v>
       </c>
       <c r="D46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E46">
         <v>3.7</v>
@@ -4058,13 +4058,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E47">
         <v>1.4</v>
@@ -4121,13 +4121,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48">
         <v>2003</v>
       </c>
       <c r="D48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E48">
         <v>2</v>
@@ -4184,13 +4184,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49">
         <v>2006</v>
       </c>
       <c r="D49" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E49">
         <v>4.5999999999999996</v>
@@ -4247,13 +4247,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50">
         <v>2010</v>
       </c>
       <c r="D50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -4310,13 +4310,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C51">
         <v>2017</v>
       </c>
       <c r="D51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E51">
         <v>6</v>
@@ -4373,13 +4373,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C52">
         <v>2002</v>
       </c>
       <c r="D52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -4436,13 +4436,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53">
         <v>1991</v>
       </c>
       <c r="D53" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E53">
         <v>2.9</v>
@@ -4499,13 +4499,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54">
         <v>2016</v>
       </c>
       <c r="D54" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E54">
         <v>3.8</v>
@@ -4562,13 +4562,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55">
         <v>2003</v>
       </c>
       <c r="D55" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E55">
         <v>3.6</v>
@@ -4625,13 +4625,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C56">
         <v>2002</v>
       </c>
       <c r="D56" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E56">
         <v>2</v>
@@ -4688,13 +4688,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C57">
         <v>2008</v>
       </c>
       <c r="D57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E57">
         <v>3.2</v>
@@ -4751,13 +4751,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58">
         <v>2023</v>
       </c>
       <c r="D58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E58">
         <v>4</v>
@@ -4814,13 +4814,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59">
         <v>2012</v>
       </c>
       <c r="D59" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E59">
         <v>5.2</v>
@@ -4877,13 +4877,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60">
         <v>2018</v>
       </c>
       <c r="D60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E60">
         <v>1.6</v>
@@ -4940,13 +4940,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61">
         <v>2008</v>
       </c>
       <c r="D61" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E61">
         <v>2.5</v>
@@ -5003,13 +5003,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62">
         <v>2003</v>
       </c>
       <c r="D62" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -5066,13 +5066,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C63">
         <v>2002</v>
       </c>
       <c r="D63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E63">
         <v>2.2999999999999998</v>
@@ -5129,13 +5129,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64">
         <v>2004</v>
       </c>
       <c r="D64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E64">
         <v>1.8</v>
@@ -5192,13 +5192,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C65">
         <v>1969</v>
       </c>
       <c r="D65" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E65">
         <v>6.6</v>
@@ -5255,13 +5255,13 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C66">
         <v>1999</v>
       </c>
       <c r="D66" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E66">
         <v>4.5999999999999996</v>
@@ -5318,13 +5318,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C67">
         <v>1982</v>
       </c>
       <c r="D67" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E67">
         <v>1.6</v>
@@ -5381,13 +5381,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C68">
         <v>2006</v>
       </c>
       <c r="D68" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E68">
         <v>1.8</v>
@@ -5444,13 +5444,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69">
         <v>2007</v>
       </c>
       <c r="D69" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E69">
         <v>3.5</v>
@@ -5507,13 +5507,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70">
         <v>1999</v>
       </c>
       <c r="D70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E70">
         <v>4.2</v>
@@ -5570,13 +5570,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C71">
         <v>1999</v>
       </c>
       <c r="D71" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E71">
         <v>5.7</v>
@@ -5633,13 +5633,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C72">
         <v>1965</v>
       </c>
       <c r="D72" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E72">
         <v>7</v>
@@ -5696,13 +5696,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C73">
         <v>2005</v>
       </c>
       <c r="D73" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E73">
         <v>4.4000000000000004</v>
@@ -5759,13 +5759,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C74">
         <v>2018</v>
       </c>
       <c r="D74" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -5822,13 +5822,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C75">
         <v>2008</v>
       </c>
       <c r="D75" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E75">
         <v>4.7</v>
@@ -5885,13 +5885,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C76">
         <v>2017</v>
       </c>
       <c r="D76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E76">
         <v>6.2</v>
@@ -5948,13 +5948,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C77">
         <v>2018</v>
       </c>
       <c r="D77" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E77">
         <v>1.5</v>
@@ -6011,13 +6011,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C78">
         <v>2011</v>
       </c>
       <c r="D78" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E78">
         <v>3.2</v>
@@ -6074,13 +6074,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C79">
         <v>2015</v>
       </c>
       <c r="D79" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E79">
         <v>5</v>
@@ -6137,13 +6137,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C80">
         <v>2011</v>
       </c>
       <c r="D80" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E80">
         <v>2.5</v>
@@ -6200,13 +6200,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C81">
         <v>2017</v>
       </c>
       <c r="D81" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E81">
         <v>5</v>
@@ -6263,13 +6263,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C82">
         <v>2005</v>
       </c>
       <c r="D82" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E82">
         <v>6.2</v>
@@ -6326,13 +6326,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C83">
         <v>2014</v>
       </c>
       <c r="D83" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E83">
         <v>4.4000000000000004</v>
@@ -6389,13 +6389,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C84">
         <v>2020</v>
       </c>
       <c r="D84" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E84">
         <v>4</v>
@@ -6452,13 +6452,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C85">
         <v>2014</v>
       </c>
       <c r="D85" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E85">
         <v>6.5</v>
@@ -6515,13 +6515,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C86">
         <v>2008</v>
       </c>
       <c r="D86" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E86">
         <v>3.4</v>
@@ -6578,13 +6578,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C87">
         <v>2017</v>
       </c>
       <c r="D87" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E87">
         <v>8</v>
@@ -6641,13 +6641,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C88">
         <v>2014</v>
       </c>
       <c r="D88" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E88">
         <v>4.7</v>
@@ -6704,13 +6704,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C89">
         <v>2003</v>
       </c>
       <c r="D89" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E89">
         <v>1.8</v>
@@ -6767,13 +6767,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C90">
         <v>2023</v>
       </c>
       <c r="D90" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E90">
         <v>4</v>
@@ -6830,13 +6830,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C91">
         <v>2017</v>
       </c>
       <c r="D91" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E91">
         <v>4.4000000000000004</v>
@@ -6893,13 +6893,13 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C92">
         <v>2012</v>
       </c>
       <c r="D92" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E92">
         <v>6</v>
@@ -6956,13 +6956,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C93">
         <v>2015</v>
       </c>
       <c r="D93" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E93">
         <v>1.8</v>
@@ -7019,13 +7019,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C94">
         <v>2005</v>
       </c>
       <c r="D94" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E94">
         <v>3</v>
@@ -7082,13 +7082,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C95">
         <v>1964</v>
       </c>
       <c r="D95" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E95">
         <v>4.7</v>
@@ -7145,13 +7145,13 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C96">
         <v>2009</v>
       </c>
       <c r="D96" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E96">
         <v>8.4</v>
@@ -7208,13 +7208,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C97">
         <v>2018</v>
       </c>
       <c r="D97" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E97">
         <v>4.4000000000000004</v>
@@ -7271,13 +7271,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C98">
         <v>2007</v>
       </c>
       <c r="D98" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E98">
         <v>3.4</v>
@@ -7334,13 +7334,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C99">
         <v>2009</v>
       </c>
       <c r="D99" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E99">
         <v>2</v>
@@ -7397,13 +7397,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C100">
         <v>1988</v>
       </c>
       <c r="D100" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E100">
         <v>2.8</v>
@@ -7460,13 +7460,13 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C101">
         <v>1967</v>
       </c>
       <c r="D101" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E101">
         <v>5.3</v>
@@ -7523,13 +7523,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C102">
         <v>1957</v>
       </c>
       <c r="D102" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E102">
         <v>4.5999999999999996</v>
@@ -7586,13 +7586,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C103">
         <v>1963</v>
       </c>
       <c r="D103" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E103">
         <v>3</v>
@@ -7649,13 +7649,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C104">
         <v>1991</v>
       </c>
       <c r="D104" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E104">
         <v>3.4</v>
@@ -7712,13 +7712,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C105">
         <v>2019</v>
       </c>
       <c r="D105" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E105">
         <v>4</v>
@@ -7775,13 +7775,13 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C106">
         <v>2007</v>
       </c>
       <c r="D106" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E106">
         <v>2.5</v>
@@ -7838,13 +7838,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C107">
         <v>1969</v>
       </c>
       <c r="D107" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E107">
         <v>2.2999999999999998</v>
@@ -7901,13 +7901,13 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C108">
         <v>1993</v>
       </c>
       <c r="D108" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E108">
         <v>3.5</v>
@@ -7964,13 +7964,13 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C109">
         <v>1963</v>
       </c>
       <c r="D109" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E109">
         <v>2.2999999999999998</v>
@@ -8027,13 +8027,13 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C110">
         <v>1994</v>
       </c>
       <c r="D110" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E110">
         <v>1.6</v>
@@ -8090,13 +8090,13 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C111">
         <v>1983</v>
       </c>
       <c r="D111" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E111">
         <v>4.8</v>
@@ -8153,13 +8153,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C112">
         <v>2017</v>
       </c>
       <c r="D112" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E112">
         <v>4</v>
@@ -8216,13 +8216,13 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C113">
         <v>1996</v>
       </c>
       <c r="D113" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E113">
         <v>4.7</v>
@@ -8279,13 +8279,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C114">
         <v>2013</v>
       </c>
       <c r="D114" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E114">
         <v>3.4</v>
@@ -8342,13 +8342,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C115">
         <v>2012</v>
       </c>
       <c r="D115" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E115">
         <v>5.2</v>
@@ -8405,13 +8405,13 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C116">
         <v>2003</v>
       </c>
       <c r="D116" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E116">
         <v>2</v>
@@ -8468,13 +8468,13 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C117">
         <v>2023</v>
       </c>
       <c r="D117" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E117">
         <v>4</v>
@@ -8531,13 +8531,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C118">
         <v>2019</v>
       </c>
       <c r="D118" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E118">
         <v>4</v>
@@ -8594,13 +8594,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C119">
         <v>2018</v>
       </c>
       <c r="D119" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E119">
         <v>3.9</v>
@@ -8657,13 +8657,13 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C120">
         <v>2017</v>
       </c>
       <c r="D120" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E120">
         <v>3.8</v>
@@ -8720,13 +8720,13 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C121">
         <v>2023</v>
       </c>
       <c r="D121" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E121">
         <v>5.2</v>
@@ -8783,13 +8783,13 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C122">
         <v>2013</v>
       </c>
       <c r="D122" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E122">
         <v>3</v>
@@ -8846,13 +8846,13 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C123">
         <v>2002</v>
       </c>
       <c r="D123" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E123">
         <v>1.8</v>
@@ -8909,13 +8909,13 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C124">
         <v>2013</v>
       </c>
       <c r="D124" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E124">
         <v>2</v>
@@ -8972,13 +8972,13 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C125">
         <v>2019</v>
       </c>
       <c r="D125" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E125">
         <v>3</v>
@@ -9035,13 +9035,13 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C126">
         <v>1993</v>
       </c>
       <c r="D126" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E126">
         <v>4.9000000000000004</v>
@@ -9098,13 +9098,13 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C127">
         <v>2012</v>
       </c>
       <c r="D127" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E127">
         <v>4</v>
@@ -9161,13 +9161,13 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C128">
         <v>2018</v>
       </c>
       <c r="D128" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E128">
         <v>1.7</v>
@@ -9224,13 +9224,13 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C129">
         <v>2010</v>
       </c>
       <c r="D129" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E129">
         <v>5.2</v>
@@ -9287,13 +9287,13 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C130">
         <v>2004</v>
       </c>
       <c r="D130" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E130">
         <v>2</v>
@@ -9350,13 +9350,13 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C131">
         <v>2022</v>
       </c>
       <c r="D131" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E131">
         <v>4</v>
@@ -9413,13 +9413,13 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C132">
         <v>2010</v>
       </c>
       <c r="D132" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E132">
         <v>4.2</v>
@@ -9476,13 +9476,13 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C133">
         <v>2010</v>
       </c>
       <c r="D133" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E133">
         <v>5</v>
@@ -9539,13 +9539,13 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C134">
         <v>2010</v>
       </c>
       <c r="D134" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E134">
         <v>4.2</v>
@@ -9602,13 +9602,13 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C135">
         <v>1996</v>
       </c>
       <c r="D135" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E135">
         <v>5.5</v>
@@ -9665,13 +9665,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C136">
         <v>2016</v>
       </c>
       <c r="D136" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E136">
         <v>2</v>
@@ -9728,13 +9728,13 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C137">
         <v>2016</v>
       </c>
       <c r="D137" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E137">
         <v>5.5</v>
@@ -9791,13 +9791,13 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C138">
         <v>2004</v>
       </c>
       <c r="D138" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E138">
         <v>4.5999999999999996</v>
@@ -9854,13 +9854,13 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C139">
         <v>2006</v>
       </c>
       <c r="D139" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E139">
         <v>2</v>
@@ -9917,13 +9917,13 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C140">
         <v>2005</v>
       </c>
       <c r="D140" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E140">
         <v>4.9000000000000004</v>
@@ -9980,13 +9980,13 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C141">
         <v>2004</v>
       </c>
       <c r="D141" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E141">
         <v>4.2</v>
@@ -10043,13 +10043,13 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C142">
         <v>2004</v>
       </c>
       <c r="D142" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E142">
         <v>3</v>
@@ -10106,13 +10106,13 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C143">
         <v>1967</v>
       </c>
       <c r="D143" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E143">
         <v>1.3</v>
@@ -10169,13 +10169,13 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C144">
         <v>1965</v>
       </c>
       <c r="D144" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E144">
         <v>1.6</v>
@@ -10232,13 +10232,13 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C145">
         <v>1982</v>
       </c>
       <c r="D145" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E145">
         <v>2</v>
@@ -10295,13 +10295,13 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C146">
         <v>2020</v>
       </c>
       <c r="D146" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E146">
         <v>2</v>
@@ -10358,13 +10358,13 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C147">
         <v>2005</v>
       </c>
       <c r="D147" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E147">
         <v>5</v>
@@ -10421,13 +10421,13 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C148">
         <v>2022</v>
       </c>
       <c r="D148" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E148">
         <v>3</v>
@@ -10484,13 +10484,13 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C149">
         <v>2017</v>
       </c>
       <c r="D149" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E149">
         <v>4.4000000000000004</v>
@@ -10547,13 +10547,13 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C150">
         <v>2021</v>
       </c>
       <c r="D150" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E150">
         <v>6.5</v>
@@ -10610,13 +10610,13 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C151">
         <v>2010</v>
       </c>
       <c r="D151" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E151">
         <v>6.5</v>
@@ -10673,13 +10673,13 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C152">
         <v>2014</v>
       </c>
       <c r="D152" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E152">
         <v>6.2</v>
@@ -10736,13 +10736,13 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C153">
         <v>2020</v>
       </c>
       <c r="D153" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E153">
         <v>4</v>
@@ -10799,13 +10799,13 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C154">
         <v>2008</v>
       </c>
       <c r="D154" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E154">
         <v>5.4</v>
@@ -10862,13 +10862,13 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C155">
         <v>1999</v>
       </c>
       <c r="D155" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E155">
         <v>6</v>
@@ -10925,13 +10925,13 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C156">
         <v>2009</v>
       </c>
       <c r="D156" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E156">
         <v>6.5</v>
@@ -10988,13 +10988,13 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C157">
         <v>2007</v>
       </c>
       <c r="D157" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E157">
         <v>1.3</v>
@@ -11051,13 +11051,13 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C158">
         <v>2020</v>
       </c>
       <c r="D158" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E158">
         <v>2</v>
@@ -11114,13 +11114,13 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C159">
         <v>2023</v>
       </c>
       <c r="D159" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E159">
         <v>3</v>
@@ -11177,13 +11177,13 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C160">
         <v>2016</v>
       </c>
       <c r="D160" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E160">
         <v>4</v>
@@ -11240,13 +11240,13 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C161">
         <v>1966</v>
       </c>
       <c r="D161" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E161">
         <v>7</v>
@@ -11303,13 +11303,13 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C162">
         <v>2000</v>
       </c>
       <c r="D162" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E162">
         <v>8</v>
@@ -11366,13 +11366,13 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C163">
         <v>1969</v>
       </c>
       <c r="D163" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E163">
         <v>7</v>
@@ -11429,13 +11429,13 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C164">
         <v>2018</v>
       </c>
       <c r="D164" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E164">
         <v>5.2</v>
@@ -11492,13 +11492,13 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C165">
         <v>1963</v>
       </c>
       <c r="D165" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E165">
         <v>4</v>
@@ -11555,13 +11555,13 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C166">
         <v>1970</v>
       </c>
       <c r="D166" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E166">
         <v>7.4</v>
@@ -11618,13 +11618,13 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C167">
         <v>2015</v>
       </c>
       <c r="D167" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E167">
         <v>2.5</v>
@@ -11681,13 +11681,13 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C168">
         <v>2017</v>
       </c>
       <c r="D168" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E168">
         <v>4</v>
@@ -11744,13 +11744,13 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C169">
         <v>2012</v>
       </c>
       <c r="D169" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E169">
         <v>3.5</v>
@@ -11807,13 +11807,13 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C170">
         <v>1963</v>
       </c>
       <c r="D170" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E170">
         <v>5.4</v>
@@ -11870,13 +11870,13 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C171">
         <v>2010</v>
       </c>
       <c r="D171" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E171">
         <v>3.8</v>
@@ -11933,13 +11933,13 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C172">
         <v>2007</v>
       </c>
       <c r="D172" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E172">
         <v>4.2</v>
@@ -11996,13 +11996,13 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C173">
         <v>2023</v>
       </c>
       <c r="D173" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E173">
         <v>0</v>
@@ -12059,13 +12059,13 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C174">
         <v>2018</v>
       </c>
       <c r="D174" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E174">
         <v>4</v>
@@ -12122,13 +12122,13 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C175">
         <v>1997</v>
       </c>
       <c r="D175" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E175">
         <v>6</v>
@@ -12185,13 +12185,13 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C176">
         <v>2007</v>
       </c>
       <c r="D176" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E176">
         <v>3</v>
@@ -12248,13 +12248,13 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C177">
         <v>1972</v>
       </c>
       <c r="D177" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E177">
         <v>7.5</v>
@@ -12311,13 +12311,13 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C178">
         <v>2014</v>
       </c>
       <c r="D178" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E178">
         <v>3.7</v>
@@ -12374,13 +12374,13 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C179">
         <v>2022</v>
       </c>
       <c r="D179" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E179">
         <v>0</v>
@@ -12437,13 +12437,13 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C180">
         <v>2018</v>
       </c>
       <c r="D180" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E180">
         <v>3</v>
@@ -12500,13 +12500,13 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C181">
         <v>1973</v>
       </c>
       <c r="D181" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E181">
         <v>2.4</v>
@@ -12563,13 +12563,13 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C182">
         <v>2001</v>
       </c>
       <c r="D182" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E182">
         <v>2.7</v>
@@ -12626,13 +12626,13 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C183">
         <v>1977</v>
       </c>
       <c r="D183" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E183">
         <v>2</v>
@@ -12689,13 +12689,13 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C184">
         <v>2005</v>
       </c>
       <c r="D184" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E184">
         <v>5</v>
@@ -12752,13 +12752,13 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C185">
         <v>2018</v>
       </c>
       <c r="D185" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E185">
         <v>2</v>
@@ -12815,13 +12815,13 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C186">
         <v>2013</v>
       </c>
       <c r="D186" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E186">
         <v>2</v>
@@ -12878,13 +12878,13 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C187">
         <v>1967</v>
       </c>
       <c r="D187" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E187">
         <v>7</v>
@@ -12941,13 +12941,13 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C188">
         <v>2022</v>
       </c>
       <c r="D188" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E188">
         <v>6.5</v>
@@ -13004,13 +13004,13 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C189">
         <v>2009</v>
       </c>
       <c r="D189" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E189">
         <v>6.5</v>
@@ -13067,13 +13067,13 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C190">
         <v>2019</v>
       </c>
       <c r="D190" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E190">
         <v>5</v>
@@ -13130,13 +13130,13 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C191">
         <v>2021</v>
       </c>
       <c r="D191" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E191">
         <v>6.2</v>
@@ -13193,13 +13193,13 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C192">
         <v>2017</v>
       </c>
       <c r="D192" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E192">
         <v>3.5</v>
@@ -13256,13 +13256,13 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C193">
         <v>2022</v>
       </c>
       <c r="D193" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E193">
         <v>4.4000000000000004</v>
@@ -13319,13 +13319,13 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C194">
         <v>1995</v>
       </c>
       <c r="D194" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E194">
         <v>6</v>
@@ -13382,13 +13382,13 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C195">
         <v>2016</v>
       </c>
       <c r="D195" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E195">
         <v>7</v>
@@ -13445,13 +13445,13 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C196">
         <v>2020</v>
       </c>
       <c r="D196" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E196">
         <v>3.5</v>
@@ -13508,13 +13508,13 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C197">
         <v>1978</v>
       </c>
       <c r="D197" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E197">
         <v>5.7</v>
@@ -13571,13 +13571,13 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C198">
         <v>2019</v>
       </c>
       <c r="D198" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E198">
         <v>3.8</v>
@@ -13634,13 +13634,13 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C199">
         <v>2014</v>
       </c>
       <c r="D199" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E199">
         <v>4.5</v>
@@ -13697,13 +13697,13 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C200">
         <v>2012</v>
       </c>
       <c r="D200" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E200">
         <v>5.2</v>
@@ -13760,13 +13760,13 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C201">
         <v>2021</v>
       </c>
       <c r="D201" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E201">
         <v>6.5</v>
@@ -13823,13 +13823,13 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C202">
         <v>2019</v>
       </c>
       <c r="D202" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E202">
         <v>8</v>
@@ -13886,13 +13886,13 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C203">
         <v>2000</v>
       </c>
       <c r="D203" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E203">
         <v>2.6</v>
@@ -13949,13 +13949,13 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C204">
         <v>2013</v>
       </c>
       <c r="D204" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E204">
         <v>4.5999999999999996</v>
@@ -14012,13 +14012,13 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C205">
         <v>2018</v>
       </c>
       <c r="D205" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E205">
         <v>3.8</v>
@@ -14075,13 +14075,13 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C206">
         <v>2017</v>
       </c>
       <c r="D206" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E206">
         <v>6.2</v>
@@ -14138,13 +14138,13 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C207">
         <v>2009</v>
       </c>
       <c r="D207" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E207">
         <v>3.8</v>
@@ -14201,13 +14201,13 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C208">
         <v>2020</v>
       </c>
       <c r="D208" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E208">
         <v>3</v>
@@ -14264,13 +14264,13 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C209">
         <v>2009</v>
       </c>
       <c r="D209" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E209">
         <v>4</v>
@@ -14327,13 +14327,13 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C210">
         <v>2020</v>
       </c>
       <c r="D210" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E210">
         <v>5.2</v>
@@ -14390,13 +14390,13 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C211">
         <v>2007</v>
       </c>
       <c r="D211" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E211">
         <v>7</v>
@@ -14453,13 +14453,13 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C212">
         <v>2001</v>
       </c>
       <c r="D212" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E212">
         <v>1.3</v>
@@ -14516,13 +14516,13 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C213">
         <v>2020</v>
       </c>
       <c r="D213" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E213">
         <v>5.2</v>
@@ -14579,13 +14579,13 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C214">
         <v>2016</v>
       </c>
       <c r="D214" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E214">
         <v>4</v>
@@ -14642,13 +14642,13 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C215">
         <v>2007</v>
       </c>
       <c r="D215" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E215">
         <v>5.4</v>
@@ -14705,13 +14705,13 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C216">
         <v>2010</v>
       </c>
       <c r="D216" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E216">
         <v>3.8</v>
@@ -14768,13 +14768,13 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C217">
         <v>2013</v>
       </c>
       <c r="D217" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E217">
         <v>8.4</v>
@@ -14831,13 +14831,13 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C218">
         <v>2015</v>
       </c>
       <c r="D218" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E218">
         <v>6.5</v>
@@ -14894,13 +14894,13 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C219">
         <v>2003</v>
       </c>
       <c r="D219" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E219">
         <v>3.5</v>
@@ -14957,13 +14957,13 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C220">
         <v>2017</v>
       </c>
       <c r="D220" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E220">
         <v>5.2</v>
@@ -15020,13 +15020,13 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C221">
         <v>2011</v>
       </c>
       <c r="D221" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E221">
         <v>3.6</v>
@@ -15083,13 +15083,13 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C222">
         <v>2018</v>
       </c>
       <c r="D222" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E222">
         <v>6.2</v>
@@ -15146,13 +15146,13 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C223">
         <v>2014</v>
       </c>
       <c r="D223" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E223">
         <v>3.8</v>
@@ -15209,13 +15209,13 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C224">
         <v>2007</v>
       </c>
       <c r="D224" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E224">
         <v>2.5</v>
@@ -15272,13 +15272,13 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C225">
         <v>2005</v>
       </c>
       <c r="D225" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E225">
         <v>5.7</v>
@@ -15335,13 +15335,13 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C226">
         <v>2016</v>
       </c>
       <c r="D226" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E226">
         <v>3</v>
@@ -15398,13 +15398,13 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C227">
         <v>2014</v>
       </c>
       <c r="D227" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E227">
         <v>3.8</v>
@@ -15461,13 +15461,13 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C228">
         <v>2021</v>
       </c>
       <c r="D228" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E228">
         <v>3</v>
@@ -15524,13 +15524,13 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C229">
         <v>2023</v>
       </c>
       <c r="D229" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E229">
         <v>2.4</v>
@@ -15587,13 +15587,13 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C230">
         <v>1971</v>
       </c>
       <c r="D230" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E230">
         <v>3.9</v>
@@ -15650,13 +15650,13 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C231">
         <v>2015</v>
       </c>
       <c r="D231" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E231">
         <v>6.2</v>
@@ -15713,13 +15713,13 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C232">
         <v>2012</v>
       </c>
       <c r="D232" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E232">
         <v>5.2</v>
@@ -15776,13 +15776,13 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C233">
         <v>2012</v>
       </c>
       <c r="D233" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E233">
         <v>6</v>
@@ -15839,13 +15839,13 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C234">
         <v>2016</v>
       </c>
       <c r="D234" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E234">
         <v>6</v>
@@ -15902,13 +15902,13 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C235">
         <v>2015</v>
       </c>
       <c r="D235" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E235">
         <v>6.5</v>
@@ -15965,13 +15965,13 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C236">
         <v>2022</v>
       </c>
       <c r="D236" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E236">
         <v>3</v>
@@ -16028,13 +16028,13 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C237">
         <v>2018</v>
       </c>
       <c r="D237" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E237">
         <v>3</v>
@@ -16091,13 +16091,13 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C238">
         <v>2020</v>
       </c>
       <c r="D238" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E238">
         <v>8</v>
@@ -16154,13 +16154,13 @@
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C239">
         <v>2023</v>
       </c>
       <c r="D239" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E239">
         <v>3.5</v>
@@ -16217,13 +16217,13 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C240">
         <v>2020</v>
       </c>
       <c r="D240" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E240">
         <v>3.5</v>
@@ -16280,13 +16280,13 @@
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C241">
         <v>1995</v>
       </c>
       <c r="D241" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E241">
         <v>2</v>
@@ -16343,13 +16343,13 @@
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C242">
         <v>1982</v>
       </c>
       <c r="D242" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E242">
         <v>2.9</v>
@@ -16406,13 +16406,13 @@
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C243">
         <v>1971</v>
       </c>
       <c r="D243" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E243">
         <v>7.2</v>
@@ -16469,13 +16469,13 @@
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C244">
         <v>2016</v>
       </c>
       <c r="D244" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E244">
         <v>3.7</v>
@@ -16532,13 +16532,13 @@
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C245">
         <v>1993</v>
       </c>
       <c r="D245" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E245">
         <v>3.6</v>
@@ -16595,13 +16595,13 @@
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C246">
         <v>1987</v>
       </c>
       <c r="D246" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E246">
         <v>3.8</v>
@@ -16658,13 +16658,13 @@
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C247">
         <v>1995</v>
       </c>
       <c r="D247" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E247">
         <v>3</v>
@@ -16721,13 +16721,13 @@
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C248">
         <v>1972</v>
       </c>
       <c r="D248" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E248">
         <v>5</v>
@@ -16784,13 +16784,13 @@
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C249">
         <v>2008</v>
       </c>
       <c r="D249" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E249">
         <v>2</v>
@@ -16847,13 +16847,13 @@
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C250">
         <v>2006</v>
       </c>
       <c r="D250" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E250">
         <v>2.2999999999999998</v>
@@ -16911,10 +16911,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D8D5CA-9744-4893-9B14-DF471DE70DC3}">
-  <dimension ref="A1:A245"/>
+  <dimension ref="A1:A249"/>
   <sheetViews>
-    <sheetView topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="D236" sqref="D236"/>
+    <sheetView topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18376,18 +18376,42 @@
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A243" t="str">
+        <f>'Kompletne dane'!B244</f>
+        <v>W Motors Lykan Hypersport</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="str">
+        <f>'Kompletne dane'!B245</f>
+        <v>Porsche 911 Turbo (964)</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="str">
+        <f>'Kompletne dane'!B246</f>
+        <v>Buick Regal Grand National</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="str">
+        <f>'Kompletne dane'!B247</f>
+        <v>Toyota Supra A80</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="str">
         <f>'Kompletne dane'!B248</f>
         <v>Chevrolet Camaro</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" t="str">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="str">
         <f>'Kompletne dane'!B249</f>
         <v>Seat Leon Cupra</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" t="str">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="str">
         <f>'Kompletne dane'!B250</f>
         <v>Mazda 3 MPS</v>
       </c>
@@ -18399,10 +18423,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD037B1-ACD9-48BE-8904-7C9CBB062CA9}">
-  <dimension ref="A1:R245"/>
+  <dimension ref="A1:R249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S229" sqref="S229"/>
+    <sheetView topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="U240" sqref="U240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36317,222 +36341,518 @@
     </row>
     <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243">
+        <f>'Kompletne dane'!C244</f>
+        <v>2016</v>
+      </c>
+      <c r="B243">
+        <f>IF('Kompletne dane'!$D244="A",1,IF('Kompletne dane'!$D244="B",2,IF('Kompletne dane'!$D244="C",3,IF('Kompletne dane'!$D244="D",4,IF('Kompletne dane'!$D244="E",5,IF('Kompletne dane'!$D244="F",6,7))))))</f>
+        <v>7</v>
+      </c>
+      <c r="C243">
+        <f>'Kompletne dane'!E244</f>
+        <v>3.7</v>
+      </c>
+      <c r="D243">
+        <f>'Kompletne dane'!F244</f>
+        <v>6</v>
+      </c>
+      <c r="E243">
+        <f>'Kompletne dane'!G244</f>
+        <v>780</v>
+      </c>
+      <c r="F243">
+        <f>'Kompletne dane'!H244</f>
+        <v>2</v>
+      </c>
+      <c r="G243">
+        <f>'Kompletne dane'!I244</f>
+        <v>2</v>
+      </c>
+      <c r="H243">
+        <f>'Kompletne dane'!J244</f>
+        <v>2.8</v>
+      </c>
+      <c r="I243">
+        <f>'Kompletne dane'!K244</f>
+        <v>385</v>
+      </c>
+      <c r="J243">
+        <f>'Kompletne dane'!L244</f>
+        <v>960</v>
+      </c>
+      <c r="K243">
+        <f>'Kompletne dane'!M244</f>
+        <v>1400</v>
+      </c>
+      <c r="L243">
+        <f>'Kompletne dane'!N244</f>
+        <v>110</v>
+      </c>
+      <c r="M243">
+        <f>'Kompletne dane'!O244</f>
+        <v>90</v>
+      </c>
+      <c r="N243">
+        <f>'Kompletne dane'!P244</f>
+        <v>450</v>
+      </c>
+      <c r="O243">
+        <f>'Kompletne dane'!Q244</f>
+        <v>200</v>
+      </c>
+      <c r="P243">
+        <f>'Kompletne dane'!R244</f>
+        <v>118</v>
+      </c>
+      <c r="Q243">
+        <f>'Kompletne dane'!S244</f>
+        <v>263</v>
+      </c>
+      <c r="R243">
+        <f>'Kompletne dane'!T244</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <f>'Kompletne dane'!C245</f>
+        <v>1993</v>
+      </c>
+      <c r="B244">
+        <f>IF('Kompletne dane'!$D245="A",1,IF('Kompletne dane'!$D245="B",2,IF('Kompletne dane'!$D245="C",3,IF('Kompletne dane'!$D245="D",4,IF('Kompletne dane'!$D245="E",5,IF('Kompletne dane'!$D245="F",6,7))))))</f>
+        <v>7</v>
+      </c>
+      <c r="C244">
+        <f>'Kompletne dane'!E245</f>
+        <v>3.6</v>
+      </c>
+      <c r="D244">
+        <f>'Kompletne dane'!F245</f>
+        <v>6</v>
+      </c>
+      <c r="E244">
+        <f>'Kompletne dane'!G245</f>
+        <v>360</v>
+      </c>
+      <c r="F244">
+        <f>'Kompletne dane'!H245</f>
+        <v>4</v>
+      </c>
+      <c r="G244">
+        <f>'Kompletne dane'!I245</f>
+        <v>2</v>
+      </c>
+      <c r="H244">
+        <f>'Kompletne dane'!J245</f>
+        <v>4.8</v>
+      </c>
+      <c r="I244">
+        <f>'Kompletne dane'!K245</f>
+        <v>280</v>
+      </c>
+      <c r="J244">
+        <f>'Kompletne dane'!L245</f>
+        <v>520</v>
+      </c>
+      <c r="K244">
+        <f>'Kompletne dane'!M245</f>
+        <v>1470</v>
+      </c>
+      <c r="L244">
+        <f>'Kompletne dane'!N245</f>
+        <v>90</v>
+      </c>
+      <c r="M244">
+        <f>'Kompletne dane'!O245</f>
+        <v>77</v>
+      </c>
+      <c r="N244">
+        <f>'Kompletne dane'!P245</f>
+        <v>428</v>
+      </c>
+      <c r="O244">
+        <f>'Kompletne dane'!Q245</f>
+        <v>178</v>
+      </c>
+      <c r="P244">
+        <f>'Kompletne dane'!R245</f>
+        <v>129</v>
+      </c>
+      <c r="Q244">
+        <f>'Kompletne dane'!S245</f>
+        <v>227</v>
+      </c>
+      <c r="R244">
+        <f>'Kompletne dane'!T245</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <f>'Kompletne dane'!C246</f>
+        <v>1987</v>
+      </c>
+      <c r="B245">
+        <f>IF('Kompletne dane'!$D246="A",1,IF('Kompletne dane'!$D246="B",2,IF('Kompletne dane'!$D246="C",3,IF('Kompletne dane'!$D246="D",4,IF('Kompletne dane'!$D246="E",5,IF('Kompletne dane'!$D246="F",6,7))))))</f>
+        <v>5</v>
+      </c>
+      <c r="C245">
+        <f>'Kompletne dane'!E246</f>
+        <v>3.8</v>
+      </c>
+      <c r="D245">
+        <f>'Kompletne dane'!F246</f>
+        <v>6</v>
+      </c>
+      <c r="E245">
+        <f>'Kompletne dane'!G246</f>
+        <v>276</v>
+      </c>
+      <c r="F245">
+        <f>'Kompletne dane'!H246</f>
+        <v>4</v>
+      </c>
+      <c r="G245">
+        <f>'Kompletne dane'!I246</f>
+        <v>2</v>
+      </c>
+      <c r="H245">
+        <f>'Kompletne dane'!J246</f>
+        <v>5.3</v>
+      </c>
+      <c r="I245">
+        <f>'Kompletne dane'!K246</f>
+        <v>200</v>
+      </c>
+      <c r="J245">
+        <f>'Kompletne dane'!L246</f>
+        <v>488</v>
+      </c>
+      <c r="K245">
+        <f>'Kompletne dane'!M246</f>
+        <v>1576</v>
+      </c>
+      <c r="L245">
+        <f>'Kompletne dane'!N246</f>
+        <v>462</v>
+      </c>
+      <c r="M245">
+        <f>'Kompletne dane'!O246</f>
+        <v>69</v>
+      </c>
+      <c r="N245">
+        <f>'Kompletne dane'!P246</f>
+        <v>508</v>
+      </c>
+      <c r="O245">
+        <f>'Kompletne dane'!Q246</f>
+        <v>183</v>
+      </c>
+      <c r="P245">
+        <f>'Kompletne dane'!R246</f>
+        <v>136</v>
+      </c>
+      <c r="Q245">
+        <f>'Kompletne dane'!S246</f>
+        <v>275</v>
+      </c>
+      <c r="R245">
+        <f>'Kompletne dane'!T246</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <f>'Kompletne dane'!C247</f>
+        <v>1995</v>
+      </c>
+      <c r="B246">
+        <f>IF('Kompletne dane'!$D247="A",1,IF('Kompletne dane'!$D247="B",2,IF('Kompletne dane'!$D247="C",3,IF('Kompletne dane'!$D247="D",4,IF('Kompletne dane'!$D247="E",5,IF('Kompletne dane'!$D247="F",6,7))))))</f>
+        <v>7</v>
+      </c>
+      <c r="C246">
+        <f>'Kompletne dane'!E247</f>
+        <v>3</v>
+      </c>
+      <c r="D246">
+        <f>'Kompletne dane'!F247</f>
+        <v>6</v>
+      </c>
+      <c r="E246">
+        <f>'Kompletne dane'!G247</f>
+        <v>330</v>
+      </c>
+      <c r="F246">
+        <f>'Kompletne dane'!H247</f>
+        <v>4</v>
+      </c>
+      <c r="G246">
+        <f>'Kompletne dane'!I247</f>
+        <v>3</v>
+      </c>
+      <c r="H246">
+        <f>'Kompletne dane'!J247</f>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I246">
+        <f>'Kompletne dane'!K247</f>
+        <v>250</v>
+      </c>
+      <c r="J246">
+        <f>'Kompletne dane'!L247</f>
+        <v>440</v>
+      </c>
+      <c r="K246">
+        <f>'Kompletne dane'!M247</f>
+        <v>1570</v>
+      </c>
+      <c r="L246">
+        <f>'Kompletne dane'!N247</f>
+        <v>185</v>
+      </c>
+      <c r="M246">
+        <f>'Kompletne dane'!O247</f>
+        <v>70</v>
+      </c>
+      <c r="N246">
+        <f>'Kompletne dane'!P247</f>
+        <v>452</v>
+      </c>
+      <c r="O246">
+        <f>'Kompletne dane'!Q247</f>
+        <v>181</v>
+      </c>
+      <c r="P246">
+        <f>'Kompletne dane'!R247</f>
+        <v>128</v>
+      </c>
+      <c r="Q246">
+        <f>'Kompletne dane'!S247</f>
+        <v>250</v>
+      </c>
+      <c r="R246">
+        <f>'Kompletne dane'!T247</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A247">
         <f>'Kompletne dane'!C248</f>
         <v>1972</v>
       </c>
-      <c r="B243">
+      <c r="B247">
         <f>IF('Kompletne dane'!$D248="A",1,IF('Kompletne dane'!$D248="B",2,IF('Kompletne dane'!$D248="C",3,IF('Kompletne dane'!$D248="D",4,IF('Kompletne dane'!$D248="E",5,IF('Kompletne dane'!$D248="F",6,7))))))</f>
         <v>4</v>
       </c>
-      <c r="C243">
+      <c r="C247">
         <f>'Kompletne dane'!E248</f>
         <v>5</v>
       </c>
-      <c r="D243">
+      <c r="D247">
         <f>'Kompletne dane'!F248</f>
         <v>8</v>
       </c>
-      <c r="E243">
+      <c r="E247">
         <f>'Kompletne dane'!G248</f>
         <v>203</v>
       </c>
-      <c r="F243">
+      <c r="F247">
         <f>'Kompletne dane'!H248</f>
         <v>4</v>
       </c>
-      <c r="G243">
+      <c r="G247">
         <f>'Kompletne dane'!I248</f>
         <v>2</v>
       </c>
-      <c r="H243">
+      <c r="H247">
         <f>'Kompletne dane'!J248</f>
         <v>7.8</v>
       </c>
-      <c r="I243">
+      <c r="I247">
         <f>'Kompletne dane'!K248</f>
         <v>201</v>
       </c>
-      <c r="J243">
+      <c r="J247">
         <f>'Kompletne dane'!L248</f>
         <v>407</v>
       </c>
-      <c r="K243">
+      <c r="K247">
         <f>'Kompletne dane'!M248</f>
         <v>1560</v>
       </c>
-      <c r="L243">
+      <c r="L247">
         <f>'Kompletne dane'!N248</f>
         <v>178</v>
       </c>
-      <c r="M243">
+      <c r="M247">
         <f>'Kompletne dane'!O248</f>
         <v>79</v>
       </c>
-      <c r="N243">
+      <c r="N247">
         <f>'Kompletne dane'!P248</f>
         <v>478</v>
       </c>
-      <c r="O243">
+      <c r="O247">
         <f>'Kompletne dane'!Q248</f>
         <v>189</v>
       </c>
-      <c r="P243">
+      <c r="P247">
         <f>'Kompletne dane'!R248</f>
         <v>130</v>
       </c>
-      <c r="Q243">
+      <c r="Q247">
         <f>'Kompletne dane'!S248</f>
         <v>274</v>
       </c>
-      <c r="R243">
+      <c r="R247">
         <f>'Kompletne dane'!T248</f>
         <v>3</v>
       </c>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A244">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A248">
         <f>'Kompletne dane'!C249</f>
         <v>2008</v>
       </c>
-      <c r="B244">
+      <c r="B248">
         <f>IF('Kompletne dane'!$D249="A",1,IF('Kompletne dane'!$D249="B",2,IF('Kompletne dane'!$D249="C",3,IF('Kompletne dane'!$D249="D",4,IF('Kompletne dane'!$D249="E",5,IF('Kompletne dane'!$D249="F",6,7))))))</f>
         <v>3</v>
       </c>
-      <c r="C244">
+      <c r="C248">
         <f>'Kompletne dane'!E249</f>
         <v>2</v>
       </c>
-      <c r="D244">
+      <c r="D248">
         <f>'Kompletne dane'!F249</f>
         <v>4</v>
       </c>
-      <c r="E244">
+      <c r="E248">
         <f>'Kompletne dane'!G249</f>
         <v>240</v>
       </c>
-      <c r="F244">
+      <c r="F248">
         <f>'Kompletne dane'!H249</f>
         <v>5</v>
       </c>
-      <c r="G244">
+      <c r="G248">
         <f>'Kompletne dane'!I249</f>
         <v>5</v>
       </c>
-      <c r="H244">
+      <c r="H248">
         <f>'Kompletne dane'!J249</f>
         <v>6.4</v>
       </c>
-      <c r="I244">
+      <c r="I248">
         <f>'Kompletne dane'!K249</f>
         <v>247</v>
       </c>
-      <c r="J244">
+      <c r="J248">
         <f>'Kompletne dane'!L249</f>
         <v>300</v>
       </c>
-      <c r="K244">
+      <c r="K248">
         <f>'Kompletne dane'!M249</f>
         <v>1375</v>
       </c>
-      <c r="L244">
+      <c r="L248">
         <f>'Kompletne dane'!N249</f>
         <v>341</v>
       </c>
-      <c r="M244">
+      <c r="M248">
         <f>'Kompletne dane'!O249</f>
         <v>55</v>
       </c>
-      <c r="N244">
+      <c r="N248">
         <f>'Kompletne dane'!P249</f>
         <v>432</v>
       </c>
-      <c r="O244">
+      <c r="O248">
         <f>'Kompletne dane'!Q249</f>
         <v>177</v>
       </c>
-      <c r="P244">
+      <c r="P248">
         <f>'Kompletne dane'!R249</f>
         <v>146</v>
       </c>
-      <c r="Q244">
+      <c r="Q248">
         <f>'Kompletne dane'!S249</f>
         <v>258</v>
       </c>
-      <c r="R244">
+      <c r="R248">
         <f>'Kompletne dane'!T249</f>
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A245">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A249">
         <f>'Kompletne dane'!C250</f>
         <v>2006</v>
       </c>
-      <c r="B245">
+      <c r="B249">
         <f>IF('Kompletne dane'!$D250="A",1,IF('Kompletne dane'!$D250="B",2,IF('Kompletne dane'!$D250="C",3,IF('Kompletne dane'!$D250="D",4,IF('Kompletne dane'!$D250="E",5,IF('Kompletne dane'!$D250="F",6,7))))))</f>
         <v>3</v>
       </c>
-      <c r="C245">
+      <c r="C249">
         <f>'Kompletne dane'!E250</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="D245">
+      <c r="D249">
         <f>'Kompletne dane'!F250</f>
         <v>4</v>
       </c>
-      <c r="E245">
+      <c r="E249">
         <f>'Kompletne dane'!G250</f>
         <v>260</v>
       </c>
-      <c r="F245">
+      <c r="F249">
         <f>'Kompletne dane'!H250</f>
         <v>5</v>
       </c>
-      <c r="G245">
+      <c r="G249">
         <f>'Kompletne dane'!I250</f>
         <v>5</v>
       </c>
-      <c r="H245">
+      <c r="H249">
         <f>'Kompletne dane'!J250</f>
         <v>6.1</v>
       </c>
-      <c r="I245">
+      <c r="I249">
         <f>'Kompletne dane'!K250</f>
         <v>250</v>
       </c>
-      <c r="J245">
+      <c r="J249">
         <f>'Kompletne dane'!L250</f>
         <v>380</v>
       </c>
-      <c r="K245">
+      <c r="K249">
         <f>'Kompletne dane'!M250</f>
         <v>1410</v>
       </c>
-      <c r="L245">
+      <c r="L249">
         <f>'Kompletne dane'!N250</f>
         <v>290</v>
       </c>
-      <c r="M245">
+      <c r="M249">
         <f>'Kompletne dane'!O250</f>
         <v>55</v>
       </c>
-      <c r="N245">
+      <c r="N249">
         <f>'Kompletne dane'!P250</f>
         <v>444</v>
       </c>
-      <c r="O245">
+      <c r="O249">
         <f>'Kompletne dane'!Q250</f>
         <v>177</v>
       </c>
-      <c r="P245">
+      <c r="P249">
         <f>'Kompletne dane'!R250</f>
         <v>147</v>
       </c>
-      <c r="Q245">
+      <c r="Q249">
         <f>'Kompletne dane'!S250</f>
         <v>264</v>
       </c>
-      <c r="R245">
+      <c r="R249">
         <f>'Kompletne dane'!T250</f>
         <v>6</v>
       </c>
@@ -36555,7 +36875,7 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f t="array" ref="A1:A20">TRANSPOSE('Kompletne dane'!A1:'Kompletne dane'!T1)</f>
-        <v>Numer</v>
+        <v>Id</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -36625,7 +36945,7 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <v>Pojemnośc baku [l]</v>
+        <v>Pojemność baku [l]</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed exception handling fixed user values duplication bug added no value in results fixed display of user values in results
</commit_message>
<xml_diff>
--- a/Samochody.xlsx
+++ b/Samochody.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NASA\PracaInz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B584CE-F182-4D5E-B810-056BC754A9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF218CB-2D0E-4C85-891B-9C13DA9342EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28725" yWindow="1305" windowWidth="27900" windowHeight="12270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kompletne dane" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="267">
   <si>
     <t>Nazwa</t>
   </si>
@@ -824,6 +824,12 @@
   <si>
     <t>Porsche 911 Carrera RS</t>
   </si>
+  <si>
+    <t>Mercedes 500SL</t>
+  </si>
+  <si>
+    <t>Aston Martin DB7</t>
+  </si>
 </sst>
 </file>
 
@@ -1140,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T254"/>
+  <dimension ref="A1:T256"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="K258" sqref="K258"/>
+    <sheetView topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="O257" sqref="O257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17168,6 +17174,130 @@
         <v>6</v>
       </c>
     </row>
+    <row r="255" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>254</v>
+      </c>
+      <c r="B255" t="s">
+        <v>265</v>
+      </c>
+      <c r="C255">
+        <v>2000</v>
+      </c>
+      <c r="D255" t="s">
+        <v>233</v>
+      </c>
+      <c r="E255">
+        <v>5</v>
+      </c>
+      <c r="F255">
+        <v>8</v>
+      </c>
+      <c r="G255">
+        <v>306</v>
+      </c>
+      <c r="H255">
+        <v>2</v>
+      </c>
+      <c r="I255">
+        <v>2</v>
+      </c>
+      <c r="J255">
+        <v>6.5</v>
+      </c>
+      <c r="K255">
+        <v>250</v>
+      </c>
+      <c r="L255">
+        <v>460</v>
+      </c>
+      <c r="M255">
+        <v>1815</v>
+      </c>
+      <c r="N255">
+        <v>265</v>
+      </c>
+      <c r="O255">
+        <v>80</v>
+      </c>
+      <c r="P255">
+        <v>450</v>
+      </c>
+      <c r="Q255">
+        <v>181</v>
+      </c>
+      <c r="R255">
+        <v>130</v>
+      </c>
+      <c r="S255">
+        <v>252</v>
+      </c>
+      <c r="T255">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>255</v>
+      </c>
+      <c r="B256" t="s">
+        <v>266</v>
+      </c>
+      <c r="C256">
+        <v>1998</v>
+      </c>
+      <c r="D256" t="s">
+        <v>233</v>
+      </c>
+      <c r="E256">
+        <v>3.2</v>
+      </c>
+      <c r="F256">
+        <v>6</v>
+      </c>
+      <c r="G256">
+        <v>360</v>
+      </c>
+      <c r="H256">
+        <v>4</v>
+      </c>
+      <c r="I256">
+        <v>2</v>
+      </c>
+      <c r="J256">
+        <v>6</v>
+      </c>
+      <c r="K256">
+        <v>265</v>
+      </c>
+      <c r="L256">
+        <v>499</v>
+      </c>
+      <c r="M256">
+        <v>1725</v>
+      </c>
+      <c r="N256">
+        <v>178</v>
+      </c>
+      <c r="O256">
+        <v>89</v>
+      </c>
+      <c r="P256">
+        <v>463</v>
+      </c>
+      <c r="Q256">
+        <v>182</v>
+      </c>
+      <c r="R256">
+        <v>127</v>
+      </c>
+      <c r="S256">
+        <v>259</v>
+      </c>
+      <c r="T256">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17175,10 +17305,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D8D5CA-9744-4893-9B14-DF471DE70DC3}">
-  <dimension ref="A1:A249"/>
+  <dimension ref="A1:A251"/>
   <sheetViews>
     <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="D233" sqref="D233"/>
+      <selection activeCell="F248" sqref="F248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18680,6 +18810,18 @@
         <v>Mazda 3 MPS</v>
       </c>
     </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="str">
+        <f>'Kompletne dane'!B255</f>
+        <v>Mercedes 500SL</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="str">
+        <f>'Kompletne dane'!B256</f>
+        <v>Aston Martin DB7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18687,10 +18829,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD037B1-ACD9-48BE-8904-7C9CBB062CA9}">
-  <dimension ref="A1:R253"/>
+  <dimension ref="A1:R255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="N231" sqref="N231"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="V251" sqref="V251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37415,6 +37557,154 @@
       <c r="R253">
         <f>'Kompletne dane'!T254</f>
         <v>6</v>
+      </c>
+    </row>
+    <row r="254" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <f>'Kompletne dane'!C255</f>
+        <v>2000</v>
+      </c>
+      <c r="B254">
+        <f>IF('Kompletne dane'!$D255="A",1,IF('Kompletne dane'!$D255="B",2,IF('Kompletne dane'!$D255="C",3,IF('Kompletne dane'!$D255="D",4,IF('Kompletne dane'!$D255="E",5,IF('Kompletne dane'!$D255="F",6,7))))))</f>
+        <v>7</v>
+      </c>
+      <c r="C254">
+        <f>'Kompletne dane'!E255</f>
+        <v>5</v>
+      </c>
+      <c r="D254">
+        <f>'Kompletne dane'!F255</f>
+        <v>8</v>
+      </c>
+      <c r="E254">
+        <f>'Kompletne dane'!G255</f>
+        <v>306</v>
+      </c>
+      <c r="F254">
+        <f>'Kompletne dane'!H255</f>
+        <v>2</v>
+      </c>
+      <c r="G254">
+        <f>'Kompletne dane'!I255</f>
+        <v>2</v>
+      </c>
+      <c r="H254">
+        <f>'Kompletne dane'!J255</f>
+        <v>6.5</v>
+      </c>
+      <c r="I254">
+        <f>'Kompletne dane'!K255</f>
+        <v>250</v>
+      </c>
+      <c r="J254">
+        <f>'Kompletne dane'!L255</f>
+        <v>460</v>
+      </c>
+      <c r="K254">
+        <f>'Kompletne dane'!M255</f>
+        <v>1815</v>
+      </c>
+      <c r="L254">
+        <f>'Kompletne dane'!N255</f>
+        <v>265</v>
+      </c>
+      <c r="M254">
+        <f>'Kompletne dane'!O255</f>
+        <v>80</v>
+      </c>
+      <c r="N254">
+        <f>'Kompletne dane'!P255</f>
+        <v>450</v>
+      </c>
+      <c r="O254">
+        <f>'Kompletne dane'!Q255</f>
+        <v>181</v>
+      </c>
+      <c r="P254">
+        <f>'Kompletne dane'!R255</f>
+        <v>130</v>
+      </c>
+      <c r="Q254">
+        <f>'Kompletne dane'!S255</f>
+        <v>252</v>
+      </c>
+      <c r="R254">
+        <f>'Kompletne dane'!T255</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <f>'Kompletne dane'!C256</f>
+        <v>1998</v>
+      </c>
+      <c r="B255">
+        <f>IF('Kompletne dane'!$D256="A",1,IF('Kompletne dane'!$D256="B",2,IF('Kompletne dane'!$D256="C",3,IF('Kompletne dane'!$D256="D",4,IF('Kompletne dane'!$D256="E",5,IF('Kompletne dane'!$D256="F",6,7))))))</f>
+        <v>7</v>
+      </c>
+      <c r="C255">
+        <f>'Kompletne dane'!E256</f>
+        <v>3.2</v>
+      </c>
+      <c r="D255">
+        <f>'Kompletne dane'!F256</f>
+        <v>6</v>
+      </c>
+      <c r="E255">
+        <f>'Kompletne dane'!G256</f>
+        <v>360</v>
+      </c>
+      <c r="F255">
+        <f>'Kompletne dane'!H256</f>
+        <v>4</v>
+      </c>
+      <c r="G255">
+        <f>'Kompletne dane'!I256</f>
+        <v>2</v>
+      </c>
+      <c r="H255">
+        <f>'Kompletne dane'!J256</f>
+        <v>6</v>
+      </c>
+      <c r="I255">
+        <f>'Kompletne dane'!K256</f>
+        <v>265</v>
+      </c>
+      <c r="J255">
+        <f>'Kompletne dane'!L256</f>
+        <v>499</v>
+      </c>
+      <c r="K255">
+        <f>'Kompletne dane'!M256</f>
+        <v>1725</v>
+      </c>
+      <c r="L255">
+        <f>'Kompletne dane'!N256</f>
+        <v>178</v>
+      </c>
+      <c r="M255">
+        <f>'Kompletne dane'!O256</f>
+        <v>89</v>
+      </c>
+      <c r="N255">
+        <f>'Kompletne dane'!P256</f>
+        <v>463</v>
+      </c>
+      <c r="O255">
+        <f>'Kompletne dane'!Q256</f>
+        <v>182</v>
+      </c>
+      <c r="P255">
+        <f>'Kompletne dane'!R256</f>
+        <v>127</v>
+      </c>
+      <c r="Q255">
+        <f>'Kompletne dane'!S256</f>
+        <v>259</v>
+      </c>
+      <c r="R255">
+        <f>'Kompletne dane'!T256</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added function comments in the code unified function names changed names of exe and py files increased the data set
</commit_message>
<xml_diff>
--- a/Samochody.xlsx
+++ b/Samochody.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NASA\PracaInz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF36F29-7CDF-43C9-8811-35DD37EF3ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43448341-3485-415A-AE4B-D67D3DA18B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="1635" windowWidth="22350" windowHeight="12270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2355" yWindow="1980" windowWidth="22350" windowHeight="12270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kompletne dane" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="270">
   <si>
     <t>Nazwa</t>
   </si>
@@ -836,6 +836,9 @@
   <si>
     <t>BMW 330i</t>
   </si>
+  <si>
+    <t>BMW 850CSi</t>
+  </si>
 </sst>
 </file>
 
@@ -1152,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T258"/>
+  <dimension ref="A1:T259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
-      <selection activeCell="E261" sqref="E261"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17428,6 +17431,68 @@
         <v>6</v>
       </c>
     </row>
+    <row r="259" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>258</v>
+      </c>
+      <c r="B259" t="s">
+        <v>269</v>
+      </c>
+      <c r="C259">
+        <v>1995</v>
+      </c>
+      <c r="D259" t="s">
+        <v>232</v>
+      </c>
+      <c r="E259">
+        <v>5.6</v>
+      </c>
+      <c r="F259">
+        <v>12</v>
+      </c>
+      <c r="G259">
+        <v>380</v>
+      </c>
+      <c r="H259">
+        <v>4</v>
+      </c>
+      <c r="I259">
+        <v>2</v>
+      </c>
+      <c r="J259">
+        <v>6</v>
+      </c>
+      <c r="K259">
+        <v>250</v>
+      </c>
+      <c r="L259">
+        <v>550</v>
+      </c>
+      <c r="M259">
+        <v>1900</v>
+      </c>
+      <c r="N259">
+        <v>320</v>
+      </c>
+      <c r="O259">
+        <v>90</v>
+      </c>
+      <c r="P259">
+        <v>478</v>
+      </c>
+      <c r="Q259">
+        <v>186</v>
+      </c>
+      <c r="R259">
+        <v>133</v>
+      </c>
+      <c r="S259">
+        <v>268</v>
+      </c>
+      <c r="T259">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17435,10 +17500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D8D5CA-9744-4893-9B14-DF471DE70DC3}">
-  <dimension ref="A1:A251"/>
+  <dimension ref="A1:A258"/>
   <sheetViews>
-    <sheetView topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="F248" sqref="F248"/>
+    <sheetView topLeftCell="A233" workbookViewId="0">
+      <selection sqref="A1:A258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18930,26 +18995,68 @@
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A248" t="str">
+        <f>'Kompletne dane'!B249</f>
+        <v>Opel Manta A</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="str">
+        <f>'Kompletne dane'!B250</f>
+        <v>Mercedes-Benz E400 4Matic</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="str">
+        <f>'Kompletne dane'!B251</f>
+        <v>BMW 335i</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="str">
+        <f>'Kompletne dane'!B252</f>
+        <v>Porsche 911 Carrera RS</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="str">
         <f>'Kompletne dane'!B253</f>
         <v>Seat Leon Cupra</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A249" t="str">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="str">
         <f>'Kompletne dane'!B254</f>
         <v>Mazda 3 MPS</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" t="str">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="str">
         <f>'Kompletne dane'!B255</f>
         <v>Mercedes 500SL</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" t="str">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="str">
         <f>'Kompletne dane'!B256</f>
         <v>Aston Martin DB7</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="str">
+        <f>'Kompletne dane'!B257</f>
+        <v>Porsche Panamera S</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="str">
+        <f>'Kompletne dane'!B258</f>
+        <v>BMW 330i</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="str">
+        <f>'Kompletne dane'!B259</f>
+        <v>BMW 850CSi</v>
       </c>
     </row>
   </sheetData>
@@ -18959,10 +19066,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD037B1-ACD9-48BE-8904-7C9CBB062CA9}">
-  <dimension ref="A1:R255"/>
+  <dimension ref="A1:R258"/>
   <sheetViews>
-    <sheetView topLeftCell="A240" workbookViewId="0">
-      <selection activeCell="V251" sqref="V251"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="Q254" sqref="Q254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37835,6 +37942,228 @@
       <c r="R255">
         <f>'Kompletne dane'!T256</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <f>'Kompletne dane'!C257</f>
+        <v>2012</v>
+      </c>
+      <c r="B256">
+        <f>IF('Kompletne dane'!$D257="A",1,IF('Kompletne dane'!$D257="B",2,IF('Kompletne dane'!$D257="C",3,IF('Kompletne dane'!$D257="D",4,IF('Kompletne dane'!$D257="E",5,IF('Kompletne dane'!$D257="F",6,7))))))</f>
+        <v>5</v>
+      </c>
+      <c r="C256">
+        <f>'Kompletne dane'!E257</f>
+        <v>4.8</v>
+      </c>
+      <c r="D256">
+        <f>'Kompletne dane'!F257</f>
+        <v>8</v>
+      </c>
+      <c r="E256">
+        <f>'Kompletne dane'!G257</f>
+        <v>400</v>
+      </c>
+      <c r="F256">
+        <f>'Kompletne dane'!H257</f>
+        <v>4</v>
+      </c>
+      <c r="G256">
+        <f>'Kompletne dane'!I257</f>
+        <v>5</v>
+      </c>
+      <c r="H256">
+        <f>'Kompletne dane'!J257</f>
+        <v>5.6</v>
+      </c>
+      <c r="I256">
+        <f>'Kompletne dane'!K257</f>
+        <v>285</v>
+      </c>
+      <c r="J256">
+        <f>'Kompletne dane'!L257</f>
+        <v>500</v>
+      </c>
+      <c r="K256">
+        <f>'Kompletne dane'!M257</f>
+        <v>1770</v>
+      </c>
+      <c r="L256">
+        <f>'Kompletne dane'!N257</f>
+        <v>445</v>
+      </c>
+      <c r="M256">
+        <f>'Kompletne dane'!O257</f>
+        <v>80</v>
+      </c>
+      <c r="N256">
+        <f>'Kompletne dane'!P257</f>
+        <v>497</v>
+      </c>
+      <c r="O256">
+        <f>'Kompletne dane'!Q257</f>
+        <v>191</v>
+      </c>
+      <c r="P256">
+        <f>'Kompletne dane'!R257</f>
+        <v>142</v>
+      </c>
+      <c r="Q256">
+        <f>'Kompletne dane'!S257</f>
+        <v>292</v>
+      </c>
+      <c r="R256">
+        <f>'Kompletne dane'!T257</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <f>'Kompletne dane'!C258</f>
+        <v>2011</v>
+      </c>
+      <c r="B257">
+        <f>IF('Kompletne dane'!$D258="A",1,IF('Kompletne dane'!$D258="B",2,IF('Kompletne dane'!$D258="C",3,IF('Kompletne dane'!$D258="D",4,IF('Kompletne dane'!$D258="E",5,IF('Kompletne dane'!$D258="F",6,7))))))</f>
+        <v>4</v>
+      </c>
+      <c r="C257">
+        <f>'Kompletne dane'!E258</f>
+        <v>3</v>
+      </c>
+      <c r="D257">
+        <f>'Kompletne dane'!F258</f>
+        <v>6</v>
+      </c>
+      <c r="E257">
+        <f>'Kompletne dane'!G258</f>
+        <v>272</v>
+      </c>
+      <c r="F257">
+        <f>'Kompletne dane'!H258</f>
+        <v>5</v>
+      </c>
+      <c r="G257">
+        <f>'Kompletne dane'!I258</f>
+        <v>4</v>
+      </c>
+      <c r="H257">
+        <f>'Kompletne dane'!J258</f>
+        <v>6.1</v>
+      </c>
+      <c r="I257">
+        <f>'Kompletne dane'!K258</f>
+        <v>250</v>
+      </c>
+      <c r="J257">
+        <f>'Kompletne dane'!L258</f>
+        <v>320</v>
+      </c>
+      <c r="K257">
+        <f>'Kompletne dane'!M258</f>
+        <v>1475</v>
+      </c>
+      <c r="L257">
+        <f>'Kompletne dane'!N258</f>
+        <v>460</v>
+      </c>
+      <c r="M257">
+        <f>'Kompletne dane'!O258</f>
+        <v>63</v>
+      </c>
+      <c r="N257">
+        <f>'Kompletne dane'!P258</f>
+        <v>453</v>
+      </c>
+      <c r="O257">
+        <f>'Kompletne dane'!Q258</f>
+        <v>182</v>
+      </c>
+      <c r="P257">
+        <f>'Kompletne dane'!R258</f>
+        <v>142</v>
+      </c>
+      <c r="Q257">
+        <f>'Kompletne dane'!S258</f>
+        <v>276</v>
+      </c>
+      <c r="R257">
+        <f>'Kompletne dane'!T258</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <f>'Kompletne dane'!C259</f>
+        <v>1995</v>
+      </c>
+      <c r="B258">
+        <f>IF('Kompletne dane'!$D259="A",1,IF('Kompletne dane'!$D259="B",2,IF('Kompletne dane'!$D259="C",3,IF('Kompletne dane'!$D259="D",4,IF('Kompletne dane'!$D259="E",5,IF('Kompletne dane'!$D259="F",6,7))))))</f>
+        <v>5</v>
+      </c>
+      <c r="C258">
+        <f>'Kompletne dane'!E259</f>
+        <v>5.6</v>
+      </c>
+      <c r="D258">
+        <f>'Kompletne dane'!F259</f>
+        <v>12</v>
+      </c>
+      <c r="E258">
+        <f>'Kompletne dane'!G259</f>
+        <v>380</v>
+      </c>
+      <c r="F258">
+        <f>'Kompletne dane'!H259</f>
+        <v>4</v>
+      </c>
+      <c r="G258">
+        <f>'Kompletne dane'!I259</f>
+        <v>2</v>
+      </c>
+      <c r="H258">
+        <f>'Kompletne dane'!J259</f>
+        <v>6</v>
+      </c>
+      <c r="I258">
+        <f>'Kompletne dane'!K259</f>
+        <v>250</v>
+      </c>
+      <c r="J258">
+        <f>'Kompletne dane'!L259</f>
+        <v>550</v>
+      </c>
+      <c r="K258">
+        <f>'Kompletne dane'!M259</f>
+        <v>1900</v>
+      </c>
+      <c r="L258">
+        <f>'Kompletne dane'!N259</f>
+        <v>320</v>
+      </c>
+      <c r="M258">
+        <f>'Kompletne dane'!O259</f>
+        <v>90</v>
+      </c>
+      <c r="N258">
+        <f>'Kompletne dane'!P259</f>
+        <v>478</v>
+      </c>
+      <c r="O258">
+        <f>'Kompletne dane'!Q259</f>
+        <v>186</v>
+      </c>
+      <c r="P258">
+        <f>'Kompletne dane'!R259</f>
+        <v>133</v>
+      </c>
+      <c r="Q258">
+        <f>'Kompletne dane'!S259</f>
+        <v>268</v>
+      </c>
+      <c r="R258">
+        <f>'Kompletne dane'!T259</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed normalizing fixed mix,max
</commit_message>
<xml_diff>
--- a/Samochody.xlsx
+++ b/Samochody.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NASA\PracaInz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43448341-3485-415A-AE4B-D67D3DA18B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C527BD70-9123-43DC-9A26-9CBCD612FAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="1980" windowWidth="22350" windowHeight="12270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="3105" windowWidth="25140" windowHeight="12285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kompletne dane" sheetId="1" r:id="rId1"/>
@@ -1157,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T259"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="H144" sqref="H144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10208,7 +10208,7 @@
         <v>1.6</v>
       </c>
       <c r="F144">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G144">
         <v>116</v>
@@ -19068,7 +19068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD037B1-ACD9-48BE-8904-7C9CBB062CA9}">
   <dimension ref="A1:R258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+    <sheetView topLeftCell="A243" workbookViewId="0">
       <selection activeCell="Q254" sqref="Q254"/>
     </sheetView>
   </sheetViews>
@@ -29597,7 +29597,7 @@
       </c>
       <c r="D143">
         <f>'Kompletne dane'!F144</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E143">
         <f>'Kompletne dane'!G144</f>

</xml_diff>